<commit_message>
prep nexus files for other clades
</commit_message>
<xml_diff>
--- a/main/beast/all/chromosome/clade/clades_data_summary.xlsx
+++ b/main/beast/all/chromosome/clade/clades_data_summary.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,21 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ktmea\Projects\plague-phylogeography-projects\main\beast\all\chromosome\clade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{6F94D4AD-F842-45D7-9EB7-6D9F0ABAE5E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{950A7271-540C-4A18-82F2-F797DD32D8F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="noHyperPrior" sheetId="3" r:id="rId1"/>
     <sheet name="summary" sheetId="6" r:id="rId2"/>
-    <sheet name="epop" sheetId="4" r:id="rId3"/>
+    <sheet name="kat_summary" sheetId="7" r:id="rId3"/>
+    <sheet name="epop" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="44">
   <si>
     <t>Clade</t>
   </si>
@@ -152,13 +164,16 @@
   <si>
     <t>Log Likelihood (GSS)</t>
   </si>
+  <si>
+    <t>Log Bayes Factor</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="21" x14ac:knownFonts="1">
     <font>
@@ -530,7 +545,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -700,6 +715,68 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -745,7 +822,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -872,99 +949,156 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1329,7 +1463,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1948,11 +2082,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1990,13 +2124,13 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="80" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -2005,31 +2139,31 @@
       <c r="E2" s="2">
         <v>-5899661.4930999996</v>
       </c>
-      <c r="F2" s="72">
+      <c r="F2" s="65">
         <f>E2-E4</f>
         <v>29.621400000527501</v>
       </c>
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="44"/>
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
+      <c r="A3" s="70"/>
+      <c r="B3" s="80"/>
+      <c r="C3" s="80"/>
       <c r="D3" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E3" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="62" t="s">
+      <c r="F3" s="55" t="s">
         <v>40</v>
       </c>
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="44"/>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42" t="s">
+      <c r="A4" s="70"/>
+      <c r="B4" s="80"/>
+      <c r="C4" s="80" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -2038,33 +2172,33 @@
       <c r="E4" s="9">
         <v>-5899691.1145000001</v>
       </c>
-      <c r="F4" s="61">
+      <c r="F4" s="54">
         <f>E4-E2</f>
         <v>-29.621400000527501</v>
       </c>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="44"/>
-      <c r="B5" s="42"/>
-      <c r="C5" s="42"/>
+      <c r="A5" s="70"/>
+      <c r="B5" s="80"/>
+      <c r="C5" s="80"/>
       <c r="D5" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E5" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="F5" s="62" t="s">
+      <c r="F5" s="55" t="s">
         <v>40</v>
       </c>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="44"/>
-      <c r="B6" s="46" t="s">
+      <c r="A6" s="70"/>
+      <c r="B6" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="46" t="s">
+      <c r="C6" s="75" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="11" t="s">
@@ -2073,31 +2207,31 @@
       <c r="E6" s="11">
         <v>-5899565.7433000002</v>
       </c>
-      <c r="F6" s="63">
+      <c r="F6" s="56">
         <f>E6-E8</f>
         <v>35.669999999925494</v>
       </c>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="44"/>
-      <c r="B7" s="46"/>
-      <c r="C7" s="46"/>
+      <c r="A7" s="70"/>
+      <c r="B7" s="75"/>
+      <c r="C7" s="75"/>
       <c r="D7" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E7" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="62" t="s">
+      <c r="F7" s="55" t="s">
         <v>40</v>
       </c>
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="44"/>
-      <c r="B8" s="46"/>
-      <c r="C8" s="42" t="s">
+      <c r="A8" s="70"/>
+      <c r="B8" s="75"/>
+      <c r="C8" s="80" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -2106,35 +2240,35 @@
       <c r="E8" s="2">
         <v>-5899601.4133000001</v>
       </c>
-      <c r="F8" s="61">
+      <c r="F8" s="54">
         <f>E8-E6</f>
         <v>-35.669999999925494</v>
       </c>
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="45"/>
-      <c r="B9" s="47"/>
-      <c r="C9" s="43"/>
+      <c r="A9" s="71"/>
+      <c r="B9" s="76"/>
+      <c r="C9" s="81"/>
       <c r="D9" s="3" t="s">
         <v>33</v>
       </c>
       <c r="E9" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="62" t="s">
+      <c r="F9" s="55" t="s">
         <v>40</v>
       </c>
       <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="57" t="s">
+      <c r="A10" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="58" t="s">
+      <c r="B10" s="79" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="58" t="s">
+      <c r="C10" s="79" t="s">
         <v>3</v>
       </c>
       <c r="D10" s="4" t="s">
@@ -2143,31 +2277,31 @@
       <c r="E10" s="4">
         <v>-5891402.6964999996</v>
       </c>
-      <c r="F10" s="64">
+      <c r="F10" s="57">
         <f>E10-E12</f>
         <v>-3.5282999994233251</v>
       </c>
-      <c r="G10" s="59"/>
+      <c r="G10" s="52"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="44"/>
-      <c r="B11" s="42"/>
-      <c r="C11" s="42"/>
+      <c r="A11" s="70"/>
+      <c r="B11" s="80"/>
+      <c r="C11" s="80"/>
       <c r="D11" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E11" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="62" t="s">
+      <c r="F11" s="55" t="s">
         <v>40</v>
       </c>
       <c r="G11" s="6"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="44"/>
-      <c r="B12" s="42"/>
-      <c r="C12" s="42" t="s">
+      <c r="A12" s="70"/>
+      <c r="B12" s="80"/>
+      <c r="C12" s="80" t="s">
         <v>4</v>
       </c>
       <c r="D12" s="2" t="s">
@@ -2176,33 +2310,33 @@
       <c r="E12" s="2">
         <v>-5891399.1682000002</v>
       </c>
-      <c r="F12" s="73">
+      <c r="F12" s="66">
         <f>E12-E10</f>
         <v>3.5282999994233251</v>
       </c>
       <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="44"/>
-      <c r="B13" s="42"/>
-      <c r="C13" s="42"/>
+      <c r="A13" s="70"/>
+      <c r="B13" s="80"/>
+      <c r="C13" s="80"/>
       <c r="D13" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E13" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="62" t="s">
+      <c r="F13" s="55" t="s">
         <v>40</v>
       </c>
       <c r="G13" s="6"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="44"/>
-      <c r="B14" s="54" t="s">
+      <c r="A14" s="70"/>
+      <c r="B14" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="42" t="s">
+      <c r="C14" s="80" t="s">
         <v>3</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -2211,31 +2345,31 @@
       <c r="E14" s="2">
         <v>-5891354.5140000004</v>
       </c>
-      <c r="F14" s="61">
+      <c r="F14" s="54">
         <f>E14-E16</f>
         <v>-10.331400000490248</v>
       </c>
       <c r="G14" s="6"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="44"/>
-      <c r="B15" s="54"/>
-      <c r="C15" s="42"/>
+      <c r="A15" s="70"/>
+      <c r="B15" s="73"/>
+      <c r="C15" s="80"/>
       <c r="D15" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E15" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="F15" s="62" t="s">
+      <c r="F15" s="55" t="s">
         <v>40</v>
       </c>
       <c r="G15" s="6"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="44"/>
-      <c r="B16" s="54"/>
-      <c r="C16" s="54" t="s">
+      <c r="A16" s="70"/>
+      <c r="B16" s="73"/>
+      <c r="C16" s="73" t="s">
         <v>4</v>
       </c>
       <c r="D16" s="8" t="s">
@@ -2244,99 +2378,99 @@
       <c r="E16" s="8">
         <v>-5891344.1825999999</v>
       </c>
-      <c r="F16" s="65">
+      <c r="F16" s="58">
         <f>E16-E14</f>
         <v>10.331400000490248</v>
       </c>
       <c r="G16" s="6"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="45"/>
-      <c r="B17" s="55"/>
-      <c r="C17" s="55"/>
+      <c r="A17" s="71"/>
+      <c r="B17" s="74"/>
+      <c r="C17" s="74"/>
       <c r="D17" s="3" t="s">
         <v>33</v>
       </c>
       <c r="E17" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="F17" s="66" t="s">
+      <c r="F17" s="59" t="s">
         <v>40</v>
       </c>
       <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="44" t="s">
+      <c r="A18" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="48" t="s">
+      <c r="B18" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="48" t="s">
+      <c r="C18" s="72" t="s">
         <v>3</v>
       </c>
       <c r="D18" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E18" s="49">
+      <c r="E18" s="46">
         <v>-5882586.8744000001</v>
       </c>
-      <c r="F18" s="74">
+      <c r="F18" s="67">
         <f t="shared" ref="F18" si="0">E18-E20</f>
         <v>9.2806000001728535</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="44"/>
-      <c r="B19" s="48"/>
-      <c r="C19" s="48"/>
+      <c r="A19" s="70"/>
+      <c r="B19" s="72"/>
+      <c r="C19" s="72"/>
       <c r="D19" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E19" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="F19" s="62" t="s">
+      <c r="E19" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19" s="55" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="44"/>
-      <c r="B20" s="48"/>
-      <c r="C20" s="48" t="s">
+      <c r="A20" s="70"/>
+      <c r="B20" s="72"/>
+      <c r="C20" s="72" t="s">
         <v>4</v>
       </c>
       <c r="D20" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E20" s="49">
+      <c r="E20" s="46">
         <v>-5882596.1550000003</v>
       </c>
-      <c r="F20" s="67">
+      <c r="F20" s="60">
         <f t="shared" ref="F20" si="1">E20-E18</f>
         <v>-9.2806000001728535</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="44"/>
-      <c r="B21" s="48"/>
-      <c r="C21" s="48"/>
+      <c r="A21" s="70"/>
+      <c r="B21" s="72"/>
+      <c r="C21" s="72"/>
       <c r="D21" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E21" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="F21" s="62" t="s">
+      <c r="E21" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F21" s="55" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="44"/>
-      <c r="B22" s="46" t="s">
+      <c r="A22" s="70"/>
+      <c r="B22" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="46" t="s">
+      <c r="C22" s="75" t="s">
         <v>3</v>
       </c>
       <c r="D22" s="11" t="s">
@@ -2345,128 +2479,128 @@
       <c r="E22" s="5">
         <v>-5882581.8636999996</v>
       </c>
-      <c r="F22" s="68">
+      <c r="F22" s="61">
         <f t="shared" ref="F22" si="2">E22-E24</f>
         <v>12.690900000743568</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="44"/>
-      <c r="B23" s="46"/>
-      <c r="C23" s="46"/>
+      <c r="A23" s="70"/>
+      <c r="B23" s="75"/>
+      <c r="C23" s="75"/>
       <c r="D23" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E23" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="F23" s="62" t="s">
+      <c r="E23" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F23" s="55" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="44"/>
-      <c r="B24" s="46"/>
-      <c r="C24" s="48" t="s">
+      <c r="A24" s="70"/>
+      <c r="B24" s="75"/>
+      <c r="C24" s="72" t="s">
         <v>4</v>
       </c>
       <c r="D24" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E24" s="49">
+      <c r="E24" s="46">
         <v>-5882594.5546000004</v>
       </c>
-      <c r="F24" s="67">
+      <c r="F24" s="60">
         <f t="shared" ref="F24" si="3">E24-E22</f>
         <v>-12.690900000743568</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="45"/>
-      <c r="B25" s="47"/>
-      <c r="C25" s="51"/>
+      <c r="A25" s="71"/>
+      <c r="B25" s="76"/>
+      <c r="C25" s="77"/>
       <c r="D25" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E25" s="52" t="s">
-        <v>40</v>
-      </c>
-      <c r="F25" s="69" t="s">
+      <c r="E25" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="F25" s="62" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="44" t="s">
+      <c r="A26" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="B26" s="48" t="s">
+      <c r="B26" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="48" t="s">
+      <c r="C26" s="72" t="s">
         <v>3</v>
       </c>
       <c r="D26" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E26" s="49">
+      <c r="E26" s="46">
         <v>-5888129.8859000001</v>
       </c>
-      <c r="F26" s="74">
+      <c r="F26" s="67">
         <f t="shared" ref="F26" si="4">E26-E28</f>
         <v>10.098799999803305</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="44"/>
-      <c r="B27" s="48"/>
-      <c r="C27" s="48"/>
+      <c r="A27" s="70"/>
+      <c r="B27" s="72"/>
+      <c r="C27" s="72"/>
       <c r="D27" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E27" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="F27" s="62" t="s">
+      <c r="E27" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F27" s="55" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="44"/>
-      <c r="B28" s="48"/>
-      <c r="C28" s="48" t="s">
+      <c r="A28" s="70"/>
+      <c r="B28" s="72"/>
+      <c r="C28" s="72" t="s">
         <v>4</v>
       </c>
       <c r="D28" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E28" s="49">
+      <c r="E28" s="46">
         <v>-5888139.9846999999</v>
       </c>
-      <c r="F28" s="67">
+      <c r="F28" s="60">
         <f t="shared" ref="F28" si="5">E28-E26</f>
         <v>-10.098799999803305</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="44"/>
-      <c r="B29" s="48"/>
-      <c r="C29" s="48"/>
+      <c r="A29" s="70"/>
+      <c r="B29" s="72"/>
+      <c r="C29" s="72"/>
       <c r="D29" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E29" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="F29" s="62" t="s">
+      <c r="E29" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F29" s="55" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="44"/>
-      <c r="B30" s="46" t="s">
+      <c r="A30" s="70"/>
+      <c r="B30" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="C30" s="46" t="s">
+      <c r="C30" s="75" t="s">
         <v>3</v>
       </c>
       <c r="D30" s="11" t="s">
@@ -2475,128 +2609,128 @@
       <c r="E30" s="5">
         <v>-5888038.0526000001</v>
       </c>
-      <c r="F30" s="68">
+      <c r="F30" s="61">
         <f t="shared" ref="F30" si="6">E30-E32</f>
         <v>44.081500000320375</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="44"/>
-      <c r="B31" s="46"/>
-      <c r="C31" s="46"/>
+      <c r="A31" s="70"/>
+      <c r="B31" s="75"/>
+      <c r="C31" s="75"/>
       <c r="D31" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E31" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="F31" s="62" t="s">
+      <c r="E31" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F31" s="55" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="44"/>
-      <c r="B32" s="46"/>
-      <c r="C32" s="48" t="s">
+      <c r="A32" s="70"/>
+      <c r="B32" s="75"/>
+      <c r="C32" s="72" t="s">
         <v>4</v>
       </c>
       <c r="D32" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E32" s="49">
+      <c r="E32" s="46">
         <v>-5888082.1341000004</v>
       </c>
-      <c r="F32" s="67">
+      <c r="F32" s="60">
         <f t="shared" ref="F32" si="7">E32-E30</f>
         <v>-44.081500000320375</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="45"/>
-      <c r="B33" s="47"/>
-      <c r="C33" s="51"/>
+      <c r="A33" s="71"/>
+      <c r="B33" s="76"/>
+      <c r="C33" s="77"/>
       <c r="D33" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E33" s="52" t="s">
-        <v>40</v>
-      </c>
-      <c r="F33" s="69" t="s">
+      <c r="E33" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="F33" s="62" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="44" t="s">
+      <c r="A34" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="B34" s="48" t="s">
+      <c r="B34" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="C34" s="48" t="s">
+      <c r="C34" s="72" t="s">
         <v>3</v>
       </c>
       <c r="D34" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E34" s="49">
+      <c r="E34" s="46">
         <v>-5920732.7741</v>
       </c>
-      <c r="F34" s="74">
+      <c r="F34" s="67">
         <f t="shared" ref="F34:F90" si="8">E34-E36</f>
         <v>104.57550000026822</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="44"/>
-      <c r="B35" s="48"/>
-      <c r="C35" s="48"/>
+      <c r="A35" s="70"/>
+      <c r="B35" s="72"/>
+      <c r="C35" s="72"/>
       <c r="D35" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E35" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="F35" s="71" t="s">
+      <c r="E35" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F35" s="64" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="44"/>
-      <c r="B36" s="48"/>
-      <c r="C36" s="48" t="s">
+      <c r="A36" s="70"/>
+      <c r="B36" s="72"/>
+      <c r="C36" s="72" t="s">
         <v>4</v>
       </c>
       <c r="D36" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E36" s="49">
+      <c r="E36" s="46">
         <v>-5920837.3496000003</v>
       </c>
-      <c r="F36" s="67">
+      <c r="F36" s="60">
         <f t="shared" ref="F36:F92" si="9">E36-E34</f>
         <v>-104.57550000026822</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="44"/>
-      <c r="B37" s="48"/>
-      <c r="C37" s="48"/>
+      <c r="A37" s="70"/>
+      <c r="B37" s="72"/>
+      <c r="C37" s="72"/>
       <c r="D37" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E37" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="F37" s="71" t="s">
+      <c r="E37" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F37" s="64" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="44"/>
-      <c r="B38" s="46" t="s">
+      <c r="A38" s="70"/>
+      <c r="B38" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="C38" s="46" t="s">
+      <c r="C38" s="75" t="s">
         <v>3</v>
       </c>
       <c r="D38" s="11" t="s">
@@ -2605,252 +2739,252 @@
       <c r="E38" s="5">
         <v>-5919658.1359000001</v>
       </c>
-      <c r="F38" s="68">
+      <c r="F38" s="61">
         <f t="shared" ref="F38:F94" si="10">E38-E40</f>
         <v>3.9017000002786517</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="44"/>
-      <c r="B39" s="46"/>
-      <c r="C39" s="46"/>
+      <c r="A39" s="70"/>
+      <c r="B39" s="75"/>
+      <c r="C39" s="75"/>
       <c r="D39" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E39" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="F39" s="71" t="s">
+      <c r="E39" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F39" s="64" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="44"/>
-      <c r="B40" s="46"/>
-      <c r="C40" s="48" t="s">
+      <c r="A40" s="70"/>
+      <c r="B40" s="75"/>
+      <c r="C40" s="72" t="s">
         <v>4</v>
       </c>
       <c r="D40" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E40" s="49">
+      <c r="E40" s="46">
         <v>-5919662.0376000004</v>
       </c>
-      <c r="F40" s="67">
+      <c r="F40" s="60">
         <f t="shared" ref="F40:F96" si="11">E40-E38</f>
         <v>-3.9017000002786517</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="45"/>
-      <c r="B41" s="47"/>
-      <c r="C41" s="51"/>
+      <c r="A41" s="71"/>
+      <c r="B41" s="76"/>
+      <c r="C41" s="77"/>
       <c r="D41" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E41" s="52" t="s">
-        <v>40</v>
-      </c>
-      <c r="F41" s="69" t="s">
+      <c r="E41" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="F41" s="62" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="44" t="s">
+      <c r="A42" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="B42" s="48" t="s">
+      <c r="B42" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="C42" s="48" t="s">
+      <c r="C42" s="72" t="s">
         <v>3</v>
       </c>
       <c r="D42" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E42" s="49">
+      <c r="E42" s="46">
         <v>-5892894.9243999999</v>
       </c>
-      <c r="F42" s="67">
+      <c r="F42" s="60">
         <f t="shared" si="8"/>
         <v>-18.697699999436736</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="44"/>
-      <c r="B43" s="48"/>
-      <c r="C43" s="48"/>
+      <c r="A43" s="70"/>
+      <c r="B43" s="72"/>
+      <c r="C43" s="72"/>
       <c r="D43" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E43" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="F43" s="67"/>
+      <c r="E43" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F43" s="60"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="44"/>
-      <c r="B44" s="48"/>
-      <c r="C44" s="48" t="s">
+      <c r="A44" s="70"/>
+      <c r="B44" s="72"/>
+      <c r="C44" s="72" t="s">
         <v>4</v>
       </c>
       <c r="D44" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="49">
+      <c r="E44" s="46">
         <v>-5892876.2267000005</v>
       </c>
-      <c r="F44" s="75">
+      <c r="F44" s="68">
         <f t="shared" si="9"/>
         <v>18.697699999436736</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="44"/>
-      <c r="B45" s="48"/>
-      <c r="C45" s="48"/>
+      <c r="A45" s="70"/>
+      <c r="B45" s="72"/>
+      <c r="C45" s="72"/>
       <c r="D45" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E45" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="F45" s="67"/>
+      <c r="E45" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F45" s="60"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="44"/>
-      <c r="B46" s="54" t="s">
+      <c r="A46" s="70"/>
+      <c r="B46" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="C46" s="48" t="s">
+      <c r="C46" s="72" t="s">
         <v>3</v>
       </c>
       <c r="D46" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E46" s="49">
+      <c r="E46" s="46">
         <v>-5892804.6540000001</v>
       </c>
-      <c r="F46" s="67">
+      <c r="F46" s="60">
         <f t="shared" si="10"/>
         <v>-13.384899999946356</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="44"/>
-      <c r="B47" s="54"/>
-      <c r="C47" s="48"/>
+      <c r="A47" s="70"/>
+      <c r="B47" s="73"/>
+      <c r="C47" s="72"/>
       <c r="D47" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E47" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="F47" s="67"/>
+      <c r="E47" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F47" s="60"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="44"/>
-      <c r="B48" s="54"/>
-      <c r="C48" s="54" t="s">
+      <c r="A48" s="70"/>
+      <c r="B48" s="73"/>
+      <c r="C48" s="73" t="s">
         <v>4</v>
       </c>
       <c r="D48" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E48" s="56">
+      <c r="E48" s="50">
         <v>-5892791.2691000002</v>
       </c>
-      <c r="F48" s="60">
+      <c r="F48" s="53">
         <f t="shared" si="11"/>
         <v>13.384899999946356</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="45"/>
-      <c r="B49" s="55"/>
-      <c r="C49" s="55"/>
+      <c r="A49" s="71"/>
+      <c r="B49" s="74"/>
+      <c r="C49" s="74"/>
       <c r="D49" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E49" s="52" t="s">
-        <v>40</v>
-      </c>
-      <c r="F49" s="69" t="s">
+      <c r="E49" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="F49" s="62" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="44" t="s">
+      <c r="A50" s="70" t="s">
         <v>10</v>
       </c>
-      <c r="B50" s="48" t="s">
+      <c r="B50" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="C50" s="48" t="s">
+      <c r="C50" s="72" t="s">
         <v>3</v>
       </c>
       <c r="D50" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E50" s="49">
+      <c r="E50" s="46">
         <v>-5886034.1161000002</v>
       </c>
-      <c r="F50" s="67">
+      <c r="F50" s="60">
         <f t="shared" si="8"/>
         <v>-2.6929999999701977</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="44"/>
-      <c r="B51" s="48"/>
-      <c r="C51" s="48"/>
+      <c r="A51" s="70"/>
+      <c r="B51" s="72"/>
+      <c r="C51" s="72"/>
       <c r="D51" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E51" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="F51" s="71" t="s">
+      <c r="E51" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F51" s="64" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="44"/>
-      <c r="B52" s="48"/>
-      <c r="C52" s="48" t="s">
+      <c r="A52" s="70"/>
+      <c r="B52" s="72"/>
+      <c r="C52" s="72" t="s">
         <v>4</v>
       </c>
       <c r="D52" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E52" s="49">
+      <c r="E52" s="46">
         <v>-5886031.4231000002</v>
       </c>
-      <c r="F52" s="76">
+      <c r="F52" s="69">
         <f t="shared" si="9"/>
         <v>2.6929999999701977</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="44"/>
-      <c r="B53" s="48"/>
-      <c r="C53" s="48"/>
+      <c r="A53" s="70"/>
+      <c r="B53" s="72"/>
+      <c r="C53" s="72"/>
       <c r="D53" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E53" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="F53" s="71" t="s">
+      <c r="E53" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F53" s="64" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="44"/>
-      <c r="B54" s="46" t="s">
+      <c r="A54" s="70"/>
+      <c r="B54" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="C54" s="46" t="s">
+      <c r="C54" s="75" t="s">
         <v>3</v>
       </c>
       <c r="D54" s="11" t="s">
@@ -2859,258 +2993,258 @@
       <c r="E54" s="5">
         <v>-5886021.9687000001</v>
       </c>
-      <c r="F54" s="68">
+      <c r="F54" s="61">
         <f t="shared" si="10"/>
         <v>3.6091000000014901</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="44"/>
-      <c r="B55" s="46"/>
-      <c r="C55" s="46"/>
+      <c r="A55" s="70"/>
+      <c r="B55" s="75"/>
+      <c r="C55" s="75"/>
       <c r="D55" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E55" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="F55" s="71" t="s">
+      <c r="E55" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F55" s="64" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="44"/>
-      <c r="B56" s="46"/>
-      <c r="C56" s="48" t="s">
+      <c r="A56" s="70"/>
+      <c r="B56" s="75"/>
+      <c r="C56" s="72" t="s">
         <v>4</v>
       </c>
       <c r="D56" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E56" s="49">
+      <c r="E56" s="46">
         <v>-5886025.5778000001</v>
       </c>
-      <c r="F56" s="67">
+      <c r="F56" s="60">
         <f t="shared" si="11"/>
         <v>-3.6091000000014901</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="45"/>
-      <c r="B57" s="47"/>
-      <c r="C57" s="51"/>
+      <c r="A57" s="71"/>
+      <c r="B57" s="76"/>
+      <c r="C57" s="77"/>
       <c r="D57" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E57" s="52" t="s">
-        <v>40</v>
-      </c>
-      <c r="F57" s="69" t="s">
+      <c r="E57" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="F57" s="62" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="44" t="s">
+      <c r="A58" s="70" t="s">
         <v>11</v>
       </c>
-      <c r="B58" s="48" t="s">
+      <c r="B58" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="C58" s="48" t="s">
+      <c r="C58" s="72" t="s">
         <v>3</v>
       </c>
       <c r="D58" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E58" s="49">
+      <c r="E58" s="46">
         <v>-5887506.0362999998</v>
       </c>
-      <c r="F58" s="67">
+      <c r="F58" s="60">
         <f t="shared" si="8"/>
         <v>-9.4918999997898936</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="44"/>
-      <c r="B59" s="48"/>
-      <c r="C59" s="48"/>
+      <c r="A59" s="70"/>
+      <c r="B59" s="72"/>
+      <c r="C59" s="72"/>
       <c r="D59" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E59" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="F59" s="71" t="s">
+      <c r="E59" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F59" s="64" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="44"/>
-      <c r="B60" s="48"/>
-      <c r="C60" s="48" t="s">
+      <c r="A60" s="70"/>
+      <c r="B60" s="72"/>
+      <c r="C60" s="72" t="s">
         <v>4</v>
       </c>
       <c r="D60" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E60" s="49">
+      <c r="E60" s="46">
         <v>-5887496.5444</v>
       </c>
-      <c r="F60" s="75">
+      <c r="F60" s="68">
         <f t="shared" si="9"/>
         <v>9.4918999997898936</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="44"/>
-      <c r="B61" s="48"/>
-      <c r="C61" s="48"/>
+      <c r="A61" s="70"/>
+      <c r="B61" s="72"/>
+      <c r="C61" s="72"/>
       <c r="D61" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E61" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="F61" s="71" t="s">
+      <c r="E61" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F61" s="64" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="44"/>
-      <c r="B62" s="54" t="s">
+      <c r="A62" s="70"/>
+      <c r="B62" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="C62" s="48" t="s">
+      <c r="C62" s="72" t="s">
         <v>3</v>
       </c>
       <c r="D62" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E62" s="49">
+      <c r="E62" s="46">
         <v>-5887505.8404999999</v>
       </c>
-      <c r="F62" s="67">
+      <c r="F62" s="60">
         <f t="shared" si="10"/>
         <v>-11.17200000025332</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="44"/>
-      <c r="B63" s="54"/>
-      <c r="C63" s="48"/>
+      <c r="A63" s="70"/>
+      <c r="B63" s="73"/>
+      <c r="C63" s="72"/>
       <c r="D63" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E63" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="F63" s="71" t="s">
+      <c r="E63" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F63" s="64" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="44"/>
-      <c r="B64" s="54"/>
-      <c r="C64" s="54" t="s">
+      <c r="A64" s="70"/>
+      <c r="B64" s="73"/>
+      <c r="C64" s="73" t="s">
         <v>4</v>
       </c>
       <c r="D64" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E64" s="56">
+      <c r="E64" s="50">
         <v>-5887494.6684999997</v>
       </c>
-      <c r="F64" s="60">
+      <c r="F64" s="53">
         <f t="shared" si="11"/>
         <v>11.17200000025332</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="45"/>
-      <c r="B65" s="55"/>
-      <c r="C65" s="55"/>
+      <c r="A65" s="71"/>
+      <c r="B65" s="74"/>
+      <c r="C65" s="74"/>
       <c r="D65" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E65" s="52" t="s">
-        <v>40</v>
-      </c>
-      <c r="F65" s="69" t="s">
+      <c r="E65" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="F65" s="62" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="44" t="s">
+      <c r="A66" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="B66" s="48" t="s">
+      <c r="B66" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="C66" s="48" t="s">
+      <c r="C66" s="72" t="s">
         <v>3</v>
       </c>
       <c r="D66" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E66" s="49">
+      <c r="E66" s="46">
         <v>-5896016.4718000004</v>
       </c>
-      <c r="F66" s="67">
+      <c r="F66" s="60">
         <f t="shared" si="8"/>
         <v>-2.3832000000402331</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="44"/>
-      <c r="B67" s="48"/>
-      <c r="C67" s="48"/>
+      <c r="A67" s="70"/>
+      <c r="B67" s="72"/>
+      <c r="C67" s="72"/>
       <c r="D67" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E67" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="F67" s="71" t="s">
+      <c r="E67" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F67" s="64" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="44"/>
-      <c r="B68" s="48"/>
-      <c r="C68" s="48" t="s">
+      <c r="A68" s="70"/>
+      <c r="B68" s="72"/>
+      <c r="C68" s="72" t="s">
         <v>4</v>
       </c>
       <c r="D68" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E68" s="49">
+      <c r="E68" s="46">
         <v>-5896014.0886000004</v>
       </c>
-      <c r="F68" s="76">
+      <c r="F68" s="69">
         <f t="shared" si="9"/>
         <v>2.3832000000402331</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="44"/>
-      <c r="B69" s="48"/>
-      <c r="C69" s="48"/>
+      <c r="A69" s="70"/>
+      <c r="B69" s="72"/>
+      <c r="C69" s="72"/>
       <c r="D69" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E69" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="F69" s="71" t="s">
+      <c r="E69" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F69" s="64" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="44"/>
-      <c r="B70" s="46" t="s">
+      <c r="A70" s="70"/>
+      <c r="B70" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="C70" s="46" t="s">
+      <c r="C70" s="75" t="s">
         <v>3</v>
       </c>
       <c r="D70" s="11" t="s">
@@ -3119,128 +3253,128 @@
       <c r="E70" s="5">
         <v>-5882581.9853999997</v>
       </c>
-      <c r="F70" s="68">
+      <c r="F70" s="61">
         <f t="shared" si="10"/>
         <v>13297.716300000437</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="44"/>
-      <c r="B71" s="46"/>
-      <c r="C71" s="46"/>
+      <c r="A71" s="70"/>
+      <c r="B71" s="75"/>
+      <c r="C71" s="75"/>
       <c r="D71" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E71" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="F71" s="71" t="s">
+      <c r="E71" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F71" s="64" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="44"/>
-      <c r="B72" s="46"/>
-      <c r="C72" s="48" t="s">
+      <c r="A72" s="70"/>
+      <c r="B72" s="75"/>
+      <c r="C72" s="72" t="s">
         <v>4</v>
       </c>
       <c r="D72" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E72" s="49">
+      <c r="E72" s="46">
         <v>-5895879.7017000001</v>
       </c>
-      <c r="F72" s="67">
+      <c r="F72" s="60">
         <f t="shared" si="11"/>
         <v>-13297.716300000437</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="45"/>
-      <c r="B73" s="47"/>
-      <c r="C73" s="51"/>
+      <c r="A73" s="71"/>
+      <c r="B73" s="76"/>
+      <c r="C73" s="77"/>
       <c r="D73" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E73" s="52" t="s">
-        <v>40</v>
-      </c>
-      <c r="F73" s="69" t="s">
+      <c r="E73" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="F73" s="62" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="44" t="s">
+      <c r="A74" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="B74" s="48" t="s">
+      <c r="B74" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="C74" s="48" t="s">
+      <c r="C74" s="72" t="s">
         <v>3</v>
       </c>
       <c r="D74" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E74" s="49">
+      <c r="E74" s="46">
         <v>-5889520.4452999998</v>
       </c>
-      <c r="F74" s="74">
+      <c r="F74" s="67">
         <f t="shared" si="8"/>
         <v>5.2581000002101064</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="44"/>
-      <c r="B75" s="48"/>
-      <c r="C75" s="48"/>
+      <c r="A75" s="70"/>
+      <c r="B75" s="72"/>
+      <c r="C75" s="72"/>
       <c r="D75" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E75" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="F75" s="71" t="s">
+      <c r="E75" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F75" s="64" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="44"/>
-      <c r="B76" s="48"/>
-      <c r="C76" s="48" t="s">
+      <c r="A76" s="70"/>
+      <c r="B76" s="72"/>
+      <c r="C76" s="72" t="s">
         <v>4</v>
       </c>
       <c r="D76" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E76" s="49">
+      <c r="E76" s="46">
         <v>-5889525.7034</v>
       </c>
-      <c r="F76" s="67">
+      <c r="F76" s="60">
         <f t="shared" si="9"/>
         <v>-5.2581000002101064</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="44"/>
-      <c r="B77" s="48"/>
-      <c r="C77" s="48"/>
+      <c r="A77" s="70"/>
+      <c r="B77" s="72"/>
+      <c r="C77" s="72"/>
       <c r="D77" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E77" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="F77" s="71" t="s">
+      <c r="E77" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F77" s="64" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="44"/>
-      <c r="B78" s="46" t="s">
+      <c r="A78" s="70"/>
+      <c r="B78" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="C78" s="46" t="s">
+      <c r="C78" s="75" t="s">
         <v>3</v>
       </c>
       <c r="D78" s="11" t="s">
@@ -3249,128 +3383,128 @@
       <c r="E78" s="5">
         <v>-5889495.8046000004</v>
       </c>
-      <c r="F78" s="68">
+      <c r="F78" s="61">
         <f t="shared" si="10"/>
         <v>5.9207999994978309</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="44"/>
-      <c r="B79" s="46"/>
-      <c r="C79" s="46"/>
+      <c r="A79" s="70"/>
+      <c r="B79" s="75"/>
+      <c r="C79" s="75"/>
       <c r="D79" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E79" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="F79" s="71" t="s">
+      <c r="E79" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F79" s="64" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="44"/>
-      <c r="B80" s="46"/>
-      <c r="C80" s="48" t="s">
+      <c r="A80" s="70"/>
+      <c r="B80" s="75"/>
+      <c r="C80" s="72" t="s">
         <v>4</v>
       </c>
       <c r="D80" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E80" s="49">
+      <c r="E80" s="46">
         <v>-5889501.7253999999</v>
       </c>
-      <c r="F80" s="67">
+      <c r="F80" s="60">
         <f t="shared" si="11"/>
         <v>-5.9207999994978309</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="45"/>
-      <c r="B81" s="47"/>
-      <c r="C81" s="51"/>
+      <c r="A81" s="71"/>
+      <c r="B81" s="76"/>
+      <c r="C81" s="77"/>
       <c r="D81" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E81" s="52" t="s">
-        <v>40</v>
-      </c>
-      <c r="F81" s="69" t="s">
+      <c r="E81" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="F81" s="62" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="44" t="s">
+      <c r="A82" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="B82" s="48" t="s">
+      <c r="B82" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="C82" s="48" t="s">
+      <c r="C82" s="72" t="s">
         <v>3</v>
       </c>
       <c r="D82" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E82" s="49">
+      <c r="E82" s="46">
         <v>-5945574.0226999996</v>
       </c>
-      <c r="F82" s="74">
+      <c r="F82" s="67">
         <f t="shared" si="8"/>
         <v>28.820300000719726</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A83" s="44"/>
-      <c r="B83" s="48"/>
-      <c r="C83" s="48"/>
+      <c r="A83" s="70"/>
+      <c r="B83" s="72"/>
+      <c r="C83" s="72"/>
       <c r="D83" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E83" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="F83" s="71" t="s">
+      <c r="E83" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F83" s="64" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" s="44"/>
-      <c r="B84" s="48"/>
-      <c r="C84" s="48" t="s">
+      <c r="A84" s="70"/>
+      <c r="B84" s="72"/>
+      <c r="C84" s="72" t="s">
         <v>4</v>
       </c>
       <c r="D84" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E84" s="49">
+      <c r="E84" s="46">
         <v>-5945602.8430000003</v>
       </c>
-      <c r="F84" s="67">
+      <c r="F84" s="60">
         <f t="shared" si="9"/>
         <v>-28.820300000719726</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A85" s="44"/>
-      <c r="B85" s="48"/>
-      <c r="C85" s="48"/>
+      <c r="A85" s="70"/>
+      <c r="B85" s="72"/>
+      <c r="C85" s="72"/>
       <c r="D85" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E85" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="F85" s="71" t="s">
+      <c r="E85" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F85" s="64" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86" s="44"/>
-      <c r="B86" s="46" t="s">
+      <c r="A86" s="70"/>
+      <c r="B86" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="C86" s="46" t="s">
+      <c r="C86" s="75" t="s">
         <v>3</v>
       </c>
       <c r="D86" s="11" t="s">
@@ -3379,189 +3513,266 @@
       <c r="E86" s="5">
         <v>-5944614.3201000001</v>
       </c>
-      <c r="F86" s="68">
+      <c r="F86" s="61">
         <f t="shared" si="10"/>
         <v>12.378299999982119</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A87" s="44"/>
-      <c r="B87" s="46"/>
-      <c r="C87" s="46"/>
+      <c r="A87" s="70"/>
+      <c r="B87" s="75"/>
+      <c r="C87" s="75"/>
       <c r="D87" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E87" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="F87" s="71" t="s">
+      <c r="E87" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F87" s="64" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A88" s="44"/>
-      <c r="B88" s="46"/>
-      <c r="C88" s="48" t="s">
+      <c r="A88" s="70"/>
+      <c r="B88" s="75"/>
+      <c r="C88" s="72" t="s">
         <v>4</v>
       </c>
       <c r="D88" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E88" s="49">
+      <c r="E88" s="46">
         <v>-5944626.6984000001</v>
       </c>
-      <c r="F88" s="67">
+      <c r="F88" s="60">
         <f t="shared" si="11"/>
         <v>-12.378299999982119</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A89" s="45"/>
-      <c r="B89" s="47"/>
-      <c r="C89" s="51"/>
+      <c r="A89" s="71"/>
+      <c r="B89" s="76"/>
+      <c r="C89" s="77"/>
       <c r="D89" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E89" s="52" t="s">
-        <v>40</v>
-      </c>
-      <c r="F89" s="69" t="s">
+      <c r="E89" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="F89" s="62" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" s="44" t="s">
+      <c r="A90" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="B90" s="48" t="s">
+      <c r="B90" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="C90" s="48" t="s">
+      <c r="C90" s="72" t="s">
         <v>3</v>
       </c>
       <c r="D90" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E90" s="49">
+      <c r="E90" s="46">
         <v>-5892842.8987999996</v>
       </c>
-      <c r="F90" s="76">
+      <c r="F90" s="69">
         <f t="shared" si="8"/>
         <v>83.002000000327826</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A91" s="44"/>
-      <c r="B91" s="48"/>
-      <c r="C91" s="48"/>
+      <c r="A91" s="70"/>
+      <c r="B91" s="72"/>
+      <c r="C91" s="72"/>
       <c r="D91" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E91" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="F91" s="71" t="s">
+      <c r="E91" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F91" s="64" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92" s="44"/>
-      <c r="B92" s="48"/>
-      <c r="C92" s="48" t="s">
+      <c r="A92" s="70"/>
+      <c r="B92" s="72"/>
+      <c r="C92" s="72" t="s">
         <v>4</v>
       </c>
       <c r="D92" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E92" s="49">
+      <c r="E92" s="46">
         <v>-5892925.9007999999</v>
       </c>
-      <c r="F92" s="67">
+      <c r="F92" s="60">
         <f t="shared" si="9"/>
         <v>-83.002000000327826</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A93" s="44"/>
-      <c r="B93" s="48"/>
-      <c r="C93" s="48"/>
+      <c r="A93" s="70"/>
+      <c r="B93" s="72"/>
+      <c r="C93" s="72"/>
       <c r="D93" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E93" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="F93" s="71" t="s">
-        <v>40</v>
-      </c>
-      <c r="G93" s="53"/>
+      <c r="E93" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F93" s="64" t="s">
+        <v>40</v>
+      </c>
+      <c r="G93" s="49"/>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A94" s="44"/>
-      <c r="B94" s="54" t="s">
+      <c r="A94" s="70"/>
+      <c r="B94" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="C94" s="48" t="s">
+      <c r="C94" s="72" t="s">
         <v>3</v>
       </c>
       <c r="D94" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E94" s="49">
+      <c r="E94" s="46">
         <v>-5892741.3773999996</v>
       </c>
-      <c r="F94" s="67">
+      <c r="F94" s="60">
         <f t="shared" si="10"/>
         <v>-2.8141000000759959</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95" s="44"/>
-      <c r="B95" s="54"/>
-      <c r="C95" s="48"/>
+      <c r="A95" s="70"/>
+      <c r="B95" s="73"/>
+      <c r="C95" s="72"/>
       <c r="D95" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E95" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="F95" s="71" t="s">
+      <c r="E95" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F95" s="64" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A96" s="44"/>
-      <c r="B96" s="54"/>
-      <c r="C96" s="54" t="s">
+      <c r="A96" s="70"/>
+      <c r="B96" s="73"/>
+      <c r="C96" s="73" t="s">
         <v>4</v>
       </c>
       <c r="D96" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E96" s="56">
+      <c r="E96" s="50">
         <v>-5892738.5632999996</v>
       </c>
-      <c r="F96" s="60">
+      <c r="F96" s="53">
         <f t="shared" si="11"/>
         <v>2.8141000000759959</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" s="45"/>
-      <c r="B97" s="55"/>
-      <c r="C97" s="55"/>
+      <c r="A97" s="71"/>
+      <c r="B97" s="74"/>
+      <c r="C97" s="74"/>
       <c r="D97" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E97" s="52" t="s">
-        <v>40</v>
-      </c>
-      <c r="F97" s="70" t="s">
+      <c r="E97" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="F97" s="63" t="s">
         <v>40</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="84">
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="A10:A17"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="A18:A25"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="A26:A33"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="A34:A41"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="A42:A49"/>
+    <mergeCell ref="B42:B45"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="B46:B49"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="A50:A57"/>
+    <mergeCell ref="B50:B53"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="B54:B57"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="A58:A65"/>
+    <mergeCell ref="B58:B61"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="B62:B65"/>
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="C64:C65"/>
+    <mergeCell ref="A66:A73"/>
+    <mergeCell ref="B66:B69"/>
+    <mergeCell ref="C66:C67"/>
+    <mergeCell ref="C68:C69"/>
+    <mergeCell ref="B70:B73"/>
+    <mergeCell ref="C70:C71"/>
+    <mergeCell ref="C72:C73"/>
+    <mergeCell ref="A74:A81"/>
+    <mergeCell ref="B74:B77"/>
+    <mergeCell ref="C74:C75"/>
+    <mergeCell ref="C76:C77"/>
+    <mergeCell ref="B78:B81"/>
+    <mergeCell ref="C78:C79"/>
+    <mergeCell ref="C80:C81"/>
+    <mergeCell ref="A82:A89"/>
+    <mergeCell ref="B82:B85"/>
+    <mergeCell ref="C82:C83"/>
+    <mergeCell ref="C84:C85"/>
+    <mergeCell ref="B86:B89"/>
+    <mergeCell ref="C86:C87"/>
+    <mergeCell ref="C88:C89"/>
     <mergeCell ref="A90:A97"/>
     <mergeCell ref="B90:B93"/>
     <mergeCell ref="C90:C91"/>
@@ -3569,90 +3780,781 @@
     <mergeCell ref="B94:B97"/>
     <mergeCell ref="C94:C95"/>
     <mergeCell ref="C96:C97"/>
-    <mergeCell ref="A82:A89"/>
-    <mergeCell ref="B82:B85"/>
-    <mergeCell ref="C82:C83"/>
-    <mergeCell ref="C84:C85"/>
-    <mergeCell ref="B86:B89"/>
-    <mergeCell ref="C86:C87"/>
-    <mergeCell ref="C88:C89"/>
-    <mergeCell ref="A74:A81"/>
-    <mergeCell ref="B74:B77"/>
-    <mergeCell ref="C74:C75"/>
-    <mergeCell ref="C76:C77"/>
-    <mergeCell ref="B78:B81"/>
-    <mergeCell ref="C78:C79"/>
-    <mergeCell ref="C80:C81"/>
-    <mergeCell ref="A66:A73"/>
-    <mergeCell ref="B66:B69"/>
-    <mergeCell ref="C66:C67"/>
-    <mergeCell ref="C68:C69"/>
-    <mergeCell ref="B70:B73"/>
-    <mergeCell ref="C70:C71"/>
-    <mergeCell ref="C72:C73"/>
-    <mergeCell ref="A58:A65"/>
-    <mergeCell ref="B58:B61"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="B62:B65"/>
-    <mergeCell ref="C62:C63"/>
-    <mergeCell ref="C64:C65"/>
-    <mergeCell ref="A50:A57"/>
-    <mergeCell ref="B50:B53"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="B54:B57"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="A42:A49"/>
-    <mergeCell ref="B42:B45"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="B46:B49"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="A34:A41"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="B38:B41"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="A26:A33"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="A18:A25"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="A10:A17"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="A2:A9"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C6:C7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8F55FE9-ECCC-4F21-9AD8-39C9EB206E22}">
+  <dimension ref="A1:H49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E25" sqref="E24:E25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="27.42578125" customWidth="1"/>
+    <col min="5" max="6" width="27.85546875" customWidth="1"/>
+    <col min="7" max="7" width="21" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="85" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="86" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="4">
+        <v>-5873078.1357632903</v>
+      </c>
+      <c r="E2" s="96">
+        <f>D2-D3</f>
+        <v>669.48723918944597</v>
+      </c>
+      <c r="F2" s="96"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="87"/>
+    </row>
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="88"/>
+      <c r="B3" s="83"/>
+      <c r="C3" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="9">
+        <v>-5873747.6230024798</v>
+      </c>
+      <c r="E3" s="54">
+        <f>D3-D2</f>
+        <v>-669.48723918944597</v>
+      </c>
+      <c r="F3" s="54"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="89"/>
+    </row>
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="88"/>
+      <c r="B4" s="94" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="44" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="11">
+        <v>-5873065.7409666302</v>
+      </c>
+      <c r="E4" s="56">
+        <f>D4-D5</f>
+        <v>680.52461569011211</v>
+      </c>
+      <c r="F4" s="97">
+        <v>100000000</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="89"/>
+    </row>
+    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="90"/>
+      <c r="B5" s="95"/>
+      <c r="C5" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="3">
+        <v>-5873746.2655823203</v>
+      </c>
+      <c r="E5" s="92">
+        <f>D5-D4</f>
+        <v>-680.52461569011211</v>
+      </c>
+      <c r="F5" s="92"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="93"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="85" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="86" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="96">
+        <f>D6-D7</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="96"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="87"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="88"/>
+      <c r="B7" s="83"/>
+      <c r="C7" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="54">
+        <f>D7-D6</f>
+        <v>0</v>
+      </c>
+      <c r="F7" s="54"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="89"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="88"/>
+      <c r="B8" s="84" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="82">
+        <f>D8-D9</f>
+        <v>0</v>
+      </c>
+      <c r="F8" s="82"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="89"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="90"/>
+      <c r="B9" s="91"/>
+      <c r="C9" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="92">
+        <f>D9-D8</f>
+        <v>0</v>
+      </c>
+      <c r="F9" s="92"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="93"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="85" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="86" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="52"/>
+      <c r="G10" s="52"/>
+      <c r="H10" s="87"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="88"/>
+      <c r="B11" s="83"/>
+      <c r="C11" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="89"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="88"/>
+      <c r="B12" s="84" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="89"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="90"/>
+      <c r="B13" s="91"/>
+      <c r="C13" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="93"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="85" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="86" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="52"/>
+      <c r="E14" s="52"/>
+      <c r="F14" s="52"/>
+      <c r="G14" s="52"/>
+      <c r="H14" s="87"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="88"/>
+      <c r="B15" s="83"/>
+      <c r="C15" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="89"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="88"/>
+      <c r="B16" s="84" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="89"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="90"/>
+      <c r="B17" s="91"/>
+      <c r="C17" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="93"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="85" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="86" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="52"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="52"/>
+      <c r="H18" s="87"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="88"/>
+      <c r="B19" s="83"/>
+      <c r="C19" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="89"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="88"/>
+      <c r="B20" s="84" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="89"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="90"/>
+      <c r="B21" s="91"/>
+      <c r="C21" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="93"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="85" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="86" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="52"/>
+      <c r="E22" s="52"/>
+      <c r="F22" s="52"/>
+      <c r="G22" s="52"/>
+      <c r="H22" s="87"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="88"/>
+      <c r="B23" s="83"/>
+      <c r="C23" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="89"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="88"/>
+      <c r="B24" s="84" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="89"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="90"/>
+      <c r="B25" s="91"/>
+      <c r="C25" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="93"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="85" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="86" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" s="52"/>
+      <c r="E26" s="52"/>
+      <c r="F26" s="52"/>
+      <c r="G26" s="52"/>
+      <c r="H26" s="87"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="88"/>
+      <c r="B27" s="83"/>
+      <c r="C27" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="89"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="88"/>
+      <c r="B28" s="84" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="89"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="90"/>
+      <c r="B29" s="91"/>
+      <c r="C29" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="93"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="85" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" s="86" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D30" s="52"/>
+      <c r="E30" s="52"/>
+      <c r="F30" s="52"/>
+      <c r="G30" s="52"/>
+      <c r="H30" s="87"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="88"/>
+      <c r="B31" s="83"/>
+      <c r="C31" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="89"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="88"/>
+      <c r="B32" s="84" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="89"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="90"/>
+      <c r="B33" s="91"/>
+      <c r="C33" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="93"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="85" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" s="86" t="s">
+        <v>19</v>
+      </c>
+      <c r="C34" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D34" s="52"/>
+      <c r="E34" s="52"/>
+      <c r="F34" s="52"/>
+      <c r="G34" s="52"/>
+      <c r="H34" s="87"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="88"/>
+      <c r="B35" s="83"/>
+      <c r="C35" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="89"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="88"/>
+      <c r="B36" s="84" t="s">
+        <v>20</v>
+      </c>
+      <c r="C36" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="89"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="90"/>
+      <c r="B37" s="91"/>
+      <c r="C37" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="93"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="85" t="s">
+        <v>13</v>
+      </c>
+      <c r="B38" s="86" t="s">
+        <v>19</v>
+      </c>
+      <c r="C38" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D38" s="52"/>
+      <c r="E38" s="52"/>
+      <c r="F38" s="52"/>
+      <c r="G38" s="52"/>
+      <c r="H38" s="87"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="88"/>
+      <c r="B39" s="83"/>
+      <c r="C39" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="89"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="88"/>
+      <c r="B40" s="84" t="s">
+        <v>20</v>
+      </c>
+      <c r="C40" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="89"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="90"/>
+      <c r="B41" s="91"/>
+      <c r="C41" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="93"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="85" t="s">
+        <v>14</v>
+      </c>
+      <c r="B42" s="86" t="s">
+        <v>19</v>
+      </c>
+      <c r="C42" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D42" s="52"/>
+      <c r="E42" s="52"/>
+      <c r="F42" s="52"/>
+      <c r="G42" s="52"/>
+      <c r="H42" s="87"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="88"/>
+      <c r="B43" s="83"/>
+      <c r="C43" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="89"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="88"/>
+      <c r="B44" s="84" t="s">
+        <v>20</v>
+      </c>
+      <c r="C44" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="89"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="90"/>
+      <c r="B45" s="91"/>
+      <c r="C45" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="93"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="85" t="s">
+        <v>15</v>
+      </c>
+      <c r="B46" s="86" t="s">
+        <v>19</v>
+      </c>
+      <c r="C46" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D46" s="52"/>
+      <c r="E46" s="52"/>
+      <c r="F46" s="52"/>
+      <c r="G46" s="52"/>
+      <c r="H46" s="87"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="88"/>
+      <c r="B47" s="83"/>
+      <c r="C47" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="89"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="88"/>
+      <c r="B48" s="84" t="s">
+        <v>20</v>
+      </c>
+      <c r="C48" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="89"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="90"/>
+      <c r="B49" s="91"/>
+      <c r="C49" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="7"/>
+      <c r="H49" s="93"/>
+    </row>
+  </sheetData>
+  <mergeCells count="36">
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="A46:A49"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
prep 2.ANT model test
</commit_message>
<xml_diff>
--- a/main/beast/all/chromosome/clade/clades_data_summary.xlsx
+++ b/main/beast/all/chromosome/clade/clades_data_summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ktmea\Projects\plague-phylogeography-projects\main\beast\all\chromosome\clade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{950A7271-540C-4A18-82F2-F797DD32D8F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{578EF074-EE21-4794-9451-C3341EC0C21B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1023,44 +1023,68 @@
     <xf numFmtId="164" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1068,38 +1092,14 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1467,7 +1467,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2085,8 +2085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H97"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2124,13 +2124,13 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="70" t="s">
+      <c r="A2" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="80" t="s">
+      <c r="B2" s="79" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="80" t="s">
+      <c r="C2" s="79" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -2146,9 +2146,9 @@
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="70"/>
-      <c r="B3" s="80"/>
-      <c r="C3" s="80"/>
+      <c r="A3" s="77"/>
+      <c r="B3" s="79"/>
+      <c r="C3" s="79"/>
       <c r="D3" s="2" t="s">
         <v>33</v>
       </c>
@@ -2161,9 +2161,9 @@
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="70"/>
-      <c r="B4" s="80"/>
-      <c r="C4" s="80" t="s">
+      <c r="A4" s="77"/>
+      <c r="B4" s="79"/>
+      <c r="C4" s="79" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -2179,9 +2179,9 @@
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="70"/>
-      <c r="B5" s="80"/>
-      <c r="C5" s="80"/>
+      <c r="A5" s="77"/>
+      <c r="B5" s="79"/>
+      <c r="C5" s="79"/>
       <c r="D5" s="2" t="s">
         <v>33</v>
       </c>
@@ -2194,11 +2194,11 @@
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="70"/>
-      <c r="B6" s="75" t="s">
+      <c r="A6" s="77"/>
+      <c r="B6" s="80" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="75" t="s">
+      <c r="C6" s="80" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="11" t="s">
@@ -2214,9 +2214,9 @@
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="70"/>
-      <c r="B7" s="75"/>
-      <c r="C7" s="75"/>
+      <c r="A7" s="77"/>
+      <c r="B7" s="80"/>
+      <c r="C7" s="80"/>
       <c r="D7" s="2" t="s">
         <v>33</v>
       </c>
@@ -2229,9 +2229,9 @@
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="70"/>
-      <c r="B8" s="75"/>
-      <c r="C8" s="80" t="s">
+      <c r="A8" s="77"/>
+      <c r="B8" s="80"/>
+      <c r="C8" s="79" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -2247,9 +2247,9 @@
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="71"/>
-      <c r="B9" s="76"/>
-      <c r="C9" s="81"/>
+      <c r="A9" s="78"/>
+      <c r="B9" s="81"/>
+      <c r="C9" s="82"/>
       <c r="D9" s="3" t="s">
         <v>33</v>
       </c>
@@ -2262,13 +2262,13 @@
       <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="78" t="s">
+      <c r="A10" s="83" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="79" t="s">
+      <c r="B10" s="84" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="79" t="s">
+      <c r="C10" s="84" t="s">
         <v>3</v>
       </c>
       <c r="D10" s="4" t="s">
@@ -2284,9 +2284,9 @@
       <c r="G10" s="52"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="70"/>
-      <c r="B11" s="80"/>
-      <c r="C11" s="80"/>
+      <c r="A11" s="77"/>
+      <c r="B11" s="79"/>
+      <c r="C11" s="79"/>
       <c r="D11" s="2" t="s">
         <v>33</v>
       </c>
@@ -2299,9 +2299,9 @@
       <c r="G11" s="6"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="70"/>
-      <c r="B12" s="80"/>
-      <c r="C12" s="80" t="s">
+      <c r="A12" s="77"/>
+      <c r="B12" s="79"/>
+      <c r="C12" s="79" t="s">
         <v>4</v>
       </c>
       <c r="D12" s="2" t="s">
@@ -2317,9 +2317,9 @@
       <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="70"/>
-      <c r="B13" s="80"/>
-      <c r="C13" s="80"/>
+      <c r="A13" s="77"/>
+      <c r="B13" s="79"/>
+      <c r="C13" s="79"/>
       <c r="D13" s="2" t="s">
         <v>33</v>
       </c>
@@ -2332,11 +2332,11 @@
       <c r="G13" s="6"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="70"/>
-      <c r="B14" s="73" t="s">
+      <c r="A14" s="77"/>
+      <c r="B14" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="80" t="s">
+      <c r="C14" s="79" t="s">
         <v>3</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -2352,9 +2352,9 @@
       <c r="G14" s="6"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="70"/>
-      <c r="B15" s="73"/>
-      <c r="C15" s="80"/>
+      <c r="A15" s="77"/>
+      <c r="B15" s="85"/>
+      <c r="C15" s="79"/>
       <c r="D15" s="2" t="s">
         <v>33</v>
       </c>
@@ -2367,9 +2367,9 @@
       <c r="G15" s="6"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="70"/>
-      <c r="B16" s="73"/>
-      <c r="C16" s="73" t="s">
+      <c r="A16" s="77"/>
+      <c r="B16" s="85"/>
+      <c r="C16" s="85" t="s">
         <v>4</v>
       </c>
       <c r="D16" s="8" t="s">
@@ -2385,9 +2385,9 @@
       <c r="G16" s="6"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="71"/>
-      <c r="B17" s="74"/>
-      <c r="C17" s="74"/>
+      <c r="A17" s="78"/>
+      <c r="B17" s="86"/>
+      <c r="C17" s="86"/>
       <c r="D17" s="3" t="s">
         <v>33</v>
       </c>
@@ -2400,13 +2400,13 @@
       <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="70" t="s">
+      <c r="A18" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="72" t="s">
+      <c r="B18" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="72" t="s">
+      <c r="C18" s="87" t="s">
         <v>3</v>
       </c>
       <c r="D18" s="9" t="s">
@@ -2421,9 +2421,9 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="70"/>
-      <c r="B19" s="72"/>
-      <c r="C19" s="72"/>
+      <c r="A19" s="77"/>
+      <c r="B19" s="87"/>
+      <c r="C19" s="87"/>
       <c r="D19" s="9" t="s">
         <v>33</v>
       </c>
@@ -2435,9 +2435,9 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="70"/>
-      <c r="B20" s="72"/>
-      <c r="C20" s="72" t="s">
+      <c r="A20" s="77"/>
+      <c r="B20" s="87"/>
+      <c r="C20" s="87" t="s">
         <v>4</v>
       </c>
       <c r="D20" s="9" t="s">
@@ -2452,9 +2452,9 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="70"/>
-      <c r="B21" s="72"/>
-      <c r="C21" s="72"/>
+      <c r="A21" s="77"/>
+      <c r="B21" s="87"/>
+      <c r="C21" s="87"/>
       <c r="D21" s="9" t="s">
         <v>33</v>
       </c>
@@ -2466,11 +2466,11 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="70"/>
-      <c r="B22" s="75" t="s">
+      <c r="A22" s="77"/>
+      <c r="B22" s="80" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="75" t="s">
+      <c r="C22" s="80" t="s">
         <v>3</v>
       </c>
       <c r="D22" s="11" t="s">
@@ -2485,9 +2485,9 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="70"/>
-      <c r="B23" s="75"/>
-      <c r="C23" s="75"/>
+      <c r="A23" s="77"/>
+      <c r="B23" s="80"/>
+      <c r="C23" s="80"/>
       <c r="D23" s="9" t="s">
         <v>33</v>
       </c>
@@ -2499,9 +2499,9 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="70"/>
-      <c r="B24" s="75"/>
-      <c r="C24" s="72" t="s">
+      <c r="A24" s="77"/>
+      <c r="B24" s="80"/>
+      <c r="C24" s="87" t="s">
         <v>4</v>
       </c>
       <c r="D24" s="9" t="s">
@@ -2516,9 +2516,9 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="71"/>
-      <c r="B25" s="76"/>
-      <c r="C25" s="77"/>
+      <c r="A25" s="78"/>
+      <c r="B25" s="81"/>
+      <c r="C25" s="88"/>
       <c r="D25" s="10" t="s">
         <v>33</v>
       </c>
@@ -2530,13 +2530,13 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="70" t="s">
+      <c r="A26" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="B26" s="72" t="s">
+      <c r="B26" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="72" t="s">
+      <c r="C26" s="87" t="s">
         <v>3</v>
       </c>
       <c r="D26" s="9" t="s">
@@ -2551,9 +2551,9 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="70"/>
-      <c r="B27" s="72"/>
-      <c r="C27" s="72"/>
+      <c r="A27" s="77"/>
+      <c r="B27" s="87"/>
+      <c r="C27" s="87"/>
       <c r="D27" s="9" t="s">
         <v>33</v>
       </c>
@@ -2565,9 +2565,9 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="70"/>
-      <c r="B28" s="72"/>
-      <c r="C28" s="72" t="s">
+      <c r="A28" s="77"/>
+      <c r="B28" s="87"/>
+      <c r="C28" s="87" t="s">
         <v>4</v>
       </c>
       <c r="D28" s="9" t="s">
@@ -2582,9 +2582,9 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="70"/>
-      <c r="B29" s="72"/>
-      <c r="C29" s="72"/>
+      <c r="A29" s="77"/>
+      <c r="B29" s="87"/>
+      <c r="C29" s="87"/>
       <c r="D29" s="9" t="s">
         <v>33</v>
       </c>
@@ -2596,11 +2596,11 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="70"/>
-      <c r="B30" s="75" t="s">
+      <c r="A30" s="77"/>
+      <c r="B30" s="80" t="s">
         <v>20</v>
       </c>
-      <c r="C30" s="75" t="s">
+      <c r="C30" s="80" t="s">
         <v>3</v>
       </c>
       <c r="D30" s="11" t="s">
@@ -2615,9 +2615,9 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="70"/>
-      <c r="B31" s="75"/>
-      <c r="C31" s="75"/>
+      <c r="A31" s="77"/>
+      <c r="B31" s="80"/>
+      <c r="C31" s="80"/>
       <c r="D31" s="9" t="s">
         <v>33</v>
       </c>
@@ -2629,9 +2629,9 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="70"/>
-      <c r="B32" s="75"/>
-      <c r="C32" s="72" t="s">
+      <c r="A32" s="77"/>
+      <c r="B32" s="80"/>
+      <c r="C32" s="87" t="s">
         <v>4</v>
       </c>
       <c r="D32" s="9" t="s">
@@ -2646,9 +2646,9 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="71"/>
-      <c r="B33" s="76"/>
-      <c r="C33" s="77"/>
+      <c r="A33" s="78"/>
+      <c r="B33" s="81"/>
+      <c r="C33" s="88"/>
       <c r="D33" s="10" t="s">
         <v>33</v>
       </c>
@@ -2660,13 +2660,13 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="70" t="s">
+      <c r="A34" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="B34" s="72" t="s">
+      <c r="B34" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="C34" s="72" t="s">
+      <c r="C34" s="87" t="s">
         <v>3</v>
       </c>
       <c r="D34" s="9" t="s">
@@ -2681,9 +2681,9 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="70"/>
-      <c r="B35" s="72"/>
-      <c r="C35" s="72"/>
+      <c r="A35" s="77"/>
+      <c r="B35" s="87"/>
+      <c r="C35" s="87"/>
       <c r="D35" s="9" t="s">
         <v>33</v>
       </c>
@@ -2695,9 +2695,9 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="70"/>
-      <c r="B36" s="72"/>
-      <c r="C36" s="72" t="s">
+      <c r="A36" s="77"/>
+      <c r="B36" s="87"/>
+      <c r="C36" s="87" t="s">
         <v>4</v>
       </c>
       <c r="D36" s="9" t="s">
@@ -2712,9 +2712,9 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="70"/>
-      <c r="B37" s="72"/>
-      <c r="C37" s="72"/>
+      <c r="A37" s="77"/>
+      <c r="B37" s="87"/>
+      <c r="C37" s="87"/>
       <c r="D37" s="9" t="s">
         <v>33</v>
       </c>
@@ -2726,11 +2726,11 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="70"/>
-      <c r="B38" s="75" t="s">
+      <c r="A38" s="77"/>
+      <c r="B38" s="80" t="s">
         <v>20</v>
       </c>
-      <c r="C38" s="75" t="s">
+      <c r="C38" s="80" t="s">
         <v>3</v>
       </c>
       <c r="D38" s="11" t="s">
@@ -2745,9 +2745,9 @@
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="70"/>
-      <c r="B39" s="75"/>
-      <c r="C39" s="75"/>
+      <c r="A39" s="77"/>
+      <c r="B39" s="80"/>
+      <c r="C39" s="80"/>
       <c r="D39" s="9" t="s">
         <v>33</v>
       </c>
@@ -2759,9 +2759,9 @@
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="70"/>
-      <c r="B40" s="75"/>
-      <c r="C40" s="72" t="s">
+      <c r="A40" s="77"/>
+      <c r="B40" s="80"/>
+      <c r="C40" s="87" t="s">
         <v>4</v>
       </c>
       <c r="D40" s="9" t="s">
@@ -2776,9 +2776,9 @@
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="71"/>
-      <c r="B41" s="76"/>
-      <c r="C41" s="77"/>
+      <c r="A41" s="78"/>
+      <c r="B41" s="81"/>
+      <c r="C41" s="88"/>
       <c r="D41" s="10" t="s">
         <v>33</v>
       </c>
@@ -2790,13 +2790,13 @@
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="70" t="s">
+      <c r="A42" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="B42" s="72" t="s">
+      <c r="B42" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="C42" s="72" t="s">
+      <c r="C42" s="87" t="s">
         <v>3</v>
       </c>
       <c r="D42" s="9" t="s">
@@ -2811,9 +2811,9 @@
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="70"/>
-      <c r="B43" s="72"/>
-      <c r="C43" s="72"/>
+      <c r="A43" s="77"/>
+      <c r="B43" s="87"/>
+      <c r="C43" s="87"/>
       <c r="D43" s="9" t="s">
         <v>33</v>
       </c>
@@ -2823,9 +2823,9 @@
       <c r="F43" s="60"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="70"/>
-      <c r="B44" s="72"/>
-      <c r="C44" s="72" t="s">
+      <c r="A44" s="77"/>
+      <c r="B44" s="87"/>
+      <c r="C44" s="87" t="s">
         <v>4</v>
       </c>
       <c r="D44" s="9" t="s">
@@ -2840,9 +2840,9 @@
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="70"/>
-      <c r="B45" s="72"/>
-      <c r="C45" s="72"/>
+      <c r="A45" s="77"/>
+      <c r="B45" s="87"/>
+      <c r="C45" s="87"/>
       <c r="D45" s="9" t="s">
         <v>33</v>
       </c>
@@ -2852,11 +2852,11 @@
       <c r="F45" s="60"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="70"/>
-      <c r="B46" s="73" t="s">
+      <c r="A46" s="77"/>
+      <c r="B46" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="C46" s="72" t="s">
+      <c r="C46" s="87" t="s">
         <v>3</v>
       </c>
       <c r="D46" s="9" t="s">
@@ -2871,9 +2871,9 @@
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="70"/>
-      <c r="B47" s="73"/>
-      <c r="C47" s="72"/>
+      <c r="A47" s="77"/>
+      <c r="B47" s="85"/>
+      <c r="C47" s="87"/>
       <c r="D47" s="9" t="s">
         <v>33</v>
       </c>
@@ -2883,9 +2883,9 @@
       <c r="F47" s="60"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="70"/>
-      <c r="B48" s="73"/>
-      <c r="C48" s="73" t="s">
+      <c r="A48" s="77"/>
+      <c r="B48" s="85"/>
+      <c r="C48" s="85" t="s">
         <v>4</v>
       </c>
       <c r="D48" s="8" t="s">
@@ -2900,9 +2900,9 @@
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="71"/>
-      <c r="B49" s="74"/>
-      <c r="C49" s="74"/>
+      <c r="A49" s="78"/>
+      <c r="B49" s="86"/>
+      <c r="C49" s="86"/>
       <c r="D49" s="10" t="s">
         <v>33</v>
       </c>
@@ -2914,13 +2914,13 @@
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="70" t="s">
+      <c r="A50" s="77" t="s">
         <v>10</v>
       </c>
-      <c r="B50" s="72" t="s">
+      <c r="B50" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="C50" s="72" t="s">
+      <c r="C50" s="87" t="s">
         <v>3</v>
       </c>
       <c r="D50" s="9" t="s">
@@ -2935,9 +2935,9 @@
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="70"/>
-      <c r="B51" s="72"/>
-      <c r="C51" s="72"/>
+      <c r="A51" s="77"/>
+      <c r="B51" s="87"/>
+      <c r="C51" s="87"/>
       <c r="D51" s="9" t="s">
         <v>33</v>
       </c>
@@ -2949,9 +2949,9 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="70"/>
-      <c r="B52" s="72"/>
-      <c r="C52" s="72" t="s">
+      <c r="A52" s="77"/>
+      <c r="B52" s="87"/>
+      <c r="C52" s="87" t="s">
         <v>4</v>
       </c>
       <c r="D52" s="9" t="s">
@@ -2966,9 +2966,9 @@
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="70"/>
-      <c r="B53" s="72"/>
-      <c r="C53" s="72"/>
+      <c r="A53" s="77"/>
+      <c r="B53" s="87"/>
+      <c r="C53" s="87"/>
       <c r="D53" s="9" t="s">
         <v>33</v>
       </c>
@@ -2980,11 +2980,11 @@
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="70"/>
-      <c r="B54" s="75" t="s">
+      <c r="A54" s="77"/>
+      <c r="B54" s="80" t="s">
         <v>20</v>
       </c>
-      <c r="C54" s="75" t="s">
+      <c r="C54" s="80" t="s">
         <v>3</v>
       </c>
       <c r="D54" s="11" t="s">
@@ -2999,9 +2999,9 @@
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="70"/>
-      <c r="B55" s="75"/>
-      <c r="C55" s="75"/>
+      <c r="A55" s="77"/>
+      <c r="B55" s="80"/>
+      <c r="C55" s="80"/>
       <c r="D55" s="9" t="s">
         <v>33</v>
       </c>
@@ -3013,9 +3013,9 @@
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="70"/>
-      <c r="B56" s="75"/>
-      <c r="C56" s="72" t="s">
+      <c r="A56" s="77"/>
+      <c r="B56" s="80"/>
+      <c r="C56" s="87" t="s">
         <v>4</v>
       </c>
       <c r="D56" s="9" t="s">
@@ -3030,9 +3030,9 @@
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="71"/>
-      <c r="B57" s="76"/>
-      <c r="C57" s="77"/>
+      <c r="A57" s="78"/>
+      <c r="B57" s="81"/>
+      <c r="C57" s="88"/>
       <c r="D57" s="10" t="s">
         <v>33</v>
       </c>
@@ -3044,13 +3044,13 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="70" t="s">
+      <c r="A58" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="B58" s="72" t="s">
+      <c r="B58" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="C58" s="72" t="s">
+      <c r="C58" s="87" t="s">
         <v>3</v>
       </c>
       <c r="D58" s="9" t="s">
@@ -3065,9 +3065,9 @@
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="70"/>
-      <c r="B59" s="72"/>
-      <c r="C59" s="72"/>
+      <c r="A59" s="77"/>
+      <c r="B59" s="87"/>
+      <c r="C59" s="87"/>
       <c r="D59" s="9" t="s">
         <v>33</v>
       </c>
@@ -3079,9 +3079,9 @@
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="70"/>
-      <c r="B60" s="72"/>
-      <c r="C60" s="72" t="s">
+      <c r="A60" s="77"/>
+      <c r="B60" s="87"/>
+      <c r="C60" s="87" t="s">
         <v>4</v>
       </c>
       <c r="D60" s="9" t="s">
@@ -3096,9 +3096,9 @@
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="70"/>
-      <c r="B61" s="72"/>
-      <c r="C61" s="72"/>
+      <c r="A61" s="77"/>
+      <c r="B61" s="87"/>
+      <c r="C61" s="87"/>
       <c r="D61" s="9" t="s">
         <v>33</v>
       </c>
@@ -3110,11 +3110,11 @@
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="70"/>
-      <c r="B62" s="73" t="s">
+      <c r="A62" s="77"/>
+      <c r="B62" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="C62" s="72" t="s">
+      <c r="C62" s="87" t="s">
         <v>3</v>
       </c>
       <c r="D62" s="9" t="s">
@@ -3129,9 +3129,9 @@
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="70"/>
-      <c r="B63" s="73"/>
-      <c r="C63" s="72"/>
+      <c r="A63" s="77"/>
+      <c r="B63" s="85"/>
+      <c r="C63" s="87"/>
       <c r="D63" s="9" t="s">
         <v>33</v>
       </c>
@@ -3143,9 +3143,9 @@
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="70"/>
-      <c r="B64" s="73"/>
-      <c r="C64" s="73" t="s">
+      <c r="A64" s="77"/>
+      <c r="B64" s="85"/>
+      <c r="C64" s="85" t="s">
         <v>4</v>
       </c>
       <c r="D64" s="8" t="s">
@@ -3160,9 +3160,9 @@
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="71"/>
-      <c r="B65" s="74"/>
-      <c r="C65" s="74"/>
+      <c r="A65" s="78"/>
+      <c r="B65" s="86"/>
+      <c r="C65" s="86"/>
       <c r="D65" s="10" t="s">
         <v>33</v>
       </c>
@@ -3174,13 +3174,13 @@
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="70" t="s">
+      <c r="A66" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="B66" s="72" t="s">
+      <c r="B66" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="C66" s="72" t="s">
+      <c r="C66" s="87" t="s">
         <v>3</v>
       </c>
       <c r="D66" s="9" t="s">
@@ -3195,9 +3195,9 @@
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="70"/>
-      <c r="B67" s="72"/>
-      <c r="C67" s="72"/>
+      <c r="A67" s="77"/>
+      <c r="B67" s="87"/>
+      <c r="C67" s="87"/>
       <c r="D67" s="9" t="s">
         <v>33</v>
       </c>
@@ -3209,9 +3209,9 @@
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="70"/>
-      <c r="B68" s="72"/>
-      <c r="C68" s="72" t="s">
+      <c r="A68" s="77"/>
+      <c r="B68" s="87"/>
+      <c r="C68" s="87" t="s">
         <v>4</v>
       </c>
       <c r="D68" s="9" t="s">
@@ -3226,9 +3226,9 @@
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="70"/>
-      <c r="B69" s="72"/>
-      <c r="C69" s="72"/>
+      <c r="A69" s="77"/>
+      <c r="B69" s="87"/>
+      <c r="C69" s="87"/>
       <c r="D69" s="9" t="s">
         <v>33</v>
       </c>
@@ -3240,11 +3240,11 @@
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="70"/>
-      <c r="B70" s="75" t="s">
+      <c r="A70" s="77"/>
+      <c r="B70" s="80" t="s">
         <v>20</v>
       </c>
-      <c r="C70" s="75" t="s">
+      <c r="C70" s="80" t="s">
         <v>3</v>
       </c>
       <c r="D70" s="11" t="s">
@@ -3259,9 +3259,9 @@
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="70"/>
-      <c r="B71" s="75"/>
-      <c r="C71" s="75"/>
+      <c r="A71" s="77"/>
+      <c r="B71" s="80"/>
+      <c r="C71" s="80"/>
       <c r="D71" s="9" t="s">
         <v>33</v>
       </c>
@@ -3273,9 +3273,9 @@
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="70"/>
-      <c r="B72" s="75"/>
-      <c r="C72" s="72" t="s">
+      <c r="A72" s="77"/>
+      <c r="B72" s="80"/>
+      <c r="C72" s="87" t="s">
         <v>4</v>
       </c>
       <c r="D72" s="9" t="s">
@@ -3290,9 +3290,9 @@
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="71"/>
-      <c r="B73" s="76"/>
-      <c r="C73" s="77"/>
+      <c r="A73" s="78"/>
+      <c r="B73" s="81"/>
+      <c r="C73" s="88"/>
       <c r="D73" s="10" t="s">
         <v>33</v>
       </c>
@@ -3304,13 +3304,13 @@
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="70" t="s">
+      <c r="A74" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="B74" s="72" t="s">
+      <c r="B74" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="C74" s="72" t="s">
+      <c r="C74" s="87" t="s">
         <v>3</v>
       </c>
       <c r="D74" s="9" t="s">
@@ -3325,9 +3325,9 @@
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="70"/>
-      <c r="B75" s="72"/>
-      <c r="C75" s="72"/>
+      <c r="A75" s="77"/>
+      <c r="B75" s="87"/>
+      <c r="C75" s="87"/>
       <c r="D75" s="9" t="s">
         <v>33</v>
       </c>
@@ -3339,9 +3339,9 @@
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="70"/>
-      <c r="B76" s="72"/>
-      <c r="C76" s="72" t="s">
+      <c r="A76" s="77"/>
+      <c r="B76" s="87"/>
+      <c r="C76" s="87" t="s">
         <v>4</v>
       </c>
       <c r="D76" s="9" t="s">
@@ -3356,9 +3356,9 @@
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="70"/>
-      <c r="B77" s="72"/>
-      <c r="C77" s="72"/>
+      <c r="A77" s="77"/>
+      <c r="B77" s="87"/>
+      <c r="C77" s="87"/>
       <c r="D77" s="9" t="s">
         <v>33</v>
       </c>
@@ -3370,11 +3370,11 @@
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="70"/>
-      <c r="B78" s="75" t="s">
+      <c r="A78" s="77"/>
+      <c r="B78" s="80" t="s">
         <v>20</v>
       </c>
-      <c r="C78" s="75" t="s">
+      <c r="C78" s="80" t="s">
         <v>3</v>
       </c>
       <c r="D78" s="11" t="s">
@@ -3389,9 +3389,9 @@
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="70"/>
-      <c r="B79" s="75"/>
-      <c r="C79" s="75"/>
+      <c r="A79" s="77"/>
+      <c r="B79" s="80"/>
+      <c r="C79" s="80"/>
       <c r="D79" s="9" t="s">
         <v>33</v>
       </c>
@@ -3403,9 +3403,9 @@
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="70"/>
-      <c r="B80" s="75"/>
-      <c r="C80" s="72" t="s">
+      <c r="A80" s="77"/>
+      <c r="B80" s="80"/>
+      <c r="C80" s="87" t="s">
         <v>4</v>
       </c>
       <c r="D80" s="9" t="s">
@@ -3420,9 +3420,9 @@
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="71"/>
-      <c r="B81" s="76"/>
-      <c r="C81" s="77"/>
+      <c r="A81" s="78"/>
+      <c r="B81" s="81"/>
+      <c r="C81" s="88"/>
       <c r="D81" s="10" t="s">
         <v>33</v>
       </c>
@@ -3434,13 +3434,13 @@
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="70" t="s">
+      <c r="A82" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="B82" s="72" t="s">
+      <c r="B82" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="C82" s="72" t="s">
+      <c r="C82" s="87" t="s">
         <v>3</v>
       </c>
       <c r="D82" s="9" t="s">
@@ -3455,9 +3455,9 @@
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A83" s="70"/>
-      <c r="B83" s="72"/>
-      <c r="C83" s="72"/>
+      <c r="A83" s="77"/>
+      <c r="B83" s="87"/>
+      <c r="C83" s="87"/>
       <c r="D83" s="9" t="s">
         <v>33</v>
       </c>
@@ -3469,9 +3469,9 @@
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" s="70"/>
-      <c r="B84" s="72"/>
-      <c r="C84" s="72" t="s">
+      <c r="A84" s="77"/>
+      <c r="B84" s="87"/>
+      <c r="C84" s="87" t="s">
         <v>4</v>
       </c>
       <c r="D84" s="9" t="s">
@@ -3486,9 +3486,9 @@
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A85" s="70"/>
-      <c r="B85" s="72"/>
-      <c r="C85" s="72"/>
+      <c r="A85" s="77"/>
+      <c r="B85" s="87"/>
+      <c r="C85" s="87"/>
       <c r="D85" s="9" t="s">
         <v>33</v>
       </c>
@@ -3500,11 +3500,11 @@
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86" s="70"/>
-      <c r="B86" s="75" t="s">
+      <c r="A86" s="77"/>
+      <c r="B86" s="80" t="s">
         <v>20</v>
       </c>
-      <c r="C86" s="75" t="s">
+      <c r="C86" s="80" t="s">
         <v>3</v>
       </c>
       <c r="D86" s="11" t="s">
@@ -3519,9 +3519,9 @@
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A87" s="70"/>
-      <c r="B87" s="75"/>
-      <c r="C87" s="75"/>
+      <c r="A87" s="77"/>
+      <c r="B87" s="80"/>
+      <c r="C87" s="80"/>
       <c r="D87" s="9" t="s">
         <v>33</v>
       </c>
@@ -3533,9 +3533,9 @@
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A88" s="70"/>
-      <c r="B88" s="75"/>
-      <c r="C88" s="72" t="s">
+      <c r="A88" s="77"/>
+      <c r="B88" s="80"/>
+      <c r="C88" s="87" t="s">
         <v>4</v>
       </c>
       <c r="D88" s="9" t="s">
@@ -3550,9 +3550,9 @@
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A89" s="71"/>
-      <c r="B89" s="76"/>
-      <c r="C89" s="77"/>
+      <c r="A89" s="78"/>
+      <c r="B89" s="81"/>
+      <c r="C89" s="88"/>
       <c r="D89" s="10" t="s">
         <v>33</v>
       </c>
@@ -3564,13 +3564,13 @@
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" s="70" t="s">
+      <c r="A90" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="B90" s="72" t="s">
+      <c r="B90" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="C90" s="72" t="s">
+      <c r="C90" s="87" t="s">
         <v>3</v>
       </c>
       <c r="D90" s="9" t="s">
@@ -3585,9 +3585,9 @@
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A91" s="70"/>
-      <c r="B91" s="72"/>
-      <c r="C91" s="72"/>
+      <c r="A91" s="77"/>
+      <c r="B91" s="87"/>
+      <c r="C91" s="87"/>
       <c r="D91" s="9" t="s">
         <v>33</v>
       </c>
@@ -3599,9 +3599,9 @@
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92" s="70"/>
-      <c r="B92" s="72"/>
-      <c r="C92" s="72" t="s">
+      <c r="A92" s="77"/>
+      <c r="B92" s="87"/>
+      <c r="C92" s="87" t="s">
         <v>4</v>
       </c>
       <c r="D92" s="9" t="s">
@@ -3616,9 +3616,9 @@
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A93" s="70"/>
-      <c r="B93" s="72"/>
-      <c r="C93" s="72"/>
+      <c r="A93" s="77"/>
+      <c r="B93" s="87"/>
+      <c r="C93" s="87"/>
       <c r="D93" s="9" t="s">
         <v>33</v>
       </c>
@@ -3631,11 +3631,11 @@
       <c r="G93" s="49"/>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A94" s="70"/>
-      <c r="B94" s="73" t="s">
+      <c r="A94" s="77"/>
+      <c r="B94" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="C94" s="72" t="s">
+      <c r="C94" s="87" t="s">
         <v>3</v>
       </c>
       <c r="D94" s="9" t="s">
@@ -3650,9 +3650,9 @@
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95" s="70"/>
-      <c r="B95" s="73"/>
-      <c r="C95" s="72"/>
+      <c r="A95" s="77"/>
+      <c r="B95" s="85"/>
+      <c r="C95" s="87"/>
       <c r="D95" s="9" t="s">
         <v>33</v>
       </c>
@@ -3664,9 +3664,9 @@
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A96" s="70"/>
-      <c r="B96" s="73"/>
-      <c r="C96" s="73" t="s">
+      <c r="A96" s="77"/>
+      <c r="B96" s="85"/>
+      <c r="C96" s="85" t="s">
         <v>4</v>
       </c>
       <c r="D96" s="8" t="s">
@@ -3681,9 +3681,9 @@
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" s="71"/>
-      <c r="B97" s="74"/>
-      <c r="C97" s="74"/>
+      <c r="A97" s="78"/>
+      <c r="B97" s="86"/>
+      <c r="C97" s="86"/>
       <c r="D97" s="10" t="s">
         <v>33</v>
       </c>
@@ -3696,6 +3696,83 @@
     </row>
   </sheetData>
   <mergeCells count="84">
+    <mergeCell ref="A90:A97"/>
+    <mergeCell ref="B90:B93"/>
+    <mergeCell ref="C90:C91"/>
+    <mergeCell ref="C92:C93"/>
+    <mergeCell ref="B94:B97"/>
+    <mergeCell ref="C94:C95"/>
+    <mergeCell ref="C96:C97"/>
+    <mergeCell ref="A82:A89"/>
+    <mergeCell ref="B82:B85"/>
+    <mergeCell ref="C82:C83"/>
+    <mergeCell ref="C84:C85"/>
+    <mergeCell ref="B86:B89"/>
+    <mergeCell ref="C86:C87"/>
+    <mergeCell ref="C88:C89"/>
+    <mergeCell ref="A74:A81"/>
+    <mergeCell ref="B74:B77"/>
+    <mergeCell ref="C74:C75"/>
+    <mergeCell ref="C76:C77"/>
+    <mergeCell ref="B78:B81"/>
+    <mergeCell ref="C78:C79"/>
+    <mergeCell ref="C80:C81"/>
+    <mergeCell ref="A66:A73"/>
+    <mergeCell ref="B66:B69"/>
+    <mergeCell ref="C66:C67"/>
+    <mergeCell ref="C68:C69"/>
+    <mergeCell ref="B70:B73"/>
+    <mergeCell ref="C70:C71"/>
+    <mergeCell ref="C72:C73"/>
+    <mergeCell ref="A58:A65"/>
+    <mergeCell ref="B58:B61"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="B62:B65"/>
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="C64:C65"/>
+    <mergeCell ref="A50:A57"/>
+    <mergeCell ref="B50:B53"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="B54:B57"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="A42:A49"/>
+    <mergeCell ref="B42:B45"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="B46:B49"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="A34:A41"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="A26:A33"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="A18:A25"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="A10:A17"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C16:C17"/>
     <mergeCell ref="A2:A9"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="B6:B9"/>
@@ -3703,83 +3780,6 @@
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="C6:C7"/>
-    <mergeCell ref="A10:A17"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="A18:A25"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="A26:A33"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="A34:A41"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="B38:B41"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="A42:A49"/>
-    <mergeCell ref="B42:B45"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="B46:B49"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="A50:A57"/>
-    <mergeCell ref="B50:B53"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="B54:B57"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="A58:A65"/>
-    <mergeCell ref="B58:B61"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="B62:B65"/>
-    <mergeCell ref="C62:C63"/>
-    <mergeCell ref="C64:C65"/>
-    <mergeCell ref="A66:A73"/>
-    <mergeCell ref="B66:B69"/>
-    <mergeCell ref="C66:C67"/>
-    <mergeCell ref="C68:C69"/>
-    <mergeCell ref="B70:B73"/>
-    <mergeCell ref="C70:C71"/>
-    <mergeCell ref="C72:C73"/>
-    <mergeCell ref="A74:A81"/>
-    <mergeCell ref="B74:B77"/>
-    <mergeCell ref="C74:C75"/>
-    <mergeCell ref="C76:C77"/>
-    <mergeCell ref="B78:B81"/>
-    <mergeCell ref="C78:C79"/>
-    <mergeCell ref="C80:C81"/>
-    <mergeCell ref="A82:A89"/>
-    <mergeCell ref="B82:B85"/>
-    <mergeCell ref="C82:C83"/>
-    <mergeCell ref="C84:C85"/>
-    <mergeCell ref="B86:B89"/>
-    <mergeCell ref="C86:C87"/>
-    <mergeCell ref="C88:C89"/>
-    <mergeCell ref="A90:A97"/>
-    <mergeCell ref="B90:B93"/>
-    <mergeCell ref="C90:C91"/>
-    <mergeCell ref="C92:C93"/>
-    <mergeCell ref="B94:B97"/>
-    <mergeCell ref="C94:C95"/>
-    <mergeCell ref="C96:C97"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3790,7 +3790,7 @@
   <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E25" sqref="E24:E25"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3828,10 +3828,10 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="85" t="s">
+      <c r="A2" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="86" t="s">
+      <c r="B2" s="92" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="51" t="s">
@@ -3840,17 +3840,17 @@
       <c r="D2" s="4">
         <v>-5873078.1357632903</v>
       </c>
-      <c r="E2" s="96">
+      <c r="E2" s="75">
         <f>D2-D3</f>
         <v>669.48723918944597</v>
       </c>
-      <c r="F2" s="96"/>
+      <c r="F2" s="75"/>
       <c r="G2" s="4"/>
-      <c r="H2" s="87"/>
+      <c r="H2" s="71"/>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="88"/>
-      <c r="B3" s="83"/>
+      <c r="A3" s="90"/>
+      <c r="B3" s="93"/>
       <c r="C3" s="42" t="s">
         <v>4</v>
       </c>
@@ -3863,11 +3863,11 @@
       </c>
       <c r="F3" s="54"/>
       <c r="G3" s="2"/>
-      <c r="H3" s="89"/>
+      <c r="H3" s="72"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="88"/>
-      <c r="B4" s="94" t="s">
+      <c r="A4" s="90"/>
+      <c r="B4" s="96" t="s">
         <v>20</v>
       </c>
       <c r="C4" s="44" t="s">
@@ -3880,100 +3880,110 @@
         <f>D4-D5</f>
         <v>680.52461569011211</v>
       </c>
-      <c r="F4" s="97">
+      <c r="F4" s="76">
         <v>100000000</v>
       </c>
       <c r="G4" s="2"/>
-      <c r="H4" s="89"/>
+      <c r="H4" s="72"/>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="90"/>
-      <c r="B5" s="95"/>
+      <c r="A5" s="91"/>
+      <c r="B5" s="97"/>
       <c r="C5" s="43" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="3">
         <v>-5873746.2655823203</v>
       </c>
-      <c r="E5" s="92">
+      <c r="E5" s="73">
         <f>D5-D4</f>
         <v>-680.52461569011211</v>
       </c>
-      <c r="F5" s="92"/>
+      <c r="F5" s="73"/>
       <c r="G5" s="3"/>
-      <c r="H5" s="93"/>
+      <c r="H5" s="74"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="85" t="s">
+      <c r="A6" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="86" t="s">
+      <c r="B6" s="92" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="96">
+      <c r="D6" s="4">
+        <v>-5862973.9845654499</v>
+      </c>
+      <c r="E6" s="75">
         <f>D6-D7</f>
-        <v>0</v>
-      </c>
-      <c r="F6" s="96"/>
+        <v>512.97913978993893</v>
+      </c>
+      <c r="F6" s="75"/>
       <c r="G6" s="4"/>
-      <c r="H6" s="87"/>
+      <c r="H6" s="71"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="88"/>
-      <c r="B7" s="83"/>
+      <c r="A7" s="90"/>
+      <c r="B7" s="93"/>
       <c r="C7" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="9"/>
+      <c r="D7" s="9">
+        <v>-5863486.9637052398</v>
+      </c>
       <c r="E7" s="54">
         <f>D7-D6</f>
-        <v>0</v>
+        <v>-512.97913978993893</v>
       </c>
       <c r="F7" s="54"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="89"/>
+      <c r="H7" s="72"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="88"/>
-      <c r="B8" s="84" t="s">
+      <c r="A8" s="90"/>
+      <c r="B8" s="96" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="45" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="82">
+      <c r="C8" s="70" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="11">
+        <v>-5862806.2538520899</v>
+      </c>
+      <c r="E8" s="56">
         <f>D8-D9</f>
-        <v>0</v>
-      </c>
-      <c r="F8" s="82"/>
+        <v>617.84994896035641</v>
+      </c>
+      <c r="F8" s="76">
+        <v>100000000</v>
+      </c>
       <c r="G8" s="2"/>
-      <c r="H8" s="89"/>
+      <c r="H8" s="72"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="90"/>
-      <c r="B9" s="91"/>
+      <c r="A9" s="91"/>
+      <c r="B9" s="97"/>
       <c r="C9" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="92">
+      <c r="D9" s="3">
+        <v>-5863424.1038010502</v>
+      </c>
+      <c r="E9" s="73">
         <f>D9-D8</f>
-        <v>0</v>
-      </c>
-      <c r="F9" s="92"/>
+        <v>-617.84994896035641</v>
+      </c>
+      <c r="F9" s="73"/>
       <c r="G9" s="3"/>
-      <c r="H9" s="93"/>
+      <c r="H9" s="74"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="85" t="s">
+      <c r="A10" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="86" t="s">
+      <c r="B10" s="92" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="51" t="s">
@@ -3983,11 +3993,11 @@
       <c r="E10" s="52"/>
       <c r="F10" s="52"/>
       <c r="G10" s="52"/>
-      <c r="H10" s="87"/>
+      <c r="H10" s="71"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="88"/>
-      <c r="B11" s="83"/>
+      <c r="A11" s="90"/>
+      <c r="B11" s="93"/>
       <c r="C11" s="42" t="s">
         <v>4</v>
       </c>
@@ -3995,11 +4005,11 @@
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
-      <c r="H11" s="89"/>
+      <c r="H11" s="72"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="88"/>
-      <c r="B12" s="84" t="s">
+      <c r="A12" s="90"/>
+      <c r="B12" s="94" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="45" t="s">
@@ -4009,11 +4019,11 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
-      <c r="H12" s="89"/>
+      <c r="H12" s="72"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="90"/>
-      <c r="B13" s="91"/>
+      <c r="A13" s="91"/>
+      <c r="B13" s="95"/>
       <c r="C13" s="43" t="s">
         <v>4</v>
       </c>
@@ -4021,13 +4031,13 @@
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
-      <c r="H13" s="93"/>
+      <c r="H13" s="74"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="85" t="s">
+      <c r="A14" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="86" t="s">
+      <c r="B14" s="92" t="s">
         <v>19</v>
       </c>
       <c r="C14" s="51" t="s">
@@ -4037,11 +4047,11 @@
       <c r="E14" s="52"/>
       <c r="F14" s="52"/>
       <c r="G14" s="52"/>
-      <c r="H14" s="87"/>
+      <c r="H14" s="71"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="88"/>
-      <c r="B15" s="83"/>
+      <c r="A15" s="90"/>
+      <c r="B15" s="93"/>
       <c r="C15" s="42" t="s">
         <v>4</v>
       </c>
@@ -4049,11 +4059,11 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
-      <c r="H15" s="89"/>
+      <c r="H15" s="72"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="88"/>
-      <c r="B16" s="84" t="s">
+      <c r="A16" s="90"/>
+      <c r="B16" s="94" t="s">
         <v>20</v>
       </c>
       <c r="C16" s="45" t="s">
@@ -4063,11 +4073,11 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
-      <c r="H16" s="89"/>
+      <c r="H16" s="72"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="90"/>
-      <c r="B17" s="91"/>
+      <c r="A17" s="91"/>
+      <c r="B17" s="95"/>
       <c r="C17" s="43" t="s">
         <v>4</v>
       </c>
@@ -4075,13 +4085,13 @@
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
-      <c r="H17" s="93"/>
+      <c r="H17" s="74"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="85" t="s">
+      <c r="A18" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="86" t="s">
+      <c r="B18" s="92" t="s">
         <v>19</v>
       </c>
       <c r="C18" s="51" t="s">
@@ -4091,11 +4101,11 @@
       <c r="E18" s="52"/>
       <c r="F18" s="52"/>
       <c r="G18" s="52"/>
-      <c r="H18" s="87"/>
+      <c r="H18" s="71"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="88"/>
-      <c r="B19" s="83"/>
+      <c r="A19" s="90"/>
+      <c r="B19" s="93"/>
       <c r="C19" s="42" t="s">
         <v>4</v>
       </c>
@@ -4103,11 +4113,11 @@
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="89"/>
+      <c r="H19" s="72"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="88"/>
-      <c r="B20" s="84" t="s">
+      <c r="A20" s="90"/>
+      <c r="B20" s="94" t="s">
         <v>20</v>
       </c>
       <c r="C20" s="45" t="s">
@@ -4117,11 +4127,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="89"/>
+      <c r="H20" s="72"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="90"/>
-      <c r="B21" s="91"/>
+      <c r="A21" s="91"/>
+      <c r="B21" s="95"/>
       <c r="C21" s="43" t="s">
         <v>4</v>
       </c>
@@ -4129,13 +4139,13 @@
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
-      <c r="H21" s="93"/>
+      <c r="H21" s="74"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="85" t="s">
+      <c r="A22" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="86" t="s">
+      <c r="B22" s="92" t="s">
         <v>19</v>
       </c>
       <c r="C22" s="51" t="s">
@@ -4145,11 +4155,11 @@
       <c r="E22" s="52"/>
       <c r="F22" s="52"/>
       <c r="G22" s="52"/>
-      <c r="H22" s="87"/>
+      <c r="H22" s="71"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="88"/>
-      <c r="B23" s="83"/>
+      <c r="A23" s="90"/>
+      <c r="B23" s="93"/>
       <c r="C23" s="42" t="s">
         <v>4</v>
       </c>
@@ -4157,11 +4167,11 @@
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
-      <c r="H23" s="89"/>
+      <c r="H23" s="72"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="88"/>
-      <c r="B24" s="84" t="s">
+      <c r="A24" s="90"/>
+      <c r="B24" s="94" t="s">
         <v>20</v>
       </c>
       <c r="C24" s="45" t="s">
@@ -4171,11 +4181,11 @@
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
-      <c r="H24" s="89"/>
+      <c r="H24" s="72"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="90"/>
-      <c r="B25" s="91"/>
+      <c r="A25" s="91"/>
+      <c r="B25" s="95"/>
       <c r="C25" s="43" t="s">
         <v>4</v>
       </c>
@@ -4183,13 +4193,13 @@
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
-      <c r="H25" s="93"/>
+      <c r="H25" s="74"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="85" t="s">
+      <c r="A26" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="B26" s="86" t="s">
+      <c r="B26" s="92" t="s">
         <v>19</v>
       </c>
       <c r="C26" s="51" t="s">
@@ -4199,11 +4209,11 @@
       <c r="E26" s="52"/>
       <c r="F26" s="52"/>
       <c r="G26" s="52"/>
-      <c r="H26" s="87"/>
+      <c r="H26" s="71"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="88"/>
-      <c r="B27" s="83"/>
+      <c r="A27" s="90"/>
+      <c r="B27" s="93"/>
       <c r="C27" s="42" t="s">
         <v>4</v>
       </c>
@@ -4211,11 +4221,11 @@
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
-      <c r="H27" s="89"/>
+      <c r="H27" s="72"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="88"/>
-      <c r="B28" s="84" t="s">
+      <c r="A28" s="90"/>
+      <c r="B28" s="94" t="s">
         <v>20</v>
       </c>
       <c r="C28" s="45" t="s">
@@ -4225,11 +4235,11 @@
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
-      <c r="H28" s="89"/>
+      <c r="H28" s="72"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="90"/>
-      <c r="B29" s="91"/>
+      <c r="A29" s="91"/>
+      <c r="B29" s="95"/>
       <c r="C29" s="43" t="s">
         <v>4</v>
       </c>
@@ -4237,13 +4247,13 @@
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
-      <c r="H29" s="93"/>
+      <c r="H29" s="74"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="85" t="s">
+      <c r="A30" s="89" t="s">
         <v>11</v>
       </c>
-      <c r="B30" s="86" t="s">
+      <c r="B30" s="92" t="s">
         <v>19</v>
       </c>
       <c r="C30" s="51" t="s">
@@ -4253,11 +4263,11 @@
       <c r="E30" s="52"/>
       <c r="F30" s="52"/>
       <c r="G30" s="52"/>
-      <c r="H30" s="87"/>
+      <c r="H30" s="71"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="88"/>
-      <c r="B31" s="83"/>
+      <c r="A31" s="90"/>
+      <c r="B31" s="93"/>
       <c r="C31" s="42" t="s">
         <v>4</v>
       </c>
@@ -4265,11 +4275,11 @@
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
-      <c r="H31" s="89"/>
+      <c r="H31" s="72"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="88"/>
-      <c r="B32" s="84" t="s">
+      <c r="A32" s="90"/>
+      <c r="B32" s="94" t="s">
         <v>20</v>
       </c>
       <c r="C32" s="45" t="s">
@@ -4279,11 +4289,11 @@
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
-      <c r="H32" s="89"/>
+      <c r="H32" s="72"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="90"/>
-      <c r="B33" s="91"/>
+      <c r="A33" s="91"/>
+      <c r="B33" s="95"/>
       <c r="C33" s="43" t="s">
         <v>4</v>
       </c>
@@ -4291,13 +4301,13 @@
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
       <c r="G33" s="7"/>
-      <c r="H33" s="93"/>
+      <c r="H33" s="74"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="85" t="s">
+      <c r="A34" s="89" t="s">
         <v>12</v>
       </c>
-      <c r="B34" s="86" t="s">
+      <c r="B34" s="92" t="s">
         <v>19</v>
       </c>
       <c r="C34" s="51" t="s">
@@ -4307,11 +4317,11 @@
       <c r="E34" s="52"/>
       <c r="F34" s="52"/>
       <c r="G34" s="52"/>
-      <c r="H34" s="87"/>
+      <c r="H34" s="71"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="88"/>
-      <c r="B35" s="83"/>
+      <c r="A35" s="90"/>
+      <c r="B35" s="93"/>
       <c r="C35" s="42" t="s">
         <v>4</v>
       </c>
@@ -4319,11 +4329,11 @@
       <c r="E35" s="6"/>
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
-      <c r="H35" s="89"/>
+      <c r="H35" s="72"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="88"/>
-      <c r="B36" s="84" t="s">
+      <c r="A36" s="90"/>
+      <c r="B36" s="94" t="s">
         <v>20</v>
       </c>
       <c r="C36" s="45" t="s">
@@ -4333,11 +4343,11 @@
       <c r="E36" s="6"/>
       <c r="F36" s="6"/>
       <c r="G36" s="6"/>
-      <c r="H36" s="89"/>
+      <c r="H36" s="72"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="90"/>
-      <c r="B37" s="91"/>
+      <c r="A37" s="91"/>
+      <c r="B37" s="95"/>
       <c r="C37" s="43" t="s">
         <v>4</v>
       </c>
@@ -4345,13 +4355,13 @@
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
       <c r="G37" s="7"/>
-      <c r="H37" s="93"/>
+      <c r="H37" s="74"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="85" t="s">
+      <c r="A38" s="89" t="s">
         <v>13</v>
       </c>
-      <c r="B38" s="86" t="s">
+      <c r="B38" s="92" t="s">
         <v>19</v>
       </c>
       <c r="C38" s="51" t="s">
@@ -4361,11 +4371,11 @@
       <c r="E38" s="52"/>
       <c r="F38" s="52"/>
       <c r="G38" s="52"/>
-      <c r="H38" s="87"/>
+      <c r="H38" s="71"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="88"/>
-      <c r="B39" s="83"/>
+      <c r="A39" s="90"/>
+      <c r="B39" s="93"/>
       <c r="C39" s="42" t="s">
         <v>4</v>
       </c>
@@ -4373,11 +4383,11 @@
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="89"/>
+      <c r="H39" s="72"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="88"/>
-      <c r="B40" s="84" t="s">
+      <c r="A40" s="90"/>
+      <c r="B40" s="94" t="s">
         <v>20</v>
       </c>
       <c r="C40" s="45" t="s">
@@ -4387,11 +4397,11 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="89"/>
+      <c r="H40" s="72"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="90"/>
-      <c r="B41" s="91"/>
+      <c r="A41" s="91"/>
+      <c r="B41" s="95"/>
       <c r="C41" s="43" t="s">
         <v>4</v>
       </c>
@@ -4399,13 +4409,13 @@
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
-      <c r="H41" s="93"/>
+      <c r="H41" s="74"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="85" t="s">
+      <c r="A42" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="B42" s="86" t="s">
+      <c r="B42" s="92" t="s">
         <v>19</v>
       </c>
       <c r="C42" s="51" t="s">
@@ -4415,11 +4425,11 @@
       <c r="E42" s="52"/>
       <c r="F42" s="52"/>
       <c r="G42" s="52"/>
-      <c r="H42" s="87"/>
+      <c r="H42" s="71"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="88"/>
-      <c r="B43" s="83"/>
+      <c r="A43" s="90"/>
+      <c r="B43" s="93"/>
       <c r="C43" s="42" t="s">
         <v>4</v>
       </c>
@@ -4427,11 +4437,11 @@
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="89"/>
+      <c r="H43" s="72"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="88"/>
-      <c r="B44" s="84" t="s">
+      <c r="A44" s="90"/>
+      <c r="B44" s="94" t="s">
         <v>20</v>
       </c>
       <c r="C44" s="45" t="s">
@@ -4441,11 +4451,11 @@
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="89"/>
+      <c r="H44" s="72"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="90"/>
-      <c r="B45" s="91"/>
+      <c r="A45" s="91"/>
+      <c r="B45" s="95"/>
       <c r="C45" s="43" t="s">
         <v>4</v>
       </c>
@@ -4453,13 +4463,13 @@
       <c r="E45" s="7"/>
       <c r="F45" s="7"/>
       <c r="G45" s="7"/>
-      <c r="H45" s="93"/>
+      <c r="H45" s="74"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="85" t="s">
+      <c r="A46" s="89" t="s">
         <v>15</v>
       </c>
-      <c r="B46" s="86" t="s">
+      <c r="B46" s="92" t="s">
         <v>19</v>
       </c>
       <c r="C46" s="51" t="s">
@@ -4469,11 +4479,11 @@
       <c r="E46" s="52"/>
       <c r="F46" s="52"/>
       <c r="G46" s="52"/>
-      <c r="H46" s="87"/>
+      <c r="H46" s="71"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="88"/>
-      <c r="B47" s="83"/>
+      <c r="A47" s="90"/>
+      <c r="B47" s="93"/>
       <c r="C47" s="42" t="s">
         <v>4</v>
       </c>
@@ -4481,11 +4491,11 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="89"/>
+      <c r="H47" s="72"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="88"/>
-      <c r="B48" s="84" t="s">
+      <c r="A48" s="90"/>
+      <c r="B48" s="94" t="s">
         <v>20</v>
       </c>
       <c r="C48" s="45" t="s">
@@ -4495,11 +4505,11 @@
       <c r="E48" s="6"/>
       <c r="F48" s="6"/>
       <c r="G48" s="6"/>
-      <c r="H48" s="89"/>
+      <c r="H48" s="72"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="90"/>
-      <c r="B49" s="91"/>
+      <c r="A49" s="91"/>
+      <c r="B49" s="95"/>
       <c r="C49" s="43" t="s">
         <v>4</v>
       </c>
@@ -4507,46 +4517,46 @@
       <c r="E49" s="7"/>
       <c r="F49" s="7"/>
       <c r="G49" s="7"/>
-      <c r="H49" s="93"/>
+      <c r="H49" s="74"/>
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="A46:A49"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B28:B29"/>
     <mergeCell ref="A38:A41"/>
     <mergeCell ref="B38:B39"/>
     <mergeCell ref="B40:B41"/>
     <mergeCell ref="A42:A45"/>
     <mergeCell ref="B42:B43"/>
     <mergeCell ref="B44:B45"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="A46:A49"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update main beast output
</commit_message>
<xml_diff>
--- a/main/beast/all/chromosome/clade/clades_data_summary.xlsx
+++ b/main/beast/all/chromosome/clade/clades_data_summary.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ktmea\Projects\plague-phylogeography-projects\main\beast\all\chromosome\clade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{380F8ECA-688D-49DA-A2D6-0CE113C7397C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63442D45-C96F-4ED7-A81F-3B6467F9EE4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="noHyperPrior" sheetId="3" r:id="rId1"/>
     <sheet name="original" sheetId="8" r:id="rId2"/>
     <sheet name="log" sheetId="9" r:id="rId3"/>
     <sheet name="summary" sheetId="6" r:id="rId4"/>
-    <sheet name="kat_summary" sheetId="7" r:id="rId5"/>
-    <sheet name="epop" sheetId="4" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="10" r:id="rId5"/>
+    <sheet name="kat_summary" sheetId="7" r:id="rId6"/>
+    <sheet name="epop" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="66">
   <si>
     <t>Clade</t>
   </si>
@@ -408,7 +409,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -615,6 +616,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFB6A7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -865,7 +878,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1080,42 +1093,58 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1143,7 +1172,11 @@
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1513,17 +1546,17 @@
       <selection activeCell="A2" sqref="A2:A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" customWidth="1"/>
-    <col min="5" max="5" width="21.5703125" customWidth="1"/>
-    <col min="6" max="6" width="34.7109375" customWidth="1"/>
-    <col min="7" max="7" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" customWidth="1"/>
+    <col min="2" max="2" width="11.26953125" customWidth="1"/>
+    <col min="3" max="3" width="10.81640625" customWidth="1"/>
+    <col min="5" max="5" width="21.54296875" customWidth="1"/>
+    <col min="6" max="6" width="34.7265625" customWidth="1"/>
+    <col min="7" max="7" width="18.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
@@ -1546,7 +1579,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
         <v>33</v>
       </c>
@@ -1569,7 +1602,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="16"/>
       <c r="B3" s="16" t="s">
         <v>20</v>
@@ -1590,7 +1623,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="6" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
         <v>2</v>
       </c>
@@ -1613,7 +1646,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" s="7" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="16"/>
       <c r="B5" s="16" t="s">
         <v>20</v>
@@ -1634,7 +1667,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" s="6" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="13" t="s">
         <v>5</v>
       </c>
@@ -1657,7 +1690,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="7" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="16"/>
       <c r="B7" s="16" t="s">
         <v>20</v>
@@ -1678,7 +1711,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" s="6" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="13" t="s">
         <v>6</v>
       </c>
@@ -1701,7 +1734,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" s="7" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="16"/>
       <c r="B9" s="16" t="s">
         <v>20</v>
@@ -1722,7 +1755,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" s="6" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="13" t="s">
         <v>7</v>
       </c>
@@ -1745,7 +1778,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" s="7" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="16"/>
       <c r="B11" s="16" t="s">
         <v>20</v>
@@ -1766,7 +1799,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" s="6" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="13" t="s">
         <v>8</v>
       </c>
@@ -1789,7 +1822,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" s="7" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="16"/>
       <c r="B13" s="16" t="s">
         <v>20</v>
@@ -1810,7 +1843,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" s="6" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="13" t="s">
         <v>9</v>
       </c>
@@ -1833,7 +1866,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" s="7" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="16"/>
       <c r="B15" s="16" t="s">
         <v>20</v>
@@ -1854,7 +1887,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" s="6" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="13" t="s">
         <v>10</v>
       </c>
@@ -1877,7 +1910,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" s="7" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="16"/>
       <c r="B17" s="16" t="s">
         <v>20</v>
@@ -1898,7 +1931,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" s="6" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="13" t="s">
         <v>11</v>
       </c>
@@ -1921,7 +1954,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" s="7" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" s="16"/>
       <c r="B19" s="16" t="s">
         <v>20</v>
@@ -1942,7 +1975,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" s="6" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="13" t="s">
         <v>12</v>
       </c>
@@ -1965,7 +1998,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" s="7" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A21" s="16"/>
       <c r="B21" s="16" t="s">
         <v>20</v>
@@ -1986,7 +2019,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" s="6" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="13" t="s">
         <v>13</v>
       </c>
@@ -2009,7 +2042,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" s="7" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" s="16"/>
       <c r="B23" s="16" t="s">
         <v>20</v>
@@ -2030,7 +2063,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" s="6" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A24" s="13" t="s">
         <v>14</v>
       </c>
@@ -2053,7 +2086,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" s="7" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" s="16"/>
       <c r="B25" s="16" t="s">
         <v>20</v>
@@ -2074,7 +2107,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" s="6" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A26" s="13" t="s">
         <v>15</v>
       </c>
@@ -2097,7 +2130,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:7" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" s="7" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A27" s="16"/>
       <c r="B27" s="16" t="s">
         <v>20</v>
@@ -2129,12 +2162,18 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="9.7265625" customWidth="1"/>
+    <col min="4" max="4" width="18.81640625" customWidth="1"/>
+    <col min="5" max="5" width="15.90625" customWidth="1"/>
+    <col min="6" max="6" width="26.7265625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>45</v>
       </c>
@@ -2166,7 +2205,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -2198,7 +2237,7 @@
         <v>-593.88124430000005</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -2230,7 +2269,7 @@
         <v>-385.78389490000001</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -2262,7 +2301,7 @@
         <v>-254.77459999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -2278,7 +2317,7 @@
       <c r="E5">
         <v>-5892741.3773999996</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="104" t="s">
         <v>57</v>
       </c>
       <c r="G5" s="75">
@@ -2294,7 +2333,7 @@
         <v>-1201.954935</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -2326,7 +2365,7 @@
         <v>-247.68818719999999</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -2342,7 +2381,7 @@
       <c r="E7">
         <v>-5891354.5140000004</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="103" t="s">
         <v>57</v>
       </c>
       <c r="G7" s="75">
@@ -2358,7 +2397,7 @@
         <v>-183.623559</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -2390,7 +2429,7 @@
         <v>-149.0783825</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -2422,7 +2461,7 @@
         <v>-488.94726839999998</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -2438,7 +2477,7 @@
       <c r="E10">
         <v>-5892804.6540000001</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="103" t="s">
         <v>57</v>
       </c>
       <c r="G10" s="75">
@@ -2454,7 +2493,7 @@
         <v>-278.7095774</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -2486,7 +2525,7 @@
         <v>-319.89632169999999</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -2502,7 +2541,7 @@
       <c r="E12">
         <v>-5887505.8404999999</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="103" t="s">
         <v>57</v>
       </c>
       <c r="G12" s="75">
@@ -2518,7 +2557,7 @@
         <v>-129.10517160000001</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -2559,22 +2598,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{435DB2E7-3737-4CBA-AFFB-0753DD5DBB05}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="48.85546875" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" customWidth="1"/>
-    <col min="8" max="8" width="23.7109375" customWidth="1"/>
-    <col min="9" max="9" width="30.42578125" customWidth="1"/>
-    <col min="10" max="10" width="15.140625" customWidth="1"/>
+    <col min="1" max="1" width="48.81640625" customWidth="1"/>
+    <col min="2" max="2" width="16.453125" customWidth="1"/>
+    <col min="3" max="3" width="17.81640625" customWidth="1"/>
+    <col min="7" max="7" width="18.1796875" customWidth="1"/>
+    <col min="8" max="8" width="23.7265625" customWidth="1"/>
+    <col min="9" max="9" width="30.453125" customWidth="1"/>
+    <col min="10" max="10" width="15.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>58</v>
       </c>
@@ -2600,7 +2639,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
         <v>2</v>
       </c>
@@ -2629,7 +2668,7 @@
         <v>1907</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
         <v>5</v>
       </c>
@@ -2658,7 +2697,7 @@
         <v>1932</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
         <v>6</v>
       </c>
@@ -2687,7 +2726,7 @@
         <v>1855</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="13" t="s">
         <v>7</v>
       </c>
@@ -2716,7 +2755,7 @@
         <v>1324</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="13" t="s">
         <v>8</v>
       </c>
@@ -2745,7 +2784,7 @@
         <v>1868</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="13" t="s">
         <v>9</v>
       </c>
@@ -2774,7 +2813,7 @@
         <v>1879</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="13" t="s">
         <v>10</v>
       </c>
@@ -2803,7 +2842,7 @@
         <v>1975</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="13" t="s">
         <v>11</v>
       </c>
@@ -2832,7 +2871,7 @@
         <v>1960</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="13" t="s">
         <v>12</v>
       </c>
@@ -2861,7 +2900,7 @@
         <v>1491</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="13" t="s">
         <v>13</v>
       </c>
@@ -2890,7 +2929,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="13" t="s">
         <v>14</v>
       </c>
@@ -2919,7 +2958,7 @@
         <v>1906</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="13" t="s">
         <v>15</v>
       </c>
@@ -2948,7 +2987,7 @@
         <v>-2777</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="13" t="s">
         <v>33</v>
       </c>
@@ -2977,8 +3016,8 @@
         <v>-3287</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J16" s="97"/>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J16" s="81"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2990,19 +3029,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N97"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D48" sqref="A42:XFD48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="25.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.7265625" customWidth="1"/>
+    <col min="5" max="5" width="25.26953125" customWidth="1"/>
     <col min="6" max="6" width="17" style="1" customWidth="1"/>
     <col min="7" max="7" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -3028,14 +3067,14 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="76" t="s">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="86" t="s">
+      <c r="B2" s="84" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="86" t="s">
+      <c r="C2" s="84" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -3050,10 +3089,10 @@
       </c>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="76"/>
-      <c r="B3" s="86"/>
-      <c r="C3" s="86"/>
+    <row r="3" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="82"/>
+      <c r="B3" s="84"/>
+      <c r="C3" s="84"/>
       <c r="D3" s="2" t="s">
         <v>30</v>
       </c>
@@ -3065,10 +3104,10 @@
       </c>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="76"/>
-      <c r="B4" s="86"/>
-      <c r="C4" s="86" t="s">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="82"/>
+      <c r="B4" s="84"/>
+      <c r="C4" s="84" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -3083,10 +3122,10 @@
       </c>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="76"/>
-      <c r="B5" s="86"/>
-      <c r="C5" s="86"/>
+    <row r="5" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="82"/>
+      <c r="B5" s="84"/>
+      <c r="C5" s="84"/>
       <c r="D5" s="2" t="s">
         <v>30</v>
       </c>
@@ -3098,12 +3137,12 @@
       </c>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="76"/>
-      <c r="B6" s="81" t="s">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="82"/>
+      <c r="B6" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="81" t="s">
+      <c r="C6" s="85" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="11" t="s">
@@ -3118,10 +3157,10 @@
       </c>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="76"/>
-      <c r="B7" s="81"/>
-      <c r="C7" s="81"/>
+    <row r="7" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="82"/>
+      <c r="B7" s="85"/>
+      <c r="C7" s="85"/>
       <c r="D7" s="2" t="s">
         <v>30</v>
       </c>
@@ -3133,10 +3172,10 @@
       </c>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="76"/>
-      <c r="B8" s="81"/>
-      <c r="C8" s="86" t="s">
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="82"/>
+      <c r="B8" s="85"/>
+      <c r="C8" s="84" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -3151,9 +3190,9 @@
       </c>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="77"/>
-      <c r="B9" s="82"/>
+    <row r="9" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="83"/>
+      <c r="B9" s="86"/>
       <c r="C9" s="87"/>
       <c r="D9" s="3" t="s">
         <v>30</v>
@@ -3166,14 +3205,14 @@
       </c>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="84" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="85" t="s">
+      <c r="B10" s="89" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="85" t="s">
+      <c r="C10" s="89" t="s">
         <v>3</v>
       </c>
       <c r="D10" s="4" t="s">
@@ -3188,10 +3227,10 @@
       </c>
       <c r="G10" s="50"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="76"/>
-      <c r="B11" s="86"/>
-      <c r="C11" s="86"/>
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="82"/>
+      <c r="B11" s="84"/>
+      <c r="C11" s="84"/>
       <c r="D11" s="2" t="s">
         <v>30</v>
       </c>
@@ -3203,10 +3242,10 @@
       </c>
       <c r="G11" s="6"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="76"/>
-      <c r="B12" s="86"/>
-      <c r="C12" s="86" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="82"/>
+      <c r="B12" s="84"/>
+      <c r="C12" s="84" t="s">
         <v>4</v>
       </c>
       <c r="D12" s="2" t="s">
@@ -3221,10 +3260,10 @@
       </c>
       <c r="G12" s="6"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="76"/>
-      <c r="B13" s="86"/>
-      <c r="C13" s="86"/>
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="82"/>
+      <c r="B13" s="84"/>
+      <c r="C13" s="84"/>
       <c r="D13" s="2" t="s">
         <v>30</v>
       </c>
@@ -3236,12 +3275,12 @@
       </c>
       <c r="G13" s="6"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="76"/>
-      <c r="B14" s="79" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="82"/>
+      <c r="B14" s="90" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="86" t="s">
+      <c r="C14" s="84" t="s">
         <v>3</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -3256,10 +3295,10 @@
       </c>
       <c r="G14" s="6"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="76"/>
-      <c r="B15" s="79"/>
-      <c r="C15" s="86"/>
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="82"/>
+      <c r="B15" s="90"/>
+      <c r="C15" s="84"/>
       <c r="D15" s="2" t="s">
         <v>30</v>
       </c>
@@ -3271,10 +3310,10 @@
       </c>
       <c r="G15" s="6"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="76"/>
-      <c r="B16" s="79"/>
-      <c r="C16" s="79" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="82"/>
+      <c r="B16" s="90"/>
+      <c r="C16" s="90" t="s">
         <v>4</v>
       </c>
       <c r="D16" s="8" t="s">
@@ -3289,10 +3328,10 @@
       </c>
       <c r="G16" s="6"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="77"/>
-      <c r="B17" s="80"/>
-      <c r="C17" s="80"/>
+    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="83"/>
+      <c r="B17" s="91"/>
+      <c r="C17" s="91"/>
       <c r="D17" s="3" t="s">
         <v>30</v>
       </c>
@@ -3304,14 +3343,14 @@
       </c>
       <c r="G17" s="7"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="76" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" s="82" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="78" t="s">
+      <c r="B18" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="78" t="s">
+      <c r="C18" s="92" t="s">
         <v>3</v>
       </c>
       <c r="D18" s="9" t="s">
@@ -3325,10 +3364,10 @@
         <v>9.2806000001728535</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="76"/>
-      <c r="B19" s="78"/>
-      <c r="C19" s="78"/>
+    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="82"/>
+      <c r="B19" s="92"/>
+      <c r="C19" s="92"/>
       <c r="D19" s="9" t="s">
         <v>30</v>
       </c>
@@ -3339,10 +3378,10 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="76"/>
-      <c r="B20" s="78"/>
-      <c r="C20" s="78" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" s="82"/>
+      <c r="B20" s="92"/>
+      <c r="C20" s="92" t="s">
         <v>4</v>
       </c>
       <c r="D20" s="9" t="s">
@@ -3356,10 +3395,10 @@
         <v>-9.2806000001728535</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="76"/>
-      <c r="B21" s="78"/>
-      <c r="C21" s="78"/>
+    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="82"/>
+      <c r="B21" s="92"/>
+      <c r="C21" s="92"/>
       <c r="D21" s="9" t="s">
         <v>30</v>
       </c>
@@ -3370,12 +3409,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="76"/>
-      <c r="B22" s="81" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" s="82"/>
+      <c r="B22" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="81" t="s">
+      <c r="C22" s="85" t="s">
         <v>3</v>
       </c>
       <c r="D22" s="11" t="s">
@@ -3389,10 +3428,10 @@
         <v>12.690900000743568</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="76"/>
-      <c r="B23" s="81"/>
-      <c r="C23" s="81"/>
+    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="82"/>
+      <c r="B23" s="85"/>
+      <c r="C23" s="85"/>
       <c r="D23" s="9" t="s">
         <v>30</v>
       </c>
@@ -3403,10 +3442,10 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="76"/>
-      <c r="B24" s="81"/>
-      <c r="C24" s="78" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24" s="82"/>
+      <c r="B24" s="85"/>
+      <c r="C24" s="92" t="s">
         <v>4</v>
       </c>
       <c r="D24" s="9" t="s">
@@ -3420,10 +3459,10 @@
         <v>-12.690900000743568</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="77"/>
-      <c r="B25" s="82"/>
-      <c r="C25" s="83"/>
+    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="83"/>
+      <c r="B25" s="86"/>
+      <c r="C25" s="93"/>
       <c r="D25" s="10" t="s">
         <v>30</v>
       </c>
@@ -3434,14 +3473,14 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="76" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26" s="82" t="s">
         <v>7</v>
       </c>
-      <c r="B26" s="78" t="s">
+      <c r="B26" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="78" t="s">
+      <c r="C26" s="92" t="s">
         <v>3</v>
       </c>
       <c r="D26" s="9" t="s">
@@ -3455,10 +3494,10 @@
         <v>10.098799999803305</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="76"/>
-      <c r="B27" s="78"/>
-      <c r="C27" s="78"/>
+    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="82"/>
+      <c r="B27" s="92"/>
+      <c r="C27" s="92"/>
       <c r="D27" s="9" t="s">
         <v>30</v>
       </c>
@@ -3469,10 +3508,10 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="76"/>
-      <c r="B28" s="78"/>
-      <c r="C28" s="78" t="s">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28" s="82"/>
+      <c r="B28" s="92"/>
+      <c r="C28" s="92" t="s">
         <v>4</v>
       </c>
       <c r="D28" s="9" t="s">
@@ -3486,10 +3525,10 @@
         <v>-10.098799999803305</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="76"/>
-      <c r="B29" s="78"/>
-      <c r="C29" s="78"/>
+    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="82"/>
+      <c r="B29" s="92"/>
+      <c r="C29" s="92"/>
       <c r="D29" s="9" t="s">
         <v>30</v>
       </c>
@@ -3500,12 +3539,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="76"/>
-      <c r="B30" s="81" t="s">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30" s="82"/>
+      <c r="B30" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="C30" s="81" t="s">
+      <c r="C30" s="85" t="s">
         <v>3</v>
       </c>
       <c r="D30" s="11" t="s">
@@ -3519,10 +3558,10 @@
         <v>44.081500000320375</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="76"/>
-      <c r="B31" s="81"/>
-      <c r="C31" s="81"/>
+    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="82"/>
+      <c r="B31" s="85"/>
+      <c r="C31" s="85"/>
       <c r="D31" s="9" t="s">
         <v>30</v>
       </c>
@@ -3533,10 +3572,10 @@
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="76"/>
-      <c r="B32" s="81"/>
-      <c r="C32" s="78" t="s">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A32" s="82"/>
+      <c r="B32" s="85"/>
+      <c r="C32" s="92" t="s">
         <v>4</v>
       </c>
       <c r="D32" s="9" t="s">
@@ -3550,10 +3589,10 @@
         <v>-44.081500000320375</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="77"/>
-      <c r="B33" s="82"/>
-      <c r="C33" s="83"/>
+    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="83"/>
+      <c r="B33" s="86"/>
+      <c r="C33" s="93"/>
       <c r="D33" s="10" t="s">
         <v>30</v>
       </c>
@@ -3564,14 +3603,14 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="76" t="s">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" s="82" t="s">
         <v>8</v>
       </c>
-      <c r="B34" s="78" t="s">
+      <c r="B34" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="C34" s="78" t="s">
+      <c r="C34" s="92" t="s">
         <v>3</v>
       </c>
       <c r="D34" s="9" t="s">
@@ -3585,10 +3624,10 @@
         <v>104.57550000026822</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="76"/>
-      <c r="B35" s="78"/>
-      <c r="C35" s="78"/>
+    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="82"/>
+      <c r="B35" s="92"/>
+      <c r="C35" s="92"/>
       <c r="D35" s="9" t="s">
         <v>30</v>
       </c>
@@ -3599,10 +3638,10 @@
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="76"/>
-      <c r="B36" s="78"/>
-      <c r="C36" s="78" t="s">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36" s="82"/>
+      <c r="B36" s="92"/>
+      <c r="C36" s="92" t="s">
         <v>4</v>
       </c>
       <c r="D36" s="9" t="s">
@@ -3616,10 +3655,10 @@
         <v>-104.57550000026822</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="76"/>
-      <c r="B37" s="78"/>
-      <c r="C37" s="78"/>
+    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="82"/>
+      <c r="B37" s="92"/>
+      <c r="C37" s="92"/>
       <c r="D37" s="9" t="s">
         <v>30</v>
       </c>
@@ -3630,12 +3669,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="76"/>
-      <c r="B38" s="81" t="s">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38" s="82"/>
+      <c r="B38" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="C38" s="81" t="s">
+      <c r="C38" s="85" t="s">
         <v>3</v>
       </c>
       <c r="D38" s="11" t="s">
@@ -3649,10 +3688,10 @@
         <v>3.9017000002786517</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="76"/>
-      <c r="B39" s="81"/>
-      <c r="C39" s="81"/>
+    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="82"/>
+      <c r="B39" s="85"/>
+      <c r="C39" s="85"/>
       <c r="D39" s="9" t="s">
         <v>30</v>
       </c>
@@ -3663,10 +3702,10 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="76"/>
-      <c r="B40" s="81"/>
-      <c r="C40" s="78" t="s">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40" s="82"/>
+      <c r="B40" s="85"/>
+      <c r="C40" s="92" t="s">
         <v>4</v>
       </c>
       <c r="D40" s="9" t="s">
@@ -3680,10 +3719,10 @@
         <v>-3.9017000002786517</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="77"/>
-      <c r="B41" s="82"/>
-      <c r="C41" s="83"/>
+    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="83"/>
+      <c r="B41" s="86"/>
+      <c r="C41" s="93"/>
       <c r="D41" s="10" t="s">
         <v>30</v>
       </c>
@@ -3694,14 +3733,14 @@
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="76" t="s">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A42" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="B42" s="78" t="s">
+      <c r="B42" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="C42" s="78" t="s">
+      <c r="C42" s="92" t="s">
         <v>3</v>
       </c>
       <c r="D42" s="9" t="s">
@@ -3715,10 +3754,10 @@
         <v>-18.697699999436736</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="76"/>
-      <c r="B43" s="78"/>
-      <c r="C43" s="78"/>
+    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="82"/>
+      <c r="B43" s="92"/>
+      <c r="C43" s="92"/>
       <c r="D43" s="9" t="s">
         <v>30</v>
       </c>
@@ -3727,10 +3766,10 @@
       </c>
       <c r="F43" s="58"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="76"/>
-      <c r="B44" s="78"/>
-      <c r="C44" s="78" t="s">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A44" s="82"/>
+      <c r="B44" s="92"/>
+      <c r="C44" s="92" t="s">
         <v>4</v>
       </c>
       <c r="D44" s="9" t="s">
@@ -3744,10 +3783,10 @@
         <v>18.697699999436736</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="76"/>
-      <c r="B45" s="78"/>
-      <c r="C45" s="78"/>
+    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="82"/>
+      <c r="B45" s="92"/>
+      <c r="C45" s="92"/>
       <c r="D45" s="9" t="s">
         <v>30</v>
       </c>
@@ -3756,12 +3795,12 @@
       </c>
       <c r="F45" s="58"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="76"/>
-      <c r="B46" s="79" t="s">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A46" s="82"/>
+      <c r="B46" s="90" t="s">
         <v>20</v>
       </c>
-      <c r="C46" s="78" t="s">
+      <c r="C46" s="92" t="s">
         <v>3</v>
       </c>
       <c r="D46" s="9" t="s">
@@ -3775,10 +3814,10 @@
         <v>-13.384899999946356</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="76"/>
-      <c r="B47" s="79"/>
-      <c r="C47" s="78"/>
+    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="82"/>
+      <c r="B47" s="90"/>
+      <c r="C47" s="92"/>
       <c r="D47" s="9" t="s">
         <v>30</v>
       </c>
@@ -3787,10 +3826,10 @@
       </c>
       <c r="F47" s="58"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="76"/>
-      <c r="B48" s="79"/>
-      <c r="C48" s="79" t="s">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A48" s="82"/>
+      <c r="B48" s="90"/>
+      <c r="C48" s="90" t="s">
         <v>4</v>
       </c>
       <c r="D48" s="8" t="s">
@@ -3804,10 +3843,10 @@
         <v>13.384899999946356</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="77"/>
-      <c r="B49" s="80"/>
-      <c r="C49" s="80"/>
+    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="83"/>
+      <c r="B49" s="91"/>
+      <c r="C49" s="91"/>
       <c r="D49" s="10" t="s">
         <v>30</v>
       </c>
@@ -3818,14 +3857,14 @@
         <v>37</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="76" t="s">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A50" s="82" t="s">
         <v>10</v>
       </c>
-      <c r="B50" s="78" t="s">
+      <c r="B50" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="C50" s="78" t="s">
+      <c r="C50" s="92" t="s">
         <v>3</v>
       </c>
       <c r="D50" s="9" t="s">
@@ -3839,10 +3878,10 @@
         <v>-2.6929999999701977</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="76"/>
-      <c r="B51" s="78"/>
-      <c r="C51" s="78"/>
+    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="82"/>
+      <c r="B51" s="92"/>
+      <c r="C51" s="92"/>
       <c r="D51" s="9" t="s">
         <v>30</v>
       </c>
@@ -3853,10 +3892,10 @@
         <v>37</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="76"/>
-      <c r="B52" s="78"/>
-      <c r="C52" s="78" t="s">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A52" s="82"/>
+      <c r="B52" s="92"/>
+      <c r="C52" s="92" t="s">
         <v>4</v>
       </c>
       <c r="D52" s="9" t="s">
@@ -3870,10 +3909,10 @@
         <v>2.6929999999701977</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="76"/>
-      <c r="B53" s="78"/>
-      <c r="C53" s="78"/>
+    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="82"/>
+      <c r="B53" s="92"/>
+      <c r="C53" s="92"/>
       <c r="D53" s="9" t="s">
         <v>30</v>
       </c>
@@ -3884,12 +3923,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="76"/>
-      <c r="B54" s="81" t="s">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A54" s="82"/>
+      <c r="B54" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="C54" s="81" t="s">
+      <c r="C54" s="85" t="s">
         <v>3</v>
       </c>
       <c r="D54" s="11" t="s">
@@ -3903,10 +3942,10 @@
         <v>3.6091000000014901</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="76"/>
-      <c r="B55" s="81"/>
-      <c r="C55" s="81"/>
+    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="82"/>
+      <c r="B55" s="85"/>
+      <c r="C55" s="85"/>
       <c r="D55" s="9" t="s">
         <v>30</v>
       </c>
@@ -3917,10 +3956,10 @@
         <v>37</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="76"/>
-      <c r="B56" s="81"/>
-      <c r="C56" s="78" t="s">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A56" s="82"/>
+      <c r="B56" s="85"/>
+      <c r="C56" s="92" t="s">
         <v>4</v>
       </c>
       <c r="D56" s="9" t="s">
@@ -3934,10 +3973,10 @@
         <v>-3.6091000000014901</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="77"/>
-      <c r="B57" s="82"/>
-      <c r="C57" s="83"/>
+    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="83"/>
+      <c r="B57" s="86"/>
+      <c r="C57" s="93"/>
       <c r="D57" s="10" t="s">
         <v>30</v>
       </c>
@@ -3948,14 +3987,14 @@
         <v>37</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="76" t="s">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A58" s="82" t="s">
         <v>11</v>
       </c>
-      <c r="B58" s="78" t="s">
+      <c r="B58" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="C58" s="78" t="s">
+      <c r="C58" s="92" t="s">
         <v>3</v>
       </c>
       <c r="D58" s="9" t="s">
@@ -3969,10 +4008,10 @@
         <v>-9.4918999997898936</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="76"/>
-      <c r="B59" s="78"/>
-      <c r="C59" s="78"/>
+    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="82"/>
+      <c r="B59" s="92"/>
+      <c r="C59" s="92"/>
       <c r="D59" s="9" t="s">
         <v>30</v>
       </c>
@@ -3983,10 +4022,10 @@
         <v>37</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="76"/>
-      <c r="B60" s="78"/>
-      <c r="C60" s="78" t="s">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A60" s="82"/>
+      <c r="B60" s="92"/>
+      <c r="C60" s="92" t="s">
         <v>4</v>
       </c>
       <c r="D60" s="9" t="s">
@@ -4000,10 +4039,10 @@
         <v>9.4918999997898936</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="76"/>
-      <c r="B61" s="78"/>
-      <c r="C61" s="78"/>
+    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="82"/>
+      <c r="B61" s="92"/>
+      <c r="C61" s="92"/>
       <c r="D61" s="9" t="s">
         <v>30</v>
       </c>
@@ -4014,12 +4053,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="76"/>
-      <c r="B62" s="79" t="s">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A62" s="82"/>
+      <c r="B62" s="90" t="s">
         <v>20</v>
       </c>
-      <c r="C62" s="78" t="s">
+      <c r="C62" s="92" t="s">
         <v>3</v>
       </c>
       <c r="D62" s="9" t="s">
@@ -4033,10 +4072,10 @@
         <v>-11.17200000025332</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="76"/>
-      <c r="B63" s="79"/>
-      <c r="C63" s="78"/>
+    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="82"/>
+      <c r="B63" s="90"/>
+      <c r="C63" s="92"/>
       <c r="D63" s="9" t="s">
         <v>30</v>
       </c>
@@ -4047,10 +4086,10 @@
         <v>37</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="76"/>
-      <c r="B64" s="79"/>
-      <c r="C64" s="79" t="s">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A64" s="82"/>
+      <c r="B64" s="90"/>
+      <c r="C64" s="90" t="s">
         <v>4</v>
       </c>
       <c r="D64" s="8" t="s">
@@ -4064,10 +4103,10 @@
         <v>11.17200000025332</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="77"/>
-      <c r="B65" s="80"/>
-      <c r="C65" s="80"/>
+    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="83"/>
+      <c r="B65" s="91"/>
+      <c r="C65" s="91"/>
       <c r="D65" s="10" t="s">
         <v>30</v>
       </c>
@@ -4078,14 +4117,14 @@
         <v>37</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="76" t="s">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A66" s="82" t="s">
         <v>12</v>
       </c>
-      <c r="B66" s="78" t="s">
+      <c r="B66" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="C66" s="78" t="s">
+      <c r="C66" s="92" t="s">
         <v>3</v>
       </c>
       <c r="D66" s="9" t="s">
@@ -4099,10 +4138,10 @@
         <v>-2.3832000000402331</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="76"/>
-      <c r="B67" s="78"/>
-      <c r="C67" s="78"/>
+    <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="82"/>
+      <c r="B67" s="92"/>
+      <c r="C67" s="92"/>
       <c r="D67" s="9" t="s">
         <v>30</v>
       </c>
@@ -4113,10 +4152,10 @@
         <v>37</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="76"/>
-      <c r="B68" s="78"/>
-      <c r="C68" s="78" t="s">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A68" s="82"/>
+      <c r="B68" s="92"/>
+      <c r="C68" s="92" t="s">
         <v>4</v>
       </c>
       <c r="D68" s="9" t="s">
@@ -4125,15 +4164,15 @@
       <c r="E68" s="44">
         <v>-5896014.0886000004</v>
       </c>
-      <c r="F68" s="67">
+      <c r="F68" s="105">
         <f t="shared" si="9"/>
         <v>2.3832000000402331</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="76"/>
-      <c r="B69" s="78"/>
-      <c r="C69" s="78"/>
+    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="82"/>
+      <c r="B69" s="92"/>
+      <c r="C69" s="92"/>
       <c r="D69" s="9" t="s">
         <v>30</v>
       </c>
@@ -4144,12 +4183,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="76"/>
-      <c r="B70" s="81" t="s">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A70" s="82"/>
+      <c r="B70" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="C70" s="81" t="s">
+      <c r="C70" s="85" t="s">
         <v>3</v>
       </c>
       <c r="D70" s="11" t="s">
@@ -4163,10 +4202,10 @@
         <v>13297.716300000437</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="76"/>
-      <c r="B71" s="81"/>
-      <c r="C71" s="81"/>
+    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="82"/>
+      <c r="B71" s="85"/>
+      <c r="C71" s="85"/>
       <c r="D71" s="9" t="s">
         <v>30</v>
       </c>
@@ -4177,10 +4216,10 @@
         <v>37</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="76"/>
-      <c r="B72" s="81"/>
-      <c r="C72" s="78" t="s">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A72" s="82"/>
+      <c r="B72" s="85"/>
+      <c r="C72" s="92" t="s">
         <v>4</v>
       </c>
       <c r="D72" s="9" t="s">
@@ -4194,10 +4233,10 @@
         <v>-13297.716300000437</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="77"/>
-      <c r="B73" s="82"/>
-      <c r="C73" s="83"/>
+    <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="83"/>
+      <c r="B73" s="86"/>
+      <c r="C73" s="93"/>
       <c r="D73" s="10" t="s">
         <v>30</v>
       </c>
@@ -4208,14 +4247,14 @@
         <v>37</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="76" t="s">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A74" s="82" t="s">
         <v>13</v>
       </c>
-      <c r="B74" s="78" t="s">
+      <c r="B74" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="C74" s="78" t="s">
+      <c r="C74" s="92" t="s">
         <v>3</v>
       </c>
       <c r="D74" s="9" t="s">
@@ -4229,10 +4268,10 @@
         <v>5.2581000002101064</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="76"/>
-      <c r="B75" s="78"/>
-      <c r="C75" s="78"/>
+    <row r="75" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A75" s="82"/>
+      <c r="B75" s="92"/>
+      <c r="C75" s="92"/>
       <c r="D75" s="9" t="s">
         <v>30</v>
       </c>
@@ -4243,10 +4282,10 @@
         <v>37</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="76"/>
-      <c r="B76" s="78"/>
-      <c r="C76" s="78" t="s">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A76" s="82"/>
+      <c r="B76" s="92"/>
+      <c r="C76" s="92" t="s">
         <v>4</v>
       </c>
       <c r="D76" s="9" t="s">
@@ -4260,10 +4299,10 @@
         <v>-5.2581000002101064</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="76"/>
-      <c r="B77" s="78"/>
-      <c r="C77" s="78"/>
+    <row r="77" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A77" s="82"/>
+      <c r="B77" s="92"/>
+      <c r="C77" s="92"/>
       <c r="D77" s="9" t="s">
         <v>30</v>
       </c>
@@ -4274,12 +4313,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="76"/>
-      <c r="B78" s="81" t="s">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A78" s="82"/>
+      <c r="B78" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="C78" s="81" t="s">
+      <c r="C78" s="85" t="s">
         <v>3</v>
       </c>
       <c r="D78" s="11" t="s">
@@ -4293,10 +4332,10 @@
         <v>5.9207999994978309</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="76"/>
-      <c r="B79" s="81"/>
-      <c r="C79" s="81"/>
+    <row r="79" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A79" s="82"/>
+      <c r="B79" s="85"/>
+      <c r="C79" s="85"/>
       <c r="D79" s="9" t="s">
         <v>30</v>
       </c>
@@ -4307,10 +4346,10 @@
         <v>37</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="76"/>
-      <c r="B80" s="81"/>
-      <c r="C80" s="78" t="s">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A80" s="82"/>
+      <c r="B80" s="85"/>
+      <c r="C80" s="92" t="s">
         <v>4</v>
       </c>
       <c r="D80" s="9" t="s">
@@ -4324,10 +4363,10 @@
         <v>-5.9207999994978309</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A81" s="77"/>
-      <c r="B81" s="82"/>
-      <c r="C81" s="83"/>
+    <row r="81" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A81" s="83"/>
+      <c r="B81" s="86"/>
+      <c r="C81" s="93"/>
       <c r="D81" s="10" t="s">
         <v>30</v>
       </c>
@@ -4338,14 +4377,14 @@
         <v>37</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A82" s="76" t="s">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A82" s="82" t="s">
         <v>14</v>
       </c>
-      <c r="B82" s="78" t="s">
+      <c r="B82" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="C82" s="78" t="s">
+      <c r="C82" s="92" t="s">
         <v>3</v>
       </c>
       <c r="D82" s="9" t="s">
@@ -4359,10 +4398,10 @@
         <v>28.820300000719726</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A83" s="76"/>
-      <c r="B83" s="78"/>
-      <c r="C83" s="78"/>
+    <row r="83" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A83" s="82"/>
+      <c r="B83" s="92"/>
+      <c r="C83" s="92"/>
       <c r="D83" s="9" t="s">
         <v>30</v>
       </c>
@@ -4373,10 +4412,10 @@
         <v>37</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A84" s="76"/>
-      <c r="B84" s="78"/>
-      <c r="C84" s="78" t="s">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A84" s="82"/>
+      <c r="B84" s="92"/>
+      <c r="C84" s="92" t="s">
         <v>4</v>
       </c>
       <c r="D84" s="9" t="s">
@@ -4390,10 +4429,10 @@
         <v>-28.820300000719726</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A85" s="76"/>
-      <c r="B85" s="78"/>
-      <c r="C85" s="78"/>
+    <row r="85" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A85" s="82"/>
+      <c r="B85" s="92"/>
+      <c r="C85" s="92"/>
       <c r="D85" s="9" t="s">
         <v>30</v>
       </c>
@@ -4404,12 +4443,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A86" s="76"/>
-      <c r="B86" s="81" t="s">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A86" s="82"/>
+      <c r="B86" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="C86" s="81" t="s">
+      <c r="C86" s="85" t="s">
         <v>3</v>
       </c>
       <c r="D86" s="11" t="s">
@@ -4423,10 +4462,10 @@
         <v>12.378299999982119</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A87" s="76"/>
-      <c r="B87" s="81"/>
-      <c r="C87" s="81"/>
+    <row r="87" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A87" s="82"/>
+      <c r="B87" s="85"/>
+      <c r="C87" s="85"/>
       <c r="D87" s="9" t="s">
         <v>30</v>
       </c>
@@ -4437,10 +4476,10 @@
         <v>37</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A88" s="76"/>
-      <c r="B88" s="81"/>
-      <c r="C88" s="78" t="s">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A88" s="82"/>
+      <c r="B88" s="85"/>
+      <c r="C88" s="92" t="s">
         <v>4</v>
       </c>
       <c r="D88" s="9" t="s">
@@ -4454,10 +4493,10 @@
         <v>-12.378299999982119</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A89" s="77"/>
-      <c r="B89" s="82"/>
-      <c r="C89" s="83"/>
+    <row r="89" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A89" s="83"/>
+      <c r="B89" s="86"/>
+      <c r="C89" s="93"/>
       <c r="D89" s="10" t="s">
         <v>30</v>
       </c>
@@ -4468,14 +4507,14 @@
         <v>37</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A90" s="76" t="s">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A90" s="82" t="s">
         <v>15</v>
       </c>
-      <c r="B90" s="78" t="s">
+      <c r="B90" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="C90" s="78" t="s">
+      <c r="C90" s="92" t="s">
         <v>3</v>
       </c>
       <c r="D90" s="9" t="s">
@@ -4493,10 +4532,10 @@
       <c r="M90" s="75"/>
       <c r="N90" s="75"/>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A91" s="76"/>
-      <c r="B91" s="78"/>
-      <c r="C91" s="78"/>
+    <row r="91" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A91" s="82"/>
+      <c r="B91" s="92"/>
+      <c r="C91" s="92"/>
       <c r="D91" s="9" t="s">
         <v>30</v>
       </c>
@@ -4507,10 +4546,10 @@
         <v>37</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A92" s="76"/>
-      <c r="B92" s="78"/>
-      <c r="C92" s="78" t="s">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A92" s="82"/>
+      <c r="B92" s="92"/>
+      <c r="C92" s="92" t="s">
         <v>4</v>
       </c>
       <c r="D92" s="9" t="s">
@@ -4524,10 +4563,10 @@
         <v>-83.002000000327826</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A93" s="76"/>
-      <c r="B93" s="78"/>
-      <c r="C93" s="78"/>
+    <row r="93" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A93" s="82"/>
+      <c r="B93" s="92"/>
+      <c r="C93" s="92"/>
       <c r="D93" s="9" t="s">
         <v>30</v>
       </c>
@@ -4539,12 +4578,12 @@
       </c>
       <c r="G93" s="47"/>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A94" s="76"/>
-      <c r="B94" s="79" t="s">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A94" s="82"/>
+      <c r="B94" s="90" t="s">
         <v>20</v>
       </c>
-      <c r="C94" s="78" t="s">
+      <c r="C94" s="92" t="s">
         <v>3</v>
       </c>
       <c r="D94" s="9" t="s">
@@ -4558,10 +4597,10 @@
         <v>-2.8141000000759959</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A95" s="76"/>
-      <c r="B95" s="79"/>
-      <c r="C95" s="78"/>
+    <row r="95" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A95" s="82"/>
+      <c r="B95" s="90"/>
+      <c r="C95" s="92"/>
       <c r="D95" s="9" t="s">
         <v>30</v>
       </c>
@@ -4572,10 +4611,10 @@
         <v>37</v>
       </c>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A96" s="76"/>
-      <c r="B96" s="79"/>
-      <c r="C96" s="79" t="s">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A96" s="82"/>
+      <c r="B96" s="90"/>
+      <c r="C96" s="90" t="s">
         <v>4</v>
       </c>
       <c r="D96" s="8" t="s">
@@ -4589,10 +4628,10 @@
         <v>2.8141000000759959</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" s="77"/>
-      <c r="B97" s="80"/>
-      <c r="C97" s="80"/>
+    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A97" s="83"/>
+      <c r="B97" s="91"/>
+      <c r="C97" s="91"/>
       <c r="D97" s="10" t="s">
         <v>30</v>
       </c>
@@ -4605,6 +4644,83 @@
     </row>
   </sheetData>
   <mergeCells count="84">
+    <mergeCell ref="A90:A97"/>
+    <mergeCell ref="B90:B93"/>
+    <mergeCell ref="C90:C91"/>
+    <mergeCell ref="C92:C93"/>
+    <mergeCell ref="B94:B97"/>
+    <mergeCell ref="C94:C95"/>
+    <mergeCell ref="C96:C97"/>
+    <mergeCell ref="A82:A89"/>
+    <mergeCell ref="B82:B85"/>
+    <mergeCell ref="C82:C83"/>
+    <mergeCell ref="C84:C85"/>
+    <mergeCell ref="B86:B89"/>
+    <mergeCell ref="C86:C87"/>
+    <mergeCell ref="C88:C89"/>
+    <mergeCell ref="A74:A81"/>
+    <mergeCell ref="B74:B77"/>
+    <mergeCell ref="C74:C75"/>
+    <mergeCell ref="C76:C77"/>
+    <mergeCell ref="B78:B81"/>
+    <mergeCell ref="C78:C79"/>
+    <mergeCell ref="C80:C81"/>
+    <mergeCell ref="A66:A73"/>
+    <mergeCell ref="B66:B69"/>
+    <mergeCell ref="C66:C67"/>
+    <mergeCell ref="C68:C69"/>
+    <mergeCell ref="B70:B73"/>
+    <mergeCell ref="C70:C71"/>
+    <mergeCell ref="C72:C73"/>
+    <mergeCell ref="A58:A65"/>
+    <mergeCell ref="B58:B61"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="B62:B65"/>
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="C64:C65"/>
+    <mergeCell ref="A50:A57"/>
+    <mergeCell ref="B50:B53"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="B54:B57"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="A42:A49"/>
+    <mergeCell ref="B42:B45"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="B46:B49"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="A34:A41"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="A26:A33"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="A18:A25"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="A10:A17"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C16:C17"/>
     <mergeCell ref="A2:A9"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="B6:B9"/>
@@ -4612,89 +4728,978 @@
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="C6:C7"/>
-    <mergeCell ref="A10:A17"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="A18:A25"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="A26:A33"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="A34:A41"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="B38:B41"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="A42:A49"/>
-    <mergeCell ref="B42:B45"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="B46:B49"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="A50:A57"/>
-    <mergeCell ref="B50:B53"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="B54:B57"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="A58:A65"/>
-    <mergeCell ref="B58:B61"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="B62:B65"/>
-    <mergeCell ref="C62:C63"/>
-    <mergeCell ref="C64:C65"/>
-    <mergeCell ref="A66:A73"/>
-    <mergeCell ref="B66:B69"/>
-    <mergeCell ref="C66:C67"/>
-    <mergeCell ref="C68:C69"/>
-    <mergeCell ref="B70:B73"/>
-    <mergeCell ref="C70:C71"/>
-    <mergeCell ref="C72:C73"/>
-    <mergeCell ref="A74:A81"/>
-    <mergeCell ref="B74:B77"/>
-    <mergeCell ref="C74:C75"/>
-    <mergeCell ref="C76:C77"/>
-    <mergeCell ref="B78:B81"/>
-    <mergeCell ref="C78:C79"/>
-    <mergeCell ref="C80:C81"/>
-    <mergeCell ref="A82:A89"/>
-    <mergeCell ref="B82:B85"/>
-    <mergeCell ref="C82:C83"/>
-    <mergeCell ref="C84:C85"/>
-    <mergeCell ref="B86:B89"/>
-    <mergeCell ref="C86:C87"/>
-    <mergeCell ref="C88:C89"/>
-    <mergeCell ref="A90:A97"/>
-    <mergeCell ref="B90:B93"/>
-    <mergeCell ref="C90:C91"/>
-    <mergeCell ref="C92:C93"/>
-    <mergeCell ref="B94:B97"/>
-    <mergeCell ref="C94:C95"/>
-    <mergeCell ref="C96:C97"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{760C4128-2718-4EC9-A531-A4436A678D51}">
+  <dimension ref="A1:F49"/>
+  <sheetViews>
+    <sheetView topLeftCell="A39" workbookViewId="0">
+      <selection sqref="A1:F49"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="15.7265625" customWidth="1"/>
+    <col min="5" max="5" width="25.26953125" customWidth="1"/>
+    <col min="6" max="6" width="17" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="82" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="84" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="80" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="2">
+        <v>-5899661.4930999996</v>
+      </c>
+      <c r="F2" s="63">
+        <f>E2-E3</f>
+        <v>29.621400000527501</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="82"/>
+      <c r="B3" s="84"/>
+      <c r="C3" s="80" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="9">
+        <v>-5899691.1145000001</v>
+      </c>
+      <c r="F3" s="52">
+        <f>E3-E2</f>
+        <v>-29.621400000527501</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="82"/>
+      <c r="B4" s="85" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="78" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="11">
+        <v>-5899565.7433000002</v>
+      </c>
+      <c r="F4" s="54">
+        <f>E4-E5</f>
+        <v>35.669999999925494</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="82"/>
+      <c r="B5" s="85"/>
+      <c r="C5" s="80" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="2">
+        <v>-5899601.4133000001</v>
+      </c>
+      <c r="F5" s="52">
+        <f>E5-E4</f>
+        <v>-35.669999999925494</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="88" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="89" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="79" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="4">
+        <v>-5891402.6964999996</v>
+      </c>
+      <c r="F6" s="55">
+        <f>E6-E7</f>
+        <v>-3.5282999994233251</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="82"/>
+      <c r="B7" s="84"/>
+      <c r="C7" s="80" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="2">
+        <v>-5891399.1682000002</v>
+      </c>
+      <c r="F7" s="64">
+        <f>E7-E6</f>
+        <v>3.5282999994233251</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="82"/>
+      <c r="B8" s="90" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="80" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="2">
+        <v>-5891354.5140000004</v>
+      </c>
+      <c r="F8" s="52">
+        <f>E8-E9</f>
+        <v>-10.331400000490248</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="82"/>
+      <c r="B9" s="90"/>
+      <c r="C9" s="77" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="8">
+        <v>-5891344.1825999999</v>
+      </c>
+      <c r="F9" s="56">
+        <f>E9-E8</f>
+        <v>10.331400000490248</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="82" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="92" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="44">
+        <v>-5882586.8744000001</v>
+      </c>
+      <c r="F10" s="65">
+        <f>E10-E11</f>
+        <v>9.2806000001728535</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="82"/>
+      <c r="B11" s="92"/>
+      <c r="C11" s="76" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="44">
+        <v>-5882596.1550000003</v>
+      </c>
+      <c r="F11" s="58">
+        <f>E11-E10</f>
+        <v>-9.2806000001728535</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="82"/>
+      <c r="B12" s="85" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="78" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="5">
+        <v>-5882581.8636999996</v>
+      </c>
+      <c r="F12" s="59">
+        <f>E12-E13</f>
+        <v>12.690900000743568</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="82"/>
+      <c r="B13" s="85"/>
+      <c r="C13" s="76" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="44">
+        <v>-5882594.5546000004</v>
+      </c>
+      <c r="F13" s="58">
+        <f>E13-E12</f>
+        <v>-12.690900000743568</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="82" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="92" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="44">
+        <v>-5888129.8859000001</v>
+      </c>
+      <c r="F14" s="65">
+        <f>E14-E15</f>
+        <v>10.098799999803305</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="82"/>
+      <c r="B15" s="92"/>
+      <c r="C15" s="76" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="44">
+        <v>-5888139.9846999999</v>
+      </c>
+      <c r="F15" s="58">
+        <f>E15-E14</f>
+        <v>-10.098799999803305</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="82"/>
+      <c r="B16" s="85" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="78" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="5">
+        <v>-5888038.0526000001</v>
+      </c>
+      <c r="F16" s="59">
+        <f>E16-E17</f>
+        <v>44.081500000320375</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="82"/>
+      <c r="B17" s="85"/>
+      <c r="C17" s="76" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="44">
+        <v>-5888082.1341000004</v>
+      </c>
+      <c r="F17" s="58">
+        <f>E17-E16</f>
+        <v>-44.081500000320375</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="82" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="92" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18" s="44">
+        <v>-5920732.7741</v>
+      </c>
+      <c r="F18" s="65">
+        <f>E18-E19</f>
+        <v>104.57550000026822</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="82"/>
+      <c r="B19" s="92"/>
+      <c r="C19" s="76" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="44">
+        <v>-5920837.3496000003</v>
+      </c>
+      <c r="F19" s="58">
+        <f>E19-E18</f>
+        <v>-104.57550000026822</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="82"/>
+      <c r="B20" s="85" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="78" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="5">
+        <v>-5919658.1359000001</v>
+      </c>
+      <c r="F20" s="59">
+        <f>E20-E21</f>
+        <v>3.9017000002786517</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="82"/>
+      <c r="B21" s="85"/>
+      <c r="C21" s="76" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="44">
+        <v>-5919662.0376000004</v>
+      </c>
+      <c r="F21" s="58">
+        <f>E21-E20</f>
+        <v>-3.9017000002786517</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="92" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" s="44">
+        <v>-5892894.9243999999</v>
+      </c>
+      <c r="F22" s="58">
+        <f>E22-E23</f>
+        <v>-18.697699999436736</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="82"/>
+      <c r="B23" s="92"/>
+      <c r="C23" s="76" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" s="44">
+        <v>-5892876.2267000005</v>
+      </c>
+      <c r="F23" s="66">
+        <f>E23-E22</f>
+        <v>18.697699999436736</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="82"/>
+      <c r="B24" s="90" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24" s="44">
+        <v>-5892804.6540000001</v>
+      </c>
+      <c r="F24" s="58">
+        <f>E24-E25</f>
+        <v>-13.384899999946356</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="82"/>
+      <c r="B25" s="90"/>
+      <c r="C25" s="77" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E25" s="48">
+        <v>-5892791.2691000002</v>
+      </c>
+      <c r="F25" s="51">
+        <f>E25-E24</f>
+        <v>13.384899999946356</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" s="82" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="92" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E26" s="44">
+        <v>-5886034.1161000002</v>
+      </c>
+      <c r="F26" s="58">
+        <f>E26-E27</f>
+        <v>-2.6929999999701977</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" s="82"/>
+      <c r="B27" s="92"/>
+      <c r="C27" s="76" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E27" s="44">
+        <v>-5886031.4231000002</v>
+      </c>
+      <c r="F27" s="67">
+        <f>E27-E26</f>
+        <v>2.6929999999701977</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" s="82"/>
+      <c r="B28" s="85" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="78" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E28" s="5">
+        <v>-5886021.9687000001</v>
+      </c>
+      <c r="F28" s="59">
+        <f>E28-E29</f>
+        <v>3.6091000000014901</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" s="82"/>
+      <c r="B29" s="85"/>
+      <c r="C29" s="76" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E29" s="44">
+        <v>-5886025.5778000001</v>
+      </c>
+      <c r="F29" s="58">
+        <f>E29-E28</f>
+        <v>-3.6091000000014901</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" s="82" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" s="92" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E30" s="44">
+        <v>-5887506.0362999998</v>
+      </c>
+      <c r="F30" s="58">
+        <f>E30-E31</f>
+        <v>-9.4918999997898936</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" s="82"/>
+      <c r="B31" s="92"/>
+      <c r="C31" s="76" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E31" s="44">
+        <v>-5887496.5444</v>
+      </c>
+      <c r="F31" s="66">
+        <f>E31-E30</f>
+        <v>9.4918999997898936</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" s="82"/>
+      <c r="B32" s="90" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E32" s="44">
+        <v>-5887505.8404999999</v>
+      </c>
+      <c r="F32" s="58">
+        <f>E32-E33</f>
+        <v>-11.17200000025332</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" s="82"/>
+      <c r="B33" s="90"/>
+      <c r="C33" s="77" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E33" s="48">
+        <v>-5887494.6684999997</v>
+      </c>
+      <c r="F33" s="51">
+        <f>E33-E32</f>
+        <v>11.17200000025332</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" s="82" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" s="92" t="s">
+        <v>19</v>
+      </c>
+      <c r="C34" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E34" s="44">
+        <v>-5896016.4718000004</v>
+      </c>
+      <c r="F34" s="58">
+        <f>E34-E35</f>
+        <v>-2.3832000000402331</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35" s="82"/>
+      <c r="B35" s="92"/>
+      <c r="C35" s="76" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E35" s="44">
+        <v>-5896014.0886000004</v>
+      </c>
+      <c r="F35" s="67">
+        <f>E35-E34</f>
+        <v>2.3832000000402331</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36" s="82"/>
+      <c r="B36" s="85" t="s">
+        <v>20</v>
+      </c>
+      <c r="C36" s="78" t="s">
+        <v>3</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E36" s="5">
+        <v>-5882581.9853999997</v>
+      </c>
+      <c r="F36" s="59">
+        <f>E36-E37</f>
+        <v>13297.716300000437</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37" s="82"/>
+      <c r="B37" s="85"/>
+      <c r="C37" s="76" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E37" s="44">
+        <v>-5895879.7017000001</v>
+      </c>
+      <c r="F37" s="58">
+        <f>E37-E36</f>
+        <v>-13297.716300000437</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38" s="82" t="s">
+        <v>13</v>
+      </c>
+      <c r="B38" s="92" t="s">
+        <v>19</v>
+      </c>
+      <c r="C38" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E38" s="44">
+        <v>-5889520.4452999998</v>
+      </c>
+      <c r="F38" s="65">
+        <f>E38-E39</f>
+        <v>5.2581000002101064</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39" s="82"/>
+      <c r="B39" s="92"/>
+      <c r="C39" s="76" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E39" s="44">
+        <v>-5889525.7034</v>
+      </c>
+      <c r="F39" s="58">
+        <f>E39-E38</f>
+        <v>-5.2581000002101064</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40" s="82"/>
+      <c r="B40" s="85" t="s">
+        <v>20</v>
+      </c>
+      <c r="C40" s="78" t="s">
+        <v>3</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E40" s="5">
+        <v>-5889495.8046000004</v>
+      </c>
+      <c r="F40" s="59">
+        <f>E40-E41</f>
+        <v>5.9207999994978309</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41" s="82"/>
+      <c r="B41" s="85"/>
+      <c r="C41" s="76" t="s">
+        <v>4</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E41" s="44">
+        <v>-5889501.7253999999</v>
+      </c>
+      <c r="F41" s="58">
+        <f>E41-E40</f>
+        <v>-5.9207999994978309</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A42" s="82" t="s">
+        <v>14</v>
+      </c>
+      <c r="B42" s="92" t="s">
+        <v>19</v>
+      </c>
+      <c r="C42" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E42" s="44">
+        <v>-5945574.0226999996</v>
+      </c>
+      <c r="F42" s="65">
+        <f>E42-E43</f>
+        <v>28.820300000719726</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A43" s="82"/>
+      <c r="B43" s="92"/>
+      <c r="C43" s="76" t="s">
+        <v>4</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E43" s="44">
+        <v>-5945602.8430000003</v>
+      </c>
+      <c r="F43" s="58">
+        <f>E43-E42</f>
+        <v>-28.820300000719726</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A44" s="82"/>
+      <c r="B44" s="85" t="s">
+        <v>20</v>
+      </c>
+      <c r="C44" s="78" t="s">
+        <v>3</v>
+      </c>
+      <c r="D44" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E44" s="5">
+        <v>-5944614.3201000001</v>
+      </c>
+      <c r="F44" s="59">
+        <f>E44-E45</f>
+        <v>12.378299999982119</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A45" s="82"/>
+      <c r="B45" s="85"/>
+      <c r="C45" s="76" t="s">
+        <v>4</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E45" s="44">
+        <v>-5944626.6984000001</v>
+      </c>
+      <c r="F45" s="58">
+        <f>E45-E44</f>
+        <v>-12.378299999982119</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A46" s="82" t="s">
+        <v>15</v>
+      </c>
+      <c r="B46" s="92" t="s">
+        <v>19</v>
+      </c>
+      <c r="C46" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E46" s="44">
+        <v>-5892842.8987999996</v>
+      </c>
+      <c r="F46" s="67">
+        <f>E46-E47</f>
+        <v>83.002000000327826</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A47" s="82"/>
+      <c r="B47" s="92"/>
+      <c r="C47" s="76" t="s">
+        <v>4</v>
+      </c>
+      <c r="D47" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E47" s="44">
+        <v>-5892925.9007999999</v>
+      </c>
+      <c r="F47" s="58">
+        <f>E47-E46</f>
+        <v>-83.002000000327826</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A48" s="82"/>
+      <c r="B48" s="90" t="s">
+        <v>20</v>
+      </c>
+      <c r="C48" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="D48" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E48" s="44">
+        <v>-5892741.3773999996</v>
+      </c>
+      <c r="F48" s="58">
+        <f>E48-E49</f>
+        <v>-2.8141000000759959</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A49" s="82"/>
+      <c r="B49" s="90"/>
+      <c r="C49" s="77" t="s">
+        <v>4</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E49" s="48">
+        <v>-5892738.5632999996</v>
+      </c>
+      <c r="F49" s="51">
+        <f>E49-E48</f>
+        <v>2.8141000000759959</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="36">
+    <mergeCell ref="A46:A49"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8F55FE9-ECCC-4F21-9AD8-39C9EB206E22}">
   <dimension ref="A1:I49"/>
   <sheetViews>
@@ -4702,15 +5707,15 @@
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="27.42578125" customWidth="1"/>
-    <col min="5" max="6" width="27.85546875" customWidth="1"/>
+    <col min="4" max="4" width="27.453125" customWidth="1"/>
+    <col min="5" max="6" width="27.81640625" customWidth="1"/>
     <col min="7" max="7" width="21" customWidth="1"/>
-    <col min="8" max="8" width="27.42578125" customWidth="1"/>
+    <col min="8" max="8" width="27.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -4736,11 +5741,11 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="88" t="s">
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="94" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="91" t="s">
+      <c r="B2" s="97" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="49" t="s">
@@ -4756,9 +5761,9 @@
       <c r="F2" s="70"/>
       <c r="G2" s="4"/>
     </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="89"/>
-      <c r="B3" s="92"/>
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="95"/>
+      <c r="B3" s="98"/>
       <c r="C3" s="40" t="s">
         <v>4</v>
       </c>
@@ -4772,9 +5777,9 @@
       <c r="F3" s="52"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="89"/>
-      <c r="B4" s="95" t="s">
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="95"/>
+      <c r="B4" s="101" t="s">
         <v>20</v>
       </c>
       <c r="C4" s="42" t="s">
@@ -4800,9 +5805,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="90"/>
-      <c r="B5" s="96"/>
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="96"/>
+      <c r="B5" s="102"/>
       <c r="C5" s="41" t="s">
         <v>4</v>
       </c>
@@ -4816,11 +5821,11 @@
       <c r="F5" s="69"/>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="88" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="94" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="91" t="s">
+      <c r="B6" s="97" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="49" t="s">
@@ -4836,9 +5841,9 @@
       <c r="F6" s="70"/>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="89"/>
-      <c r="B7" s="92"/>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="95"/>
+      <c r="B7" s="98"/>
       <c r="C7" s="40" t="s">
         <v>4</v>
       </c>
@@ -4852,9 +5857,9 @@
       <c r="F7" s="52"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="89"/>
-      <c r="B8" s="95" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="95"/>
+      <c r="B8" s="101" t="s">
         <v>20</v>
       </c>
       <c r="C8" s="68" t="s">
@@ -4880,9 +5885,9 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="90"/>
-      <c r="B9" s="96"/>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="96"/>
+      <c r="B9" s="102"/>
       <c r="C9" s="41" t="s">
         <v>4</v>
       </c>
@@ -4896,11 +5901,11 @@
       <c r="F9" s="69"/>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="88" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="94" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="91" t="s">
+      <c r="B10" s="97" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="49" t="s">
@@ -4911,9 +5916,9 @@
       <c r="F10" s="50"/>
       <c r="G10" s="50"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="89"/>
-      <c r="B11" s="92"/>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="95"/>
+      <c r="B11" s="98"/>
       <c r="C11" s="40" t="s">
         <v>4</v>
       </c>
@@ -4922,9 +5927,9 @@
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="89"/>
-      <c r="B12" s="93" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="95"/>
+      <c r="B12" s="99" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="43" t="s">
@@ -4935,9 +5940,9 @@
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="90"/>
-      <c r="B13" s="94"/>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" s="96"/>
+      <c r="B13" s="100"/>
       <c r="C13" s="41" t="s">
         <v>4</v>
       </c>
@@ -4946,11 +5951,11 @@
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="88" t="s">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" s="94" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="91" t="s">
+      <c r="B14" s="97" t="s">
         <v>19</v>
       </c>
       <c r="C14" s="49" t="s">
@@ -4961,9 +5966,9 @@
       <c r="F14" s="50"/>
       <c r="G14" s="50"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="89"/>
-      <c r="B15" s="92"/>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" s="95"/>
+      <c r="B15" s="98"/>
       <c r="C15" s="40" t="s">
         <v>4</v>
       </c>
@@ -4972,9 +5977,9 @@
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="89"/>
-      <c r="B16" s="93" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" s="95"/>
+      <c r="B16" s="99" t="s">
         <v>20</v>
       </c>
       <c r="C16" s="43" t="s">
@@ -4985,9 +5990,9 @@
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="90"/>
-      <c r="B17" s="94"/>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" s="96"/>
+      <c r="B17" s="100"/>
       <c r="C17" s="41" t="s">
         <v>4</v>
       </c>
@@ -4996,11 +6001,11 @@
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="88" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" s="94" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="91" t="s">
+      <c r="B18" s="97" t="s">
         <v>19</v>
       </c>
       <c r="C18" s="49" t="s">
@@ -5011,9 +6016,9 @@
       <c r="F18" s="50"/>
       <c r="G18" s="50"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="89"/>
-      <c r="B19" s="92"/>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" s="95"/>
+      <c r="B19" s="98"/>
       <c r="C19" s="40" t="s">
         <v>4</v>
       </c>
@@ -5022,9 +6027,9 @@
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="89"/>
-      <c r="B20" s="93" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" s="95"/>
+      <c r="B20" s="99" t="s">
         <v>20</v>
       </c>
       <c r="C20" s="43" t="s">
@@ -5035,9 +6040,9 @@
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="90"/>
-      <c r="B21" s="94"/>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" s="96"/>
+      <c r="B21" s="100"/>
       <c r="C21" s="41" t="s">
         <v>4</v>
       </c>
@@ -5046,11 +6051,11 @@
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="88" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" s="94" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="91" t="s">
+      <c r="B22" s="97" t="s">
         <v>19</v>
       </c>
       <c r="C22" s="49" t="s">
@@ -5066,9 +6071,9 @@
       <c r="F22" s="50"/>
       <c r="G22" s="50"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="89"/>
-      <c r="B23" s="92"/>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23" s="95"/>
+      <c r="B23" s="98"/>
       <c r="C23" s="40" t="s">
         <v>4</v>
       </c>
@@ -5082,9 +6087,9 @@
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="89"/>
-      <c r="B24" s="95" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24" s="95"/>
+      <c r="B24" s="101" t="s">
         <v>20</v>
       </c>
       <c r="C24" s="72" t="s">
@@ -5102,9 +6107,9 @@
       </c>
       <c r="G24" s="6"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="90"/>
-      <c r="B25" s="96"/>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25" s="96"/>
+      <c r="B25" s="102"/>
       <c r="C25" s="41" t="s">
         <v>4</v>
       </c>
@@ -5118,11 +6123,11 @@
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="88" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26" s="94" t="s">
         <v>10</v>
       </c>
-      <c r="B26" s="91" t="s">
+      <c r="B26" s="97" t="s">
         <v>19</v>
       </c>
       <c r="C26" s="49" t="s">
@@ -5133,9 +6138,9 @@
       <c r="F26" s="50"/>
       <c r="G26" s="50"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="89"/>
-      <c r="B27" s="92"/>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" s="95"/>
+      <c r="B27" s="98"/>
       <c r="C27" s="40" t="s">
         <v>4</v>
       </c>
@@ -5144,9 +6149,9 @@
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="89"/>
-      <c r="B28" s="93" t="s">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28" s="95"/>
+      <c r="B28" s="99" t="s">
         <v>20</v>
       </c>
       <c r="C28" s="43" t="s">
@@ -5157,9 +6162,9 @@
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="90"/>
-      <c r="B29" s="94"/>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A29" s="96"/>
+      <c r="B29" s="100"/>
       <c r="C29" s="41" t="s">
         <v>4</v>
       </c>
@@ -5168,11 +6173,11 @@
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="88" t="s">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30" s="94" t="s">
         <v>11</v>
       </c>
-      <c r="B30" s="91" t="s">
+      <c r="B30" s="97" t="s">
         <v>19</v>
       </c>
       <c r="C30" s="49" t="s">
@@ -5183,9 +6188,9 @@
       <c r="F30" s="50"/>
       <c r="G30" s="50"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="89"/>
-      <c r="B31" s="92"/>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A31" s="95"/>
+      <c r="B31" s="98"/>
       <c r="C31" s="40" t="s">
         <v>4</v>
       </c>
@@ -5194,9 +6199,9 @@
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="89"/>
-      <c r="B32" s="93" t="s">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A32" s="95"/>
+      <c r="B32" s="99" t="s">
         <v>20</v>
       </c>
       <c r="C32" s="43" t="s">
@@ -5207,9 +6212,9 @@
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="90"/>
-      <c r="B33" s="94"/>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A33" s="96"/>
+      <c r="B33" s="100"/>
       <c r="C33" s="41" t="s">
         <v>4</v>
       </c>
@@ -5218,11 +6223,11 @@
       <c r="F33" s="7"/>
       <c r="G33" s="7"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="88" t="s">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A34" s="94" t="s">
         <v>12</v>
       </c>
-      <c r="B34" s="91" t="s">
+      <c r="B34" s="97" t="s">
         <v>19</v>
       </c>
       <c r="C34" s="49" t="s">
@@ -5233,9 +6238,9 @@
       <c r="F34" s="50"/>
       <c r="G34" s="50"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="89"/>
-      <c r="B35" s="92"/>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A35" s="95"/>
+      <c r="B35" s="98"/>
       <c r="C35" s="40" t="s">
         <v>4</v>
       </c>
@@ -5244,9 +6249,9 @@
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="89"/>
-      <c r="B36" s="93" t="s">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A36" s="95"/>
+      <c r="B36" s="99" t="s">
         <v>20</v>
       </c>
       <c r="C36" s="43" t="s">
@@ -5257,9 +6262,9 @@
       <c r="F36" s="6"/>
       <c r="G36" s="6"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="90"/>
-      <c r="B37" s="94"/>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A37" s="96"/>
+      <c r="B37" s="100"/>
       <c r="C37" s="41" t="s">
         <v>4</v>
       </c>
@@ -5268,11 +6273,11 @@
       <c r="F37" s="7"/>
       <c r="G37" s="7"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="88" t="s">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A38" s="94" t="s">
         <v>13</v>
       </c>
-      <c r="B38" s="91" t="s">
+      <c r="B38" s="97" t="s">
         <v>19</v>
       </c>
       <c r="C38" s="49" t="s">
@@ -5283,9 +6288,9 @@
       <c r="F38" s="50"/>
       <c r="G38" s="50"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="89"/>
-      <c r="B39" s="92"/>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A39" s="95"/>
+      <c r="B39" s="98"/>
       <c r="C39" s="40" t="s">
         <v>4</v>
       </c>
@@ -5294,9 +6299,9 @@
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="89"/>
-      <c r="B40" s="93" t="s">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A40" s="95"/>
+      <c r="B40" s="99" t="s">
         <v>20</v>
       </c>
       <c r="C40" s="43" t="s">
@@ -5307,9 +6312,9 @@
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="90"/>
-      <c r="B41" s="94"/>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A41" s="96"/>
+      <c r="B41" s="100"/>
       <c r="C41" s="41" t="s">
         <v>4</v>
       </c>
@@ -5318,11 +6323,11 @@
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="88" t="s">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A42" s="94" t="s">
         <v>14</v>
       </c>
-      <c r="B42" s="91" t="s">
+      <c r="B42" s="97" t="s">
         <v>19</v>
       </c>
       <c r="C42" s="49" t="s">
@@ -5333,9 +6338,9 @@
       <c r="F42" s="50"/>
       <c r="G42" s="50"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="89"/>
-      <c r="B43" s="92"/>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A43" s="95"/>
+      <c r="B43" s="98"/>
       <c r="C43" s="40" t="s">
         <v>4</v>
       </c>
@@ -5344,9 +6349,9 @@
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="89"/>
-      <c r="B44" s="93" t="s">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A44" s="95"/>
+      <c r="B44" s="99" t="s">
         <v>20</v>
       </c>
       <c r="C44" s="43" t="s">
@@ -5357,9 +6362,9 @@
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="90"/>
-      <c r="B45" s="94"/>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A45" s="96"/>
+      <c r="B45" s="100"/>
       <c r="C45" s="41" t="s">
         <v>4</v>
       </c>
@@ -5368,11 +6373,11 @@
       <c r="F45" s="7"/>
       <c r="G45" s="7"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="88" t="s">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A46" s="94" t="s">
         <v>15</v>
       </c>
-      <c r="B46" s="91" t="s">
+      <c r="B46" s="97" t="s">
         <v>19</v>
       </c>
       <c r="C46" s="49" t="s">
@@ -5383,9 +6388,9 @@
       <c r="F46" s="50"/>
       <c r="G46" s="50"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="89"/>
-      <c r="B47" s="92"/>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A47" s="95"/>
+      <c r="B47" s="98"/>
       <c r="C47" s="40" t="s">
         <v>4</v>
       </c>
@@ -5394,9 +6399,9 @@
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="89"/>
-      <c r="B48" s="93" t="s">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A48" s="95"/>
+      <c r="B48" s="99" t="s">
         <v>20</v>
       </c>
       <c r="C48" s="43" t="s">
@@ -5407,9 +6412,9 @@
       <c r="F48" s="6"/>
       <c r="G48" s="6"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="90"/>
-      <c r="B49" s="94"/>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A49" s="96"/>
+      <c r="B49" s="100"/>
       <c r="C49" s="41" t="s">
         <v>4</v>
       </c>
@@ -5420,6 +6425,30 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B28:B29"/>
     <mergeCell ref="A46:A49"/>
     <mergeCell ref="B46:B47"/>
     <mergeCell ref="B48:B49"/>
@@ -5432,37 +6461,13 @@
     <mergeCell ref="A42:A45"/>
     <mergeCell ref="B42:B43"/>
     <mergeCell ref="B44:B45"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B12:B13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G27"/>
   <sheetViews>
@@ -5470,16 +6475,16 @@
       <selection activeCell="S27" sqref="S27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" customWidth="1"/>
-    <col min="6" max="6" width="31.85546875" customWidth="1"/>
-    <col min="7" max="7" width="23.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.54296875" customWidth="1"/>
+    <col min="5" max="5" width="22.54296875" customWidth="1"/>
+    <col min="6" max="6" width="31.81640625" customWidth="1"/>
+    <col min="7" max="7" width="23.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="23" t="s">
         <v>32</v>
       </c>
@@ -5502,7 +6507,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
         <v>33</v>
       </c>
@@ -5525,7 +6530,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="16"/>
       <c r="B3" s="16" t="s">
         <v>20</v>
@@ -5546,7 +6551,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
         <v>2</v>
       </c>
@@ -5569,7 +6574,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="16"/>
       <c r="B5" s="16" t="s">
         <v>20</v>
@@ -5590,7 +6595,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="13" t="s">
         <v>5</v>
       </c>
@@ -5613,7 +6618,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="16"/>
       <c r="B7" s="16" t="s">
         <v>20</v>
@@ -5634,7 +6639,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="13" t="s">
         <v>6</v>
       </c>
@@ -5657,7 +6662,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="16"/>
       <c r="B9" s="16" t="s">
         <v>20</v>
@@ -5678,7 +6683,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="13" t="s">
         <v>7</v>
       </c>
@@ -5701,7 +6706,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="16"/>
       <c r="B11" s="16" t="s">
         <v>20</v>
@@ -5722,7 +6727,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="13" t="s">
         <v>8</v>
       </c>
@@ -5745,7 +6750,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="16"/>
       <c r="B13" s="16" t="s">
         <v>20</v>
@@ -5766,7 +6771,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="13" t="s">
         <v>9</v>
       </c>
@@ -5789,7 +6794,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="16"/>
       <c r="B15" s="16" t="s">
         <v>20</v>
@@ -5810,7 +6815,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="13" t="s">
         <v>10</v>
       </c>
@@ -5833,7 +6838,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="16"/>
       <c r="B17" s="16" t="s">
         <v>20</v>
@@ -5854,7 +6859,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="13" t="s">
         <v>11</v>
       </c>
@@ -5877,7 +6882,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" s="16"/>
       <c r="B19" s="16" t="s">
         <v>20</v>
@@ -5898,7 +6903,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="13" t="s">
         <v>12</v>
       </c>
@@ -5921,7 +6926,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A21" s="16"/>
       <c r="B21" s="16" t="s">
         <v>20</v>
@@ -5942,7 +6947,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="13" t="s">
         <v>13</v>
       </c>
@@ -5965,7 +6970,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" s="16"/>
       <c r="B23" s="16" t="s">
         <v>20</v>
@@ -5986,7 +6991,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A24" s="13" t="s">
         <v>14</v>
       </c>
@@ -6009,7 +7014,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" s="16"/>
       <c r="B25" s="16" t="s">
         <v>20</v>
@@ -6030,7 +7035,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A26" s="13" t="s">
         <v>15</v>
       </c>
@@ -6053,7 +7058,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A27" s="16"/>
       <c r="B27" s="16" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
new mean rate figure
</commit_message>
<xml_diff>
--- a/main/beast/all/chromosome/clade/clades_data_summary.xlsx
+++ b/main/beast/all/chromosome/clade/clades_data_summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ktmea\Projects\plague-phylogeography-projects\main\beast\all\chromosome\clade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63442D45-C96F-4ED7-A81F-3B6467F9EE4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D8169C-63FC-40A2-A8E2-BF663BB06406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="noHyperPrior" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="67">
   <si>
     <t>Clade</t>
   </si>
@@ -236,13 +236,17 @@
   <si>
     <t>high calendar</t>
   </si>
+  <si>
+    <t>bf</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
   </numFmts>
   <fonts count="22" x14ac:knownFonts="1">
     <font>
@@ -878,7 +882,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1109,74 +1113,75 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2159,10 +2164,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C48BE43A-44C4-45D0-8B2E-E3D4809D2185}">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2171,9 +2176,10 @@
     <col min="4" max="4" width="18.81640625" customWidth="1"/>
     <col min="5" max="5" width="15.90625" customWidth="1"/>
     <col min="6" max="6" width="26.7265625" customWidth="1"/>
+    <col min="11" max="11" width="11.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>45</v>
       </c>
@@ -2204,8 +2210,11 @@
       <c r="J1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -2236,8 +2245,12 @@
       <c r="J2">
         <v>-593.88124430000005</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K2" s="106">
+        <f>E2-D2</f>
+        <v>5.9207999994978309</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -2268,8 +2281,12 @@
       <c r="J3">
         <v>-385.78389490000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K3" s="106">
+        <f t="shared" ref="K3:K13" si="0">E3-D3</f>
+        <v>13297.716300000437</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -2300,8 +2317,12 @@
       <c r="J4">
         <v>-254.77459999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K4" s="106">
+        <f t="shared" si="0"/>
+        <v>12.378299999982119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -2317,7 +2338,7 @@
       <c r="E5">
         <v>-5892741.3773999996</v>
       </c>
-      <c r="F5" s="104" t="s">
+      <c r="F5" s="83" t="s">
         <v>57</v>
       </c>
       <c r="G5" s="75">
@@ -2332,8 +2353,12 @@
       <c r="J5">
         <v>-1201.954935</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K5" s="106">
+        <f>C5-B5</f>
+        <v>83.002000000327826</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -2364,8 +2389,12 @@
       <c r="J6">
         <v>-247.68818719999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K6" s="106">
+        <f t="shared" si="0"/>
+        <v>12.690900000743568</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -2381,7 +2410,7 @@
       <c r="E7">
         <v>-5891354.5140000004</v>
       </c>
-      <c r="F7" s="103" t="s">
+      <c r="F7" s="82" t="s">
         <v>57</v>
       </c>
       <c r="G7" s="75">
@@ -2396,8 +2425,12 @@
       <c r="J7">
         <v>-183.623559</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K7" s="106">
+        <f t="shared" si="0"/>
+        <v>-10.331400000490248</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -2428,8 +2461,12 @@
       <c r="J8">
         <v>-149.0783825</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K8" s="106">
+        <f t="shared" si="0"/>
+        <v>35.669999999925494</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -2460,8 +2497,12 @@
       <c r="J9">
         <v>-488.94726839999998</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K9" s="106">
+        <f t="shared" si="0"/>
+        <v>44.081500000320375</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -2477,7 +2518,7 @@
       <c r="E10">
         <v>-5892804.6540000001</v>
       </c>
-      <c r="F10" s="103" t="s">
+      <c r="F10" s="82" t="s">
         <v>57</v>
       </c>
       <c r="G10" s="75">
@@ -2492,8 +2533,12 @@
       <c r="J10">
         <v>-278.7095774</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K10" s="106">
+        <f t="shared" si="0"/>
+        <v>-13.384899999946356</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -2524,8 +2569,12 @@
       <c r="J11">
         <v>-319.89632169999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K11" s="106">
+        <f t="shared" si="0"/>
+        <v>3.9017000002786517</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -2541,7 +2590,7 @@
       <c r="E12">
         <v>-5887505.8404999999</v>
       </c>
-      <c r="F12" s="103" t="s">
+      <c r="F12" s="82" t="s">
         <v>57</v>
       </c>
       <c r="G12" s="75">
@@ -2556,8 +2605,12 @@
       <c r="J12">
         <v>-129.10517160000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K12" s="106">
+        <f t="shared" si="0"/>
+        <v>-11.17200000025332</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -2587,6 +2640,10 @@
       </c>
       <c r="J13">
         <v>-88.233202599999998</v>
+      </c>
+      <c r="K13" s="106">
+        <f t="shared" si="0"/>
+        <v>3.6091000000014901</v>
       </c>
     </row>
   </sheetData>
@@ -3029,7 +3086,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D48" sqref="A42:XFD48"/>
     </sheetView>
   </sheetViews>
@@ -3068,13 +3125,13 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="82" t="s">
+      <c r="A2" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="84" t="s">
+      <c r="B2" s="95" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="84" t="s">
+      <c r="C2" s="95" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -3090,9 +3147,9 @@
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="82"/>
-      <c r="B3" s="84"/>
-      <c r="C3" s="84"/>
+      <c r="A3" s="85"/>
+      <c r="B3" s="95"/>
+      <c r="C3" s="95"/>
       <c r="D3" s="2" t="s">
         <v>30</v>
       </c>
@@ -3105,9 +3162,9 @@
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="82"/>
-      <c r="B4" s="84"/>
-      <c r="C4" s="84" t="s">
+      <c r="A4" s="85"/>
+      <c r="B4" s="95"/>
+      <c r="C4" s="95" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -3123,9 +3180,9 @@
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="82"/>
-      <c r="B5" s="84"/>
-      <c r="C5" s="84"/>
+      <c r="A5" s="85"/>
+      <c r="B5" s="95"/>
+      <c r="C5" s="95"/>
       <c r="D5" s="2" t="s">
         <v>30</v>
       </c>
@@ -3138,11 +3195,11 @@
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="82"/>
-      <c r="B6" s="85" t="s">
+      <c r="A6" s="85"/>
+      <c r="B6" s="90" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="85" t="s">
+      <c r="C6" s="90" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="11" t="s">
@@ -3158,9 +3215,9 @@
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="82"/>
-      <c r="B7" s="85"/>
-      <c r="C7" s="85"/>
+      <c r="A7" s="85"/>
+      <c r="B7" s="90"/>
+      <c r="C7" s="90"/>
       <c r="D7" s="2" t="s">
         <v>30</v>
       </c>
@@ -3173,9 +3230,9 @@
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="82"/>
-      <c r="B8" s="85"/>
-      <c r="C8" s="84" t="s">
+      <c r="A8" s="85"/>
+      <c r="B8" s="90"/>
+      <c r="C8" s="95" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -3191,9 +3248,9 @@
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="83"/>
-      <c r="B9" s="86"/>
-      <c r="C9" s="87"/>
+      <c r="A9" s="86"/>
+      <c r="B9" s="91"/>
+      <c r="C9" s="96"/>
       <c r="D9" s="3" t="s">
         <v>30</v>
       </c>
@@ -3206,13 +3263,13 @@
       <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="88" t="s">
+      <c r="A10" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="89" t="s">
+      <c r="B10" s="94" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="89" t="s">
+      <c r="C10" s="94" t="s">
         <v>3</v>
       </c>
       <c r="D10" s="4" t="s">
@@ -3228,9 +3285,9 @@
       <c r="G10" s="50"/>
     </row>
     <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="82"/>
-      <c r="B11" s="84"/>
-      <c r="C11" s="84"/>
+      <c r="A11" s="85"/>
+      <c r="B11" s="95"/>
+      <c r="C11" s="95"/>
       <c r="D11" s="2" t="s">
         <v>30</v>
       </c>
@@ -3243,9 +3300,9 @@
       <c r="G11" s="6"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="82"/>
-      <c r="B12" s="84"/>
-      <c r="C12" s="84" t="s">
+      <c r="A12" s="85"/>
+      <c r="B12" s="95"/>
+      <c r="C12" s="95" t="s">
         <v>4</v>
       </c>
       <c r="D12" s="2" t="s">
@@ -3261,9 +3318,9 @@
       <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="82"/>
-      <c r="B13" s="84"/>
-      <c r="C13" s="84"/>
+      <c r="A13" s="85"/>
+      <c r="B13" s="95"/>
+      <c r="C13" s="95"/>
       <c r="D13" s="2" t="s">
         <v>30</v>
       </c>
@@ -3276,11 +3333,11 @@
       <c r="G13" s="6"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="82"/>
-      <c r="B14" s="90" t="s">
+      <c r="A14" s="85"/>
+      <c r="B14" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="84" t="s">
+      <c r="C14" s="95" t="s">
         <v>3</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -3296,9 +3353,9 @@
       <c r="G14" s="6"/>
     </row>
     <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="82"/>
-      <c r="B15" s="90"/>
-      <c r="C15" s="84"/>
+      <c r="A15" s="85"/>
+      <c r="B15" s="88"/>
+      <c r="C15" s="95"/>
       <c r="D15" s="2" t="s">
         <v>30</v>
       </c>
@@ -3311,9 +3368,9 @@
       <c r="G15" s="6"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="82"/>
-      <c r="B16" s="90"/>
-      <c r="C16" s="90" t="s">
+      <c r="A16" s="85"/>
+      <c r="B16" s="88"/>
+      <c r="C16" s="88" t="s">
         <v>4</v>
       </c>
       <c r="D16" s="8" t="s">
@@ -3329,9 +3386,9 @@
       <c r="G16" s="6"/>
     </row>
     <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="83"/>
-      <c r="B17" s="91"/>
-      <c r="C17" s="91"/>
+      <c r="A17" s="86"/>
+      <c r="B17" s="89"/>
+      <c r="C17" s="89"/>
       <c r="D17" s="3" t="s">
         <v>30</v>
       </c>
@@ -3344,13 +3401,13 @@
       <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="82" t="s">
+      <c r="A18" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="92" t="s">
+      <c r="B18" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="92" t="s">
+      <c r="C18" s="87" t="s">
         <v>3</v>
       </c>
       <c r="D18" s="9" t="s">
@@ -3365,9 +3422,9 @@
       </c>
     </row>
     <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="82"/>
-      <c r="B19" s="92"/>
-      <c r="C19" s="92"/>
+      <c r="A19" s="85"/>
+      <c r="B19" s="87"/>
+      <c r="C19" s="87"/>
       <c r="D19" s="9" t="s">
         <v>30</v>
       </c>
@@ -3379,9 +3436,9 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="82"/>
-      <c r="B20" s="92"/>
-      <c r="C20" s="92" t="s">
+      <c r="A20" s="85"/>
+      <c r="B20" s="87"/>
+      <c r="C20" s="87" t="s">
         <v>4</v>
       </c>
       <c r="D20" s="9" t="s">
@@ -3396,9 +3453,9 @@
       </c>
     </row>
     <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="82"/>
-      <c r="B21" s="92"/>
-      <c r="C21" s="92"/>
+      <c r="A21" s="85"/>
+      <c r="B21" s="87"/>
+      <c r="C21" s="87"/>
       <c r="D21" s="9" t="s">
         <v>30</v>
       </c>
@@ -3410,11 +3467,11 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" s="82"/>
-      <c r="B22" s="85" t="s">
+      <c r="A22" s="85"/>
+      <c r="B22" s="90" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="85" t="s">
+      <c r="C22" s="90" t="s">
         <v>3</v>
       </c>
       <c r="D22" s="11" t="s">
@@ -3429,9 +3486,9 @@
       </c>
     </row>
     <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="82"/>
-      <c r="B23" s="85"/>
-      <c r="C23" s="85"/>
+      <c r="A23" s="85"/>
+      <c r="B23" s="90"/>
+      <c r="C23" s="90"/>
       <c r="D23" s="9" t="s">
         <v>30</v>
       </c>
@@ -3443,9 +3500,9 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="82"/>
-      <c r="B24" s="85"/>
-      <c r="C24" s="92" t="s">
+      <c r="A24" s="85"/>
+      <c r="B24" s="90"/>
+      <c r="C24" s="87" t="s">
         <v>4</v>
       </c>
       <c r="D24" s="9" t="s">
@@ -3460,9 +3517,9 @@
       </c>
     </row>
     <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="83"/>
-      <c r="B25" s="86"/>
-      <c r="C25" s="93"/>
+      <c r="A25" s="86"/>
+      <c r="B25" s="91"/>
+      <c r="C25" s="92"/>
       <c r="D25" s="10" t="s">
         <v>30</v>
       </c>
@@ -3474,13 +3531,13 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" s="82" t="s">
+      <c r="A26" s="85" t="s">
         <v>7</v>
       </c>
-      <c r="B26" s="92" t="s">
+      <c r="B26" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="92" t="s">
+      <c r="C26" s="87" t="s">
         <v>3</v>
       </c>
       <c r="D26" s="9" t="s">
@@ -3495,9 +3552,9 @@
       </c>
     </row>
     <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="82"/>
-      <c r="B27" s="92"/>
-      <c r="C27" s="92"/>
+      <c r="A27" s="85"/>
+      <c r="B27" s="87"/>
+      <c r="C27" s="87"/>
       <c r="D27" s="9" t="s">
         <v>30</v>
       </c>
@@ -3509,9 +3566,9 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="82"/>
-      <c r="B28" s="92"/>
-      <c r="C28" s="92" t="s">
+      <c r="A28" s="85"/>
+      <c r="B28" s="87"/>
+      <c r="C28" s="87" t="s">
         <v>4</v>
       </c>
       <c r="D28" s="9" t="s">
@@ -3526,9 +3583,9 @@
       </c>
     </row>
     <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="82"/>
-      <c r="B29" s="92"/>
-      <c r="C29" s="92"/>
+      <c r="A29" s="85"/>
+      <c r="B29" s="87"/>
+      <c r="C29" s="87"/>
       <c r="D29" s="9" t="s">
         <v>30</v>
       </c>
@@ -3540,11 +3597,11 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30" s="82"/>
-      <c r="B30" s="85" t="s">
+      <c r="A30" s="85"/>
+      <c r="B30" s="90" t="s">
         <v>20</v>
       </c>
-      <c r="C30" s="85" t="s">
+      <c r="C30" s="90" t="s">
         <v>3</v>
       </c>
       <c r="D30" s="11" t="s">
@@ -3559,9 +3616,9 @@
       </c>
     </row>
     <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="82"/>
-      <c r="B31" s="85"/>
-      <c r="C31" s="85"/>
+      <c r="A31" s="85"/>
+      <c r="B31" s="90"/>
+      <c r="C31" s="90"/>
       <c r="D31" s="9" t="s">
         <v>30</v>
       </c>
@@ -3573,9 +3630,9 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A32" s="82"/>
-      <c r="B32" s="85"/>
-      <c r="C32" s="92" t="s">
+      <c r="A32" s="85"/>
+      <c r="B32" s="90"/>
+      <c r="C32" s="87" t="s">
         <v>4</v>
       </c>
       <c r="D32" s="9" t="s">
@@ -3590,9 +3647,9 @@
       </c>
     </row>
     <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="83"/>
-      <c r="B33" s="86"/>
-      <c r="C33" s="93"/>
+      <c r="A33" s="86"/>
+      <c r="B33" s="91"/>
+      <c r="C33" s="92"/>
       <c r="D33" s="10" t="s">
         <v>30</v>
       </c>
@@ -3604,13 +3661,13 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A34" s="82" t="s">
+      <c r="A34" s="85" t="s">
         <v>8</v>
       </c>
-      <c r="B34" s="92" t="s">
+      <c r="B34" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="C34" s="92" t="s">
+      <c r="C34" s="87" t="s">
         <v>3</v>
       </c>
       <c r="D34" s="9" t="s">
@@ -3625,9 +3682,9 @@
       </c>
     </row>
     <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="82"/>
-      <c r="B35" s="92"/>
-      <c r="C35" s="92"/>
+      <c r="A35" s="85"/>
+      <c r="B35" s="87"/>
+      <c r="C35" s="87"/>
       <c r="D35" s="9" t="s">
         <v>30</v>
       </c>
@@ -3639,9 +3696,9 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" s="82"/>
-      <c r="B36" s="92"/>
-      <c r="C36" s="92" t="s">
+      <c r="A36" s="85"/>
+      <c r="B36" s="87"/>
+      <c r="C36" s="87" t="s">
         <v>4</v>
       </c>
       <c r="D36" s="9" t="s">
@@ -3656,9 +3713,9 @@
       </c>
     </row>
     <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="82"/>
-      <c r="B37" s="92"/>
-      <c r="C37" s="92"/>
+      <c r="A37" s="85"/>
+      <c r="B37" s="87"/>
+      <c r="C37" s="87"/>
       <c r="D37" s="9" t="s">
         <v>30</v>
       </c>
@@ -3670,11 +3727,11 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A38" s="82"/>
-      <c r="B38" s="85" t="s">
+      <c r="A38" s="85"/>
+      <c r="B38" s="90" t="s">
         <v>20</v>
       </c>
-      <c r="C38" s="85" t="s">
+      <c r="C38" s="90" t="s">
         <v>3</v>
       </c>
       <c r="D38" s="11" t="s">
@@ -3689,9 +3746,9 @@
       </c>
     </row>
     <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="82"/>
-      <c r="B39" s="85"/>
-      <c r="C39" s="85"/>
+      <c r="A39" s="85"/>
+      <c r="B39" s="90"/>
+      <c r="C39" s="90"/>
       <c r="D39" s="9" t="s">
         <v>30</v>
       </c>
@@ -3703,9 +3760,9 @@
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A40" s="82"/>
-      <c r="B40" s="85"/>
-      <c r="C40" s="92" t="s">
+      <c r="A40" s="85"/>
+      <c r="B40" s="90"/>
+      <c r="C40" s="87" t="s">
         <v>4</v>
       </c>
       <c r="D40" s="9" t="s">
@@ -3720,9 +3777,9 @@
       </c>
     </row>
     <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="83"/>
-      <c r="B41" s="86"/>
-      <c r="C41" s="93"/>
+      <c r="A41" s="86"/>
+      <c r="B41" s="91"/>
+      <c r="C41" s="92"/>
       <c r="D41" s="10" t="s">
         <v>30</v>
       </c>
@@ -3734,13 +3791,13 @@
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A42" s="82" t="s">
+      <c r="A42" s="85" t="s">
         <v>9</v>
       </c>
-      <c r="B42" s="92" t="s">
+      <c r="B42" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="C42" s="92" t="s">
+      <c r="C42" s="87" t="s">
         <v>3</v>
       </c>
       <c r="D42" s="9" t="s">
@@ -3755,9 +3812,9 @@
       </c>
     </row>
     <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="82"/>
-      <c r="B43" s="92"/>
-      <c r="C43" s="92"/>
+      <c r="A43" s="85"/>
+      <c r="B43" s="87"/>
+      <c r="C43" s="87"/>
       <c r="D43" s="9" t="s">
         <v>30</v>
       </c>
@@ -3767,9 +3824,9 @@
       <c r="F43" s="58"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A44" s="82"/>
-      <c r="B44" s="92"/>
-      <c r="C44" s="92" t="s">
+      <c r="A44" s="85"/>
+      <c r="B44" s="87"/>
+      <c r="C44" s="87" t="s">
         <v>4</v>
       </c>
       <c r="D44" s="9" t="s">
@@ -3784,9 +3841,9 @@
       </c>
     </row>
     <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="82"/>
-      <c r="B45" s="92"/>
-      <c r="C45" s="92"/>
+      <c r="A45" s="85"/>
+      <c r="B45" s="87"/>
+      <c r="C45" s="87"/>
       <c r="D45" s="9" t="s">
         <v>30</v>
       </c>
@@ -3796,11 +3853,11 @@
       <c r="F45" s="58"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A46" s="82"/>
-      <c r="B46" s="90" t="s">
+      <c r="A46" s="85"/>
+      <c r="B46" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="C46" s="92" t="s">
+      <c r="C46" s="87" t="s">
         <v>3</v>
       </c>
       <c r="D46" s="9" t="s">
@@ -3815,9 +3872,9 @@
       </c>
     </row>
     <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="82"/>
-      <c r="B47" s="90"/>
-      <c r="C47" s="92"/>
+      <c r="A47" s="85"/>
+      <c r="B47" s="88"/>
+      <c r="C47" s="87"/>
       <c r="D47" s="9" t="s">
         <v>30</v>
       </c>
@@ -3827,9 +3884,9 @@
       <c r="F47" s="58"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A48" s="82"/>
-      <c r="B48" s="90"/>
-      <c r="C48" s="90" t="s">
+      <c r="A48" s="85"/>
+      <c r="B48" s="88"/>
+      <c r="C48" s="88" t="s">
         <v>4</v>
       </c>
       <c r="D48" s="8" t="s">
@@ -3844,9 +3901,9 @@
       </c>
     </row>
     <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="83"/>
-      <c r="B49" s="91"/>
-      <c r="C49" s="91"/>
+      <c r="A49" s="86"/>
+      <c r="B49" s="89"/>
+      <c r="C49" s="89"/>
       <c r="D49" s="10" t="s">
         <v>30</v>
       </c>
@@ -3858,13 +3915,13 @@
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A50" s="82" t="s">
+      <c r="A50" s="85" t="s">
         <v>10</v>
       </c>
-      <c r="B50" s="92" t="s">
+      <c r="B50" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="C50" s="92" t="s">
+      <c r="C50" s="87" t="s">
         <v>3</v>
       </c>
       <c r="D50" s="9" t="s">
@@ -3879,9 +3936,9 @@
       </c>
     </row>
     <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="82"/>
-      <c r="B51" s="92"/>
-      <c r="C51" s="92"/>
+      <c r="A51" s="85"/>
+      <c r="B51" s="87"/>
+      <c r="C51" s="87"/>
       <c r="D51" s="9" t="s">
         <v>30</v>
       </c>
@@ -3893,9 +3950,9 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A52" s="82"/>
-      <c r="B52" s="92"/>
-      <c r="C52" s="92" t="s">
+      <c r="A52" s="85"/>
+      <c r="B52" s="87"/>
+      <c r="C52" s="87" t="s">
         <v>4</v>
       </c>
       <c r="D52" s="9" t="s">
@@ -3910,9 +3967,9 @@
       </c>
     </row>
     <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="82"/>
-      <c r="B53" s="92"/>
-      <c r="C53" s="92"/>
+      <c r="A53" s="85"/>
+      <c r="B53" s="87"/>
+      <c r="C53" s="87"/>
       <c r="D53" s="9" t="s">
         <v>30</v>
       </c>
@@ -3924,11 +3981,11 @@
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A54" s="82"/>
-      <c r="B54" s="85" t="s">
+      <c r="A54" s="85"/>
+      <c r="B54" s="90" t="s">
         <v>20</v>
       </c>
-      <c r="C54" s="85" t="s">
+      <c r="C54" s="90" t="s">
         <v>3</v>
       </c>
       <c r="D54" s="11" t="s">
@@ -3943,9 +4000,9 @@
       </c>
     </row>
     <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="82"/>
-      <c r="B55" s="85"/>
-      <c r="C55" s="85"/>
+      <c r="A55" s="85"/>
+      <c r="B55" s="90"/>
+      <c r="C55" s="90"/>
       <c r="D55" s="9" t="s">
         <v>30</v>
       </c>
@@ -3957,9 +4014,9 @@
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A56" s="82"/>
-      <c r="B56" s="85"/>
-      <c r="C56" s="92" t="s">
+      <c r="A56" s="85"/>
+      <c r="B56" s="90"/>
+      <c r="C56" s="87" t="s">
         <v>4</v>
       </c>
       <c r="D56" s="9" t="s">
@@ -3974,9 +4031,9 @@
       </c>
     </row>
     <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="83"/>
-      <c r="B57" s="86"/>
-      <c r="C57" s="93"/>
+      <c r="A57" s="86"/>
+      <c r="B57" s="91"/>
+      <c r="C57" s="92"/>
       <c r="D57" s="10" t="s">
         <v>30</v>
       </c>
@@ -3988,13 +4045,13 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A58" s="82" t="s">
+      <c r="A58" s="85" t="s">
         <v>11</v>
       </c>
-      <c r="B58" s="92" t="s">
+      <c r="B58" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="C58" s="92" t="s">
+      <c r="C58" s="87" t="s">
         <v>3</v>
       </c>
       <c r="D58" s="9" t="s">
@@ -4009,9 +4066,9 @@
       </c>
     </row>
     <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="82"/>
-      <c r="B59" s="92"/>
-      <c r="C59" s="92"/>
+      <c r="A59" s="85"/>
+      <c r="B59" s="87"/>
+      <c r="C59" s="87"/>
       <c r="D59" s="9" t="s">
         <v>30</v>
       </c>
@@ -4023,9 +4080,9 @@
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A60" s="82"/>
-      <c r="B60" s="92"/>
-      <c r="C60" s="92" t="s">
+      <c r="A60" s="85"/>
+      <c r="B60" s="87"/>
+      <c r="C60" s="87" t="s">
         <v>4</v>
       </c>
       <c r="D60" s="9" t="s">
@@ -4040,9 +4097,9 @@
       </c>
     </row>
     <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="82"/>
-      <c r="B61" s="92"/>
-      <c r="C61" s="92"/>
+      <c r="A61" s="85"/>
+      <c r="B61" s="87"/>
+      <c r="C61" s="87"/>
       <c r="D61" s="9" t="s">
         <v>30</v>
       </c>
@@ -4054,11 +4111,11 @@
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A62" s="82"/>
-      <c r="B62" s="90" t="s">
+      <c r="A62" s="85"/>
+      <c r="B62" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="C62" s="92" t="s">
+      <c r="C62" s="87" t="s">
         <v>3</v>
       </c>
       <c r="D62" s="9" t="s">
@@ -4073,9 +4130,9 @@
       </c>
     </row>
     <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="82"/>
-      <c r="B63" s="90"/>
-      <c r="C63" s="92"/>
+      <c r="A63" s="85"/>
+      <c r="B63" s="88"/>
+      <c r="C63" s="87"/>
       <c r="D63" s="9" t="s">
         <v>30</v>
       </c>
@@ -4087,9 +4144,9 @@
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A64" s="82"/>
-      <c r="B64" s="90"/>
-      <c r="C64" s="90" t="s">
+      <c r="A64" s="85"/>
+      <c r="B64" s="88"/>
+      <c r="C64" s="88" t="s">
         <v>4</v>
       </c>
       <c r="D64" s="8" t="s">
@@ -4104,9 +4161,9 @@
       </c>
     </row>
     <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="83"/>
-      <c r="B65" s="91"/>
-      <c r="C65" s="91"/>
+      <c r="A65" s="86"/>
+      <c r="B65" s="89"/>
+      <c r="C65" s="89"/>
       <c r="D65" s="10" t="s">
         <v>30</v>
       </c>
@@ -4118,13 +4175,13 @@
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A66" s="82" t="s">
+      <c r="A66" s="85" t="s">
         <v>12</v>
       </c>
-      <c r="B66" s="92" t="s">
+      <c r="B66" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="C66" s="92" t="s">
+      <c r="C66" s="87" t="s">
         <v>3</v>
       </c>
       <c r="D66" s="9" t="s">
@@ -4139,9 +4196,9 @@
       </c>
     </row>
     <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="82"/>
-      <c r="B67" s="92"/>
-      <c r="C67" s="92"/>
+      <c r="A67" s="85"/>
+      <c r="B67" s="87"/>
+      <c r="C67" s="87"/>
       <c r="D67" s="9" t="s">
         <v>30</v>
       </c>
@@ -4153,9 +4210,9 @@
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A68" s="82"/>
-      <c r="B68" s="92"/>
-      <c r="C68" s="92" t="s">
+      <c r="A68" s="85"/>
+      <c r="B68" s="87"/>
+      <c r="C68" s="87" t="s">
         <v>4</v>
       </c>
       <c r="D68" s="9" t="s">
@@ -4164,15 +4221,15 @@
       <c r="E68" s="44">
         <v>-5896014.0886000004</v>
       </c>
-      <c r="F68" s="105">
+      <c r="F68" s="84">
         <f t="shared" si="9"/>
         <v>2.3832000000402331</v>
       </c>
     </row>
     <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="82"/>
-      <c r="B69" s="92"/>
-      <c r="C69" s="92"/>
+      <c r="A69" s="85"/>
+      <c r="B69" s="87"/>
+      <c r="C69" s="87"/>
       <c r="D69" s="9" t="s">
         <v>30</v>
       </c>
@@ -4184,11 +4241,11 @@
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A70" s="82"/>
-      <c r="B70" s="85" t="s">
+      <c r="A70" s="85"/>
+      <c r="B70" s="90" t="s">
         <v>20</v>
       </c>
-      <c r="C70" s="85" t="s">
+      <c r="C70" s="90" t="s">
         <v>3</v>
       </c>
       <c r="D70" s="11" t="s">
@@ -4203,9 +4260,9 @@
       </c>
     </row>
     <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="82"/>
-      <c r="B71" s="85"/>
-      <c r="C71" s="85"/>
+      <c r="A71" s="85"/>
+      <c r="B71" s="90"/>
+      <c r="C71" s="90"/>
       <c r="D71" s="9" t="s">
         <v>30</v>
       </c>
@@ -4217,9 +4274,9 @@
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A72" s="82"/>
-      <c r="B72" s="85"/>
-      <c r="C72" s="92" t="s">
+      <c r="A72" s="85"/>
+      <c r="B72" s="90"/>
+      <c r="C72" s="87" t="s">
         <v>4</v>
       </c>
       <c r="D72" s="9" t="s">
@@ -4234,9 +4291,9 @@
       </c>
     </row>
     <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="83"/>
-      <c r="B73" s="86"/>
-      <c r="C73" s="93"/>
+      <c r="A73" s="86"/>
+      <c r="B73" s="91"/>
+      <c r="C73" s="92"/>
       <c r="D73" s="10" t="s">
         <v>30</v>
       </c>
@@ -4248,13 +4305,13 @@
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A74" s="82" t="s">
+      <c r="A74" s="85" t="s">
         <v>13</v>
       </c>
-      <c r="B74" s="92" t="s">
+      <c r="B74" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="C74" s="92" t="s">
+      <c r="C74" s="87" t="s">
         <v>3</v>
       </c>
       <c r="D74" s="9" t="s">
@@ -4269,9 +4326,9 @@
       </c>
     </row>
     <row r="75" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="82"/>
-      <c r="B75" s="92"/>
-      <c r="C75" s="92"/>
+      <c r="A75" s="85"/>
+      <c r="B75" s="87"/>
+      <c r="C75" s="87"/>
       <c r="D75" s="9" t="s">
         <v>30</v>
       </c>
@@ -4283,9 +4340,9 @@
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A76" s="82"/>
-      <c r="B76" s="92"/>
-      <c r="C76" s="92" t="s">
+      <c r="A76" s="85"/>
+      <c r="B76" s="87"/>
+      <c r="C76" s="87" t="s">
         <v>4</v>
       </c>
       <c r="D76" s="9" t="s">
@@ -4300,9 +4357,9 @@
       </c>
     </row>
     <row r="77" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="82"/>
-      <c r="B77" s="92"/>
-      <c r="C77" s="92"/>
+      <c r="A77" s="85"/>
+      <c r="B77" s="87"/>
+      <c r="C77" s="87"/>
       <c r="D77" s="9" t="s">
         <v>30</v>
       </c>
@@ -4314,11 +4371,11 @@
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A78" s="82"/>
-      <c r="B78" s="85" t="s">
+      <c r="A78" s="85"/>
+      <c r="B78" s="90" t="s">
         <v>20</v>
       </c>
-      <c r="C78" s="85" t="s">
+      <c r="C78" s="90" t="s">
         <v>3</v>
       </c>
       <c r="D78" s="11" t="s">
@@ -4333,9 +4390,9 @@
       </c>
     </row>
     <row r="79" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="82"/>
-      <c r="B79" s="85"/>
-      <c r="C79" s="85"/>
+      <c r="A79" s="85"/>
+      <c r="B79" s="90"/>
+      <c r="C79" s="90"/>
       <c r="D79" s="9" t="s">
         <v>30</v>
       </c>
@@ -4347,9 +4404,9 @@
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A80" s="82"/>
-      <c r="B80" s="85"/>
-      <c r="C80" s="92" t="s">
+      <c r="A80" s="85"/>
+      <c r="B80" s="90"/>
+      <c r="C80" s="87" t="s">
         <v>4</v>
       </c>
       <c r="D80" s="9" t="s">
@@ -4364,9 +4421,9 @@
       </c>
     </row>
     <row r="81" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="83"/>
-      <c r="B81" s="86"/>
-      <c r="C81" s="93"/>
+      <c r="A81" s="86"/>
+      <c r="B81" s="91"/>
+      <c r="C81" s="92"/>
       <c r="D81" s="10" t="s">
         <v>30</v>
       </c>
@@ -4378,13 +4435,13 @@
       </c>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A82" s="82" t="s">
+      <c r="A82" s="85" t="s">
         <v>14</v>
       </c>
-      <c r="B82" s="92" t="s">
+      <c r="B82" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="C82" s="92" t="s">
+      <c r="C82" s="87" t="s">
         <v>3</v>
       </c>
       <c r="D82" s="9" t="s">
@@ -4399,9 +4456,9 @@
       </c>
     </row>
     <row r="83" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="82"/>
-      <c r="B83" s="92"/>
-      <c r="C83" s="92"/>
+      <c r="A83" s="85"/>
+      <c r="B83" s="87"/>
+      <c r="C83" s="87"/>
       <c r="D83" s="9" t="s">
         <v>30</v>
       </c>
@@ -4413,9 +4470,9 @@
       </c>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A84" s="82"/>
-      <c r="B84" s="92"/>
-      <c r="C84" s="92" t="s">
+      <c r="A84" s="85"/>
+      <c r="B84" s="87"/>
+      <c r="C84" s="87" t="s">
         <v>4</v>
       </c>
       <c r="D84" s="9" t="s">
@@ -4430,9 +4487,9 @@
       </c>
     </row>
     <row r="85" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="82"/>
-      <c r="B85" s="92"/>
-      <c r="C85" s="92"/>
+      <c r="A85" s="85"/>
+      <c r="B85" s="87"/>
+      <c r="C85" s="87"/>
       <c r="D85" s="9" t="s">
         <v>30</v>
       </c>
@@ -4444,11 +4501,11 @@
       </c>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A86" s="82"/>
-      <c r="B86" s="85" t="s">
+      <c r="A86" s="85"/>
+      <c r="B86" s="90" t="s">
         <v>20</v>
       </c>
-      <c r="C86" s="85" t="s">
+      <c r="C86" s="90" t="s">
         <v>3</v>
       </c>
       <c r="D86" s="11" t="s">
@@ -4463,9 +4520,9 @@
       </c>
     </row>
     <row r="87" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="82"/>
-      <c r="B87" s="85"/>
-      <c r="C87" s="85"/>
+      <c r="A87" s="85"/>
+      <c r="B87" s="90"/>
+      <c r="C87" s="90"/>
       <c r="D87" s="9" t="s">
         <v>30</v>
       </c>
@@ -4477,9 +4534,9 @@
       </c>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A88" s="82"/>
-      <c r="B88" s="85"/>
-      <c r="C88" s="92" t="s">
+      <c r="A88" s="85"/>
+      <c r="B88" s="90"/>
+      <c r="C88" s="87" t="s">
         <v>4</v>
       </c>
       <c r="D88" s="9" t="s">
@@ -4494,9 +4551,9 @@
       </c>
     </row>
     <row r="89" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A89" s="83"/>
-      <c r="B89" s="86"/>
-      <c r="C89" s="93"/>
+      <c r="A89" s="86"/>
+      <c r="B89" s="91"/>
+      <c r="C89" s="92"/>
       <c r="D89" s="10" t="s">
         <v>30</v>
       </c>
@@ -4508,13 +4565,13 @@
       </c>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A90" s="82" t="s">
+      <c r="A90" s="85" t="s">
         <v>15</v>
       </c>
-      <c r="B90" s="92" t="s">
+      <c r="B90" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="C90" s="92" t="s">
+      <c r="C90" s="87" t="s">
         <v>3</v>
       </c>
       <c r="D90" s="9" t="s">
@@ -4533,9 +4590,9 @@
       <c r="N90" s="75"/>
     </row>
     <row r="91" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A91" s="82"/>
-      <c r="B91" s="92"/>
-      <c r="C91" s="92"/>
+      <c r="A91" s="85"/>
+      <c r="B91" s="87"/>
+      <c r="C91" s="87"/>
       <c r="D91" s="9" t="s">
         <v>30</v>
       </c>
@@ -4547,9 +4604,9 @@
       </c>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A92" s="82"/>
-      <c r="B92" s="92"/>
-      <c r="C92" s="92" t="s">
+      <c r="A92" s="85"/>
+      <c r="B92" s="87"/>
+      <c r="C92" s="87" t="s">
         <v>4</v>
       </c>
       <c r="D92" s="9" t="s">
@@ -4564,9 +4621,9 @@
       </c>
     </row>
     <row r="93" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="82"/>
-      <c r="B93" s="92"/>
-      <c r="C93" s="92"/>
+      <c r="A93" s="85"/>
+      <c r="B93" s="87"/>
+      <c r="C93" s="87"/>
       <c r="D93" s="9" t="s">
         <v>30</v>
       </c>
@@ -4579,11 +4636,11 @@
       <c r="G93" s="47"/>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A94" s="82"/>
-      <c r="B94" s="90" t="s">
+      <c r="A94" s="85"/>
+      <c r="B94" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="C94" s="92" t="s">
+      <c r="C94" s="87" t="s">
         <v>3</v>
       </c>
       <c r="D94" s="9" t="s">
@@ -4598,9 +4655,9 @@
       </c>
     </row>
     <row r="95" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="82"/>
-      <c r="B95" s="90"/>
-      <c r="C95" s="92"/>
+      <c r="A95" s="85"/>
+      <c r="B95" s="88"/>
+      <c r="C95" s="87"/>
       <c r="D95" s="9" t="s">
         <v>30</v>
       </c>
@@ -4612,9 +4669,9 @@
       </c>
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A96" s="82"/>
-      <c r="B96" s="90"/>
-      <c r="C96" s="90" t="s">
+      <c r="A96" s="85"/>
+      <c r="B96" s="88"/>
+      <c r="C96" s="88" t="s">
         <v>4</v>
       </c>
       <c r="D96" s="8" t="s">
@@ -4629,9 +4686,9 @@
       </c>
     </row>
     <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A97" s="83"/>
-      <c r="B97" s="91"/>
-      <c r="C97" s="91"/>
+      <c r="A97" s="86"/>
+      <c r="B97" s="89"/>
+      <c r="C97" s="89"/>
       <c r="D97" s="10" t="s">
         <v>30</v>
       </c>
@@ -4644,6 +4701,83 @@
     </row>
   </sheetData>
   <mergeCells count="84">
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="A10:A17"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="A18:A25"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="A26:A33"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="A34:A41"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="A42:A49"/>
+    <mergeCell ref="B42:B45"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="B46:B49"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="A50:A57"/>
+    <mergeCell ref="B50:B53"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="B54:B57"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="A58:A65"/>
+    <mergeCell ref="B58:B61"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="B62:B65"/>
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="C64:C65"/>
+    <mergeCell ref="A66:A73"/>
+    <mergeCell ref="B66:B69"/>
+    <mergeCell ref="C66:C67"/>
+    <mergeCell ref="C68:C69"/>
+    <mergeCell ref="B70:B73"/>
+    <mergeCell ref="C70:C71"/>
+    <mergeCell ref="C72:C73"/>
+    <mergeCell ref="A74:A81"/>
+    <mergeCell ref="B74:B77"/>
+    <mergeCell ref="C74:C75"/>
+    <mergeCell ref="C76:C77"/>
+    <mergeCell ref="B78:B81"/>
+    <mergeCell ref="C78:C79"/>
+    <mergeCell ref="C80:C81"/>
+    <mergeCell ref="A82:A89"/>
+    <mergeCell ref="B82:B85"/>
+    <mergeCell ref="C82:C83"/>
+    <mergeCell ref="C84:C85"/>
+    <mergeCell ref="B86:B89"/>
+    <mergeCell ref="C86:C87"/>
+    <mergeCell ref="C88:C89"/>
     <mergeCell ref="A90:A97"/>
     <mergeCell ref="B90:B93"/>
     <mergeCell ref="C90:C91"/>
@@ -4651,83 +4785,6 @@
     <mergeCell ref="B94:B97"/>
     <mergeCell ref="C94:C95"/>
     <mergeCell ref="C96:C97"/>
-    <mergeCell ref="A82:A89"/>
-    <mergeCell ref="B82:B85"/>
-    <mergeCell ref="C82:C83"/>
-    <mergeCell ref="C84:C85"/>
-    <mergeCell ref="B86:B89"/>
-    <mergeCell ref="C86:C87"/>
-    <mergeCell ref="C88:C89"/>
-    <mergeCell ref="A74:A81"/>
-    <mergeCell ref="B74:B77"/>
-    <mergeCell ref="C74:C75"/>
-    <mergeCell ref="C76:C77"/>
-    <mergeCell ref="B78:B81"/>
-    <mergeCell ref="C78:C79"/>
-    <mergeCell ref="C80:C81"/>
-    <mergeCell ref="A66:A73"/>
-    <mergeCell ref="B66:B69"/>
-    <mergeCell ref="C66:C67"/>
-    <mergeCell ref="C68:C69"/>
-    <mergeCell ref="B70:B73"/>
-    <mergeCell ref="C70:C71"/>
-    <mergeCell ref="C72:C73"/>
-    <mergeCell ref="A58:A65"/>
-    <mergeCell ref="B58:B61"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="B62:B65"/>
-    <mergeCell ref="C62:C63"/>
-    <mergeCell ref="C64:C65"/>
-    <mergeCell ref="A50:A57"/>
-    <mergeCell ref="B50:B53"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="B54:B57"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="A42:A49"/>
-    <mergeCell ref="B42:B45"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="B46:B49"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="A34:A41"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="B38:B41"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="A26:A33"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="A18:A25"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="A10:A17"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="A2:A9"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C6:C7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4769,10 +4826,10 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="82" t="s">
+      <c r="A2" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="84" t="s">
+      <c r="B2" s="95" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="80" t="s">
@@ -4790,8 +4847,8 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="82"/>
-      <c r="B3" s="84"/>
+      <c r="A3" s="85"/>
+      <c r="B3" s="95"/>
       <c r="C3" s="80" t="s">
         <v>4</v>
       </c>
@@ -4807,8 +4864,8 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="82"/>
-      <c r="B4" s="85" t="s">
+      <c r="A4" s="85"/>
+      <c r="B4" s="90" t="s">
         <v>20</v>
       </c>
       <c r="C4" s="78" t="s">
@@ -4826,8 +4883,8 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="82"/>
-      <c r="B5" s="85"/>
+      <c r="A5" s="85"/>
+      <c r="B5" s="90"/>
       <c r="C5" s="80" t="s">
         <v>4</v>
       </c>
@@ -4843,10 +4900,10 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="88" t="s">
+      <c r="A6" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="89" t="s">
+      <c r="B6" s="94" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="79" t="s">
@@ -4864,8 +4921,8 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="82"/>
-      <c r="B7" s="84"/>
+      <c r="A7" s="85"/>
+      <c r="B7" s="95"/>
       <c r="C7" s="80" t="s">
         <v>4</v>
       </c>
@@ -4881,8 +4938,8 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="82"/>
-      <c r="B8" s="90" t="s">
+      <c r="A8" s="85"/>
+      <c r="B8" s="88" t="s">
         <v>20</v>
       </c>
       <c r="C8" s="80" t="s">
@@ -4900,8 +4957,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="82"/>
-      <c r="B9" s="90"/>
+      <c r="A9" s="85"/>
+      <c r="B9" s="88"/>
       <c r="C9" s="77" t="s">
         <v>4</v>
       </c>
@@ -4917,10 +4974,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="82" t="s">
+      <c r="A10" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="92" t="s">
+      <c r="B10" s="87" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="76" t="s">
@@ -4938,8 +4995,8 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="82"/>
-      <c r="B11" s="92"/>
+      <c r="A11" s="85"/>
+      <c r="B11" s="87"/>
       <c r="C11" s="76" t="s">
         <v>4</v>
       </c>
@@ -4955,8 +5012,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="82"/>
-      <c r="B12" s="85" t="s">
+      <c r="A12" s="85"/>
+      <c r="B12" s="90" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="78" t="s">
@@ -4974,8 +5031,8 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="82"/>
-      <c r="B13" s="85"/>
+      <c r="A13" s="85"/>
+      <c r="B13" s="90"/>
       <c r="C13" s="76" t="s">
         <v>4</v>
       </c>
@@ -4991,10 +5048,10 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="82" t="s">
+      <c r="A14" s="85" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="92" t="s">
+      <c r="B14" s="87" t="s">
         <v>19</v>
       </c>
       <c r="C14" s="76" t="s">
@@ -5012,8 +5069,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="82"/>
-      <c r="B15" s="92"/>
+      <c r="A15" s="85"/>
+      <c r="B15" s="87"/>
       <c r="C15" s="76" t="s">
         <v>4</v>
       </c>
@@ -5029,8 +5086,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="82"/>
-      <c r="B16" s="85" t="s">
+      <c r="A16" s="85"/>
+      <c r="B16" s="90" t="s">
         <v>20</v>
       </c>
       <c r="C16" s="78" t="s">
@@ -5048,8 +5105,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="82"/>
-      <c r="B17" s="85"/>
+      <c r="A17" s="85"/>
+      <c r="B17" s="90"/>
       <c r="C17" s="76" t="s">
         <v>4</v>
       </c>
@@ -5065,10 +5122,10 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="82" t="s">
+      <c r="A18" s="85" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="92" t="s">
+      <c r="B18" s="87" t="s">
         <v>19</v>
       </c>
       <c r="C18" s="76" t="s">
@@ -5086,8 +5143,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="82"/>
-      <c r="B19" s="92"/>
+      <c r="A19" s="85"/>
+      <c r="B19" s="87"/>
       <c r="C19" s="76" t="s">
         <v>4</v>
       </c>
@@ -5103,8 +5160,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="82"/>
-      <c r="B20" s="85" t="s">
+      <c r="A20" s="85"/>
+      <c r="B20" s="90" t="s">
         <v>20</v>
       </c>
       <c r="C20" s="78" t="s">
@@ -5122,8 +5179,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" s="82"/>
-      <c r="B21" s="85"/>
+      <c r="A21" s="85"/>
+      <c r="B21" s="90"/>
       <c r="C21" s="76" t="s">
         <v>4</v>
       </c>
@@ -5139,10 +5196,10 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22" s="82" t="s">
+      <c r="A22" s="85" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="92" t="s">
+      <c r="B22" s="87" t="s">
         <v>19</v>
       </c>
       <c r="C22" s="76" t="s">
@@ -5160,8 +5217,8 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="82"/>
-      <c r="B23" s="92"/>
+      <c r="A23" s="85"/>
+      <c r="B23" s="87"/>
       <c r="C23" s="76" t="s">
         <v>4</v>
       </c>
@@ -5177,8 +5234,8 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="82"/>
-      <c r="B24" s="90" t="s">
+      <c r="A24" s="85"/>
+      <c r="B24" s="88" t="s">
         <v>20</v>
       </c>
       <c r="C24" s="76" t="s">
@@ -5196,8 +5253,8 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="82"/>
-      <c r="B25" s="90"/>
+      <c r="A25" s="85"/>
+      <c r="B25" s="88"/>
       <c r="C25" s="77" t="s">
         <v>4</v>
       </c>
@@ -5213,10 +5270,10 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="82" t="s">
+      <c r="A26" s="85" t="s">
         <v>10</v>
       </c>
-      <c r="B26" s="92" t="s">
+      <c r="B26" s="87" t="s">
         <v>19</v>
       </c>
       <c r="C26" s="76" t="s">
@@ -5234,8 +5291,8 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" s="82"/>
-      <c r="B27" s="92"/>
+      <c r="A27" s="85"/>
+      <c r="B27" s="87"/>
       <c r="C27" s="76" t="s">
         <v>4</v>
       </c>
@@ -5251,8 +5308,8 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A28" s="82"/>
-      <c r="B28" s="85" t="s">
+      <c r="A28" s="85"/>
+      <c r="B28" s="90" t="s">
         <v>20</v>
       </c>
       <c r="C28" s="78" t="s">
@@ -5270,8 +5327,8 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="82"/>
-      <c r="B29" s="85"/>
+      <c r="A29" s="85"/>
+      <c r="B29" s="90"/>
       <c r="C29" s="76" t="s">
         <v>4</v>
       </c>
@@ -5287,10 +5344,10 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" s="82" t="s">
+      <c r="A30" s="85" t="s">
         <v>11</v>
       </c>
-      <c r="B30" s="92" t="s">
+      <c r="B30" s="87" t="s">
         <v>19</v>
       </c>
       <c r="C30" s="76" t="s">
@@ -5308,8 +5365,8 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="82"/>
-      <c r="B31" s="92"/>
+      <c r="A31" s="85"/>
+      <c r="B31" s="87"/>
       <c r="C31" s="76" t="s">
         <v>4</v>
       </c>
@@ -5325,8 +5382,8 @@
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A32" s="82"/>
-      <c r="B32" s="90" t="s">
+      <c r="A32" s="85"/>
+      <c r="B32" s="88" t="s">
         <v>20</v>
       </c>
       <c r="C32" s="76" t="s">
@@ -5344,8 +5401,8 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="82"/>
-      <c r="B33" s="90"/>
+      <c r="A33" s="85"/>
+      <c r="B33" s="88"/>
       <c r="C33" s="77" t="s">
         <v>4</v>
       </c>
@@ -5361,10 +5418,10 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A34" s="82" t="s">
+      <c r="A34" s="85" t="s">
         <v>12</v>
       </c>
-      <c r="B34" s="92" t="s">
+      <c r="B34" s="87" t="s">
         <v>19</v>
       </c>
       <c r="C34" s="76" t="s">
@@ -5382,8 +5439,8 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A35" s="82"/>
-      <c r="B35" s="92"/>
+      <c r="A35" s="85"/>
+      <c r="B35" s="87"/>
       <c r="C35" s="76" t="s">
         <v>4</v>
       </c>
@@ -5399,8 +5456,8 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" s="82"/>
-      <c r="B36" s="85" t="s">
+      <c r="A36" s="85"/>
+      <c r="B36" s="90" t="s">
         <v>20</v>
       </c>
       <c r="C36" s="78" t="s">
@@ -5418,8 +5475,8 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A37" s="82"/>
-      <c r="B37" s="85"/>
+      <c r="A37" s="85"/>
+      <c r="B37" s="90"/>
       <c r="C37" s="76" t="s">
         <v>4</v>
       </c>
@@ -5435,10 +5492,10 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A38" s="82" t="s">
+      <c r="A38" s="85" t="s">
         <v>13</v>
       </c>
-      <c r="B38" s="92" t="s">
+      <c r="B38" s="87" t="s">
         <v>19</v>
       </c>
       <c r="C38" s="76" t="s">
@@ -5456,8 +5513,8 @@
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A39" s="82"/>
-      <c r="B39" s="92"/>
+      <c r="A39" s="85"/>
+      <c r="B39" s="87"/>
       <c r="C39" s="76" t="s">
         <v>4</v>
       </c>
@@ -5473,8 +5530,8 @@
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A40" s="82"/>
-      <c r="B40" s="85" t="s">
+      <c r="A40" s="85"/>
+      <c r="B40" s="90" t="s">
         <v>20</v>
       </c>
       <c r="C40" s="78" t="s">
@@ -5492,8 +5549,8 @@
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A41" s="82"/>
-      <c r="B41" s="85"/>
+      <c r="A41" s="85"/>
+      <c r="B41" s="90"/>
       <c r="C41" s="76" t="s">
         <v>4</v>
       </c>
@@ -5509,10 +5566,10 @@
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A42" s="82" t="s">
+      <c r="A42" s="85" t="s">
         <v>14</v>
       </c>
-      <c r="B42" s="92" t="s">
+      <c r="B42" s="87" t="s">
         <v>19</v>
       </c>
       <c r="C42" s="76" t="s">
@@ -5530,8 +5587,8 @@
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A43" s="82"/>
-      <c r="B43" s="92"/>
+      <c r="A43" s="85"/>
+      <c r="B43" s="87"/>
       <c r="C43" s="76" t="s">
         <v>4</v>
       </c>
@@ -5547,8 +5604,8 @@
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A44" s="82"/>
-      <c r="B44" s="85" t="s">
+      <c r="A44" s="85"/>
+      <c r="B44" s="90" t="s">
         <v>20</v>
       </c>
       <c r="C44" s="78" t="s">
@@ -5566,8 +5623,8 @@
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A45" s="82"/>
-      <c r="B45" s="85"/>
+      <c r="A45" s="85"/>
+      <c r="B45" s="90"/>
       <c r="C45" s="76" t="s">
         <v>4</v>
       </c>
@@ -5583,10 +5640,10 @@
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A46" s="82" t="s">
+      <c r="A46" s="85" t="s">
         <v>15</v>
       </c>
-      <c r="B46" s="92" t="s">
+      <c r="B46" s="87" t="s">
         <v>19</v>
       </c>
       <c r="C46" s="76" t="s">
@@ -5604,8 +5661,8 @@
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A47" s="82"/>
-      <c r="B47" s="92"/>
+      <c r="A47" s="85"/>
+      <c r="B47" s="87"/>
       <c r="C47" s="76" t="s">
         <v>4</v>
       </c>
@@ -5621,8 +5678,8 @@
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A48" s="82"/>
-      <c r="B48" s="90" t="s">
+      <c r="A48" s="85"/>
+      <c r="B48" s="88" t="s">
         <v>20</v>
       </c>
       <c r="C48" s="76" t="s">
@@ -5640,8 +5697,8 @@
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A49" s="82"/>
-      <c r="B49" s="90"/>
+      <c r="A49" s="85"/>
+      <c r="B49" s="88"/>
       <c r="C49" s="77" t="s">
         <v>4</v>
       </c>
@@ -5658,42 +5715,42 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="B36:B37"/>
     <mergeCell ref="A46:A49"/>
     <mergeCell ref="B46:B47"/>
     <mergeCell ref="B48:B49"/>
     <mergeCell ref="A42:A45"/>
     <mergeCell ref="B42:B43"/>
     <mergeCell ref="B44:B45"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5742,10 +5799,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="94" t="s">
+      <c r="A2" s="97" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="97" t="s">
+      <c r="B2" s="100" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="49" t="s">
@@ -5762,8 +5819,8 @@
       <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="95"/>
-      <c r="B3" s="98"/>
+      <c r="A3" s="98"/>
+      <c r="B3" s="101"/>
       <c r="C3" s="40" t="s">
         <v>4</v>
       </c>
@@ -5778,8 +5835,8 @@
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="95"/>
-      <c r="B4" s="101" t="s">
+      <c r="A4" s="98"/>
+      <c r="B4" s="104" t="s">
         <v>20</v>
       </c>
       <c r="C4" s="42" t="s">
@@ -5806,8 +5863,8 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="96"/>
-      <c r="B5" s="102"/>
+      <c r="A5" s="99"/>
+      <c r="B5" s="105"/>
       <c r="C5" s="41" t="s">
         <v>4</v>
       </c>
@@ -5822,10 +5879,10 @@
       <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="94" t="s">
+      <c r="A6" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="97" t="s">
+      <c r="B6" s="100" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="49" t="s">
@@ -5842,8 +5899,8 @@
       <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="95"/>
-      <c r="B7" s="98"/>
+      <c r="A7" s="98"/>
+      <c r="B7" s="101"/>
       <c r="C7" s="40" t="s">
         <v>4</v>
       </c>
@@ -5858,8 +5915,8 @@
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="95"/>
-      <c r="B8" s="101" t="s">
+      <c r="A8" s="98"/>
+      <c r="B8" s="104" t="s">
         <v>20</v>
       </c>
       <c r="C8" s="68" t="s">
@@ -5886,8 +5943,8 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="96"/>
-      <c r="B9" s="102"/>
+      <c r="A9" s="99"/>
+      <c r="B9" s="105"/>
       <c r="C9" s="41" t="s">
         <v>4</v>
       </c>
@@ -5902,10 +5959,10 @@
       <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="94" t="s">
+      <c r="A10" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="97" t="s">
+      <c r="B10" s="100" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="49" t="s">
@@ -5917,8 +5974,8 @@
       <c r="G10" s="50"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="95"/>
-      <c r="B11" s="98"/>
+      <c r="A11" s="98"/>
+      <c r="B11" s="101"/>
       <c r="C11" s="40" t="s">
         <v>4</v>
       </c>
@@ -5928,8 +5985,8 @@
       <c r="G11" s="6"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="95"/>
-      <c r="B12" s="99" t="s">
+      <c r="A12" s="98"/>
+      <c r="B12" s="102" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="43" t="s">
@@ -5941,8 +5998,8 @@
       <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" s="96"/>
-      <c r="B13" s="100"/>
+      <c r="A13" s="99"/>
+      <c r="B13" s="103"/>
       <c r="C13" s="41" t="s">
         <v>4</v>
       </c>
@@ -5952,10 +6009,10 @@
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" s="94" t="s">
+      <c r="A14" s="97" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="97" t="s">
+      <c r="B14" s="100" t="s">
         <v>19</v>
       </c>
       <c r="C14" s="49" t="s">
@@ -5967,8 +6024,8 @@
       <c r="G14" s="50"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" s="95"/>
-      <c r="B15" s="98"/>
+      <c r="A15" s="98"/>
+      <c r="B15" s="101"/>
       <c r="C15" s="40" t="s">
         <v>4</v>
       </c>
@@ -5978,8 +6035,8 @@
       <c r="G15" s="6"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" s="95"/>
-      <c r="B16" s="99" t="s">
+      <c r="A16" s="98"/>
+      <c r="B16" s="102" t="s">
         <v>20</v>
       </c>
       <c r="C16" s="43" t="s">
@@ -5991,8 +6048,8 @@
       <c r="G16" s="6"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="96"/>
-      <c r="B17" s="100"/>
+      <c r="A17" s="99"/>
+      <c r="B17" s="103"/>
       <c r="C17" s="41" t="s">
         <v>4</v>
       </c>
@@ -6002,10 +6059,10 @@
       <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="94" t="s">
+      <c r="A18" s="97" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="97" t="s">
+      <c r="B18" s="100" t="s">
         <v>19</v>
       </c>
       <c r="C18" s="49" t="s">
@@ -6017,8 +6074,8 @@
       <c r="G18" s="50"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="95"/>
-      <c r="B19" s="98"/>
+      <c r="A19" s="98"/>
+      <c r="B19" s="101"/>
       <c r="C19" s="40" t="s">
         <v>4</v>
       </c>
@@ -6028,8 +6085,8 @@
       <c r="G19" s="6"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="95"/>
-      <c r="B20" s="99" t="s">
+      <c r="A20" s="98"/>
+      <c r="B20" s="102" t="s">
         <v>20</v>
       </c>
       <c r="C20" s="43" t="s">
@@ -6041,8 +6098,8 @@
       <c r="G20" s="6"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="96"/>
-      <c r="B21" s="100"/>
+      <c r="A21" s="99"/>
+      <c r="B21" s="103"/>
       <c r="C21" s="41" t="s">
         <v>4</v>
       </c>
@@ -6052,10 +6109,10 @@
       <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" s="94" t="s">
+      <c r="A22" s="97" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="97" t="s">
+      <c r="B22" s="100" t="s">
         <v>19</v>
       </c>
       <c r="C22" s="49" t="s">
@@ -6072,8 +6129,8 @@
       <c r="G22" s="50"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="95"/>
-      <c r="B23" s="98"/>
+      <c r="A23" s="98"/>
+      <c r="B23" s="101"/>
       <c r="C23" s="40" t="s">
         <v>4</v>
       </c>
@@ -6088,8 +6145,8 @@
       <c r="G23" s="6"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="95"/>
-      <c r="B24" s="101" t="s">
+      <c r="A24" s="98"/>
+      <c r="B24" s="104" t="s">
         <v>20</v>
       </c>
       <c r="C24" s="72" t="s">
@@ -6108,8 +6165,8 @@
       <c r="G24" s="6"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" s="96"/>
-      <c r="B25" s="102"/>
+      <c r="A25" s="99"/>
+      <c r="B25" s="105"/>
       <c r="C25" s="41" t="s">
         <v>4</v>
       </c>
@@ -6124,10 +6181,10 @@
       <c r="G25" s="7"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" s="94" t="s">
+      <c r="A26" s="97" t="s">
         <v>10</v>
       </c>
-      <c r="B26" s="97" t="s">
+      <c r="B26" s="100" t="s">
         <v>19</v>
       </c>
       <c r="C26" s="49" t="s">
@@ -6139,8 +6196,8 @@
       <c r="G26" s="50"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="95"/>
-      <c r="B27" s="98"/>
+      <c r="A27" s="98"/>
+      <c r="B27" s="101"/>
       <c r="C27" s="40" t="s">
         <v>4</v>
       </c>
@@ -6150,8 +6207,8 @@
       <c r="G27" s="6"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="95"/>
-      <c r="B28" s="99" t="s">
+      <c r="A28" s="98"/>
+      <c r="B28" s="102" t="s">
         <v>20</v>
       </c>
       <c r="C28" s="43" t="s">
@@ -6163,8 +6220,8 @@
       <c r="G28" s="6"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" s="96"/>
-      <c r="B29" s="100"/>
+      <c r="A29" s="99"/>
+      <c r="B29" s="103"/>
       <c r="C29" s="41" t="s">
         <v>4</v>
       </c>
@@ -6174,10 +6231,10 @@
       <c r="G29" s="7"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30" s="94" t="s">
+      <c r="A30" s="97" t="s">
         <v>11</v>
       </c>
-      <c r="B30" s="97" t="s">
+      <c r="B30" s="100" t="s">
         <v>19</v>
       </c>
       <c r="C30" s="49" t="s">
@@ -6189,8 +6246,8 @@
       <c r="G30" s="50"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A31" s="95"/>
-      <c r="B31" s="98"/>
+      <c r="A31" s="98"/>
+      <c r="B31" s="101"/>
       <c r="C31" s="40" t="s">
         <v>4</v>
       </c>
@@ -6200,8 +6257,8 @@
       <c r="G31" s="6"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A32" s="95"/>
-      <c r="B32" s="99" t="s">
+      <c r="A32" s="98"/>
+      <c r="B32" s="102" t="s">
         <v>20</v>
       </c>
       <c r="C32" s="43" t="s">
@@ -6213,8 +6270,8 @@
       <c r="G32" s="6"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A33" s="96"/>
-      <c r="B33" s="100"/>
+      <c r="A33" s="99"/>
+      <c r="B33" s="103"/>
       <c r="C33" s="41" t="s">
         <v>4</v>
       </c>
@@ -6224,10 +6281,10 @@
       <c r="G33" s="7"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A34" s="94" t="s">
+      <c r="A34" s="97" t="s">
         <v>12</v>
       </c>
-      <c r="B34" s="97" t="s">
+      <c r="B34" s="100" t="s">
         <v>19</v>
       </c>
       <c r="C34" s="49" t="s">
@@ -6239,8 +6296,8 @@
       <c r="G34" s="50"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A35" s="95"/>
-      <c r="B35" s="98"/>
+      <c r="A35" s="98"/>
+      <c r="B35" s="101"/>
       <c r="C35" s="40" t="s">
         <v>4</v>
       </c>
@@ -6250,8 +6307,8 @@
       <c r="G35" s="6"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A36" s="95"/>
-      <c r="B36" s="99" t="s">
+      <c r="A36" s="98"/>
+      <c r="B36" s="102" t="s">
         <v>20</v>
       </c>
       <c r="C36" s="43" t="s">
@@ -6263,8 +6320,8 @@
       <c r="G36" s="6"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A37" s="96"/>
-      <c r="B37" s="100"/>
+      <c r="A37" s="99"/>
+      <c r="B37" s="103"/>
       <c r="C37" s="41" t="s">
         <v>4</v>
       </c>
@@ -6274,10 +6331,10 @@
       <c r="G37" s="7"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A38" s="94" t="s">
+      <c r="A38" s="97" t="s">
         <v>13</v>
       </c>
-      <c r="B38" s="97" t="s">
+      <c r="B38" s="100" t="s">
         <v>19</v>
       </c>
       <c r="C38" s="49" t="s">
@@ -6289,8 +6346,8 @@
       <c r="G38" s="50"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A39" s="95"/>
-      <c r="B39" s="98"/>
+      <c r="A39" s="98"/>
+      <c r="B39" s="101"/>
       <c r="C39" s="40" t="s">
         <v>4</v>
       </c>
@@ -6300,8 +6357,8 @@
       <c r="G39" s="6"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A40" s="95"/>
-      <c r="B40" s="99" t="s">
+      <c r="A40" s="98"/>
+      <c r="B40" s="102" t="s">
         <v>20</v>
       </c>
       <c r="C40" s="43" t="s">
@@ -6313,8 +6370,8 @@
       <c r="G40" s="6"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A41" s="96"/>
-      <c r="B41" s="100"/>
+      <c r="A41" s="99"/>
+      <c r="B41" s="103"/>
       <c r="C41" s="41" t="s">
         <v>4</v>
       </c>
@@ -6324,10 +6381,10 @@
       <c r="G41" s="7"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A42" s="94" t="s">
+      <c r="A42" s="97" t="s">
         <v>14</v>
       </c>
-      <c r="B42" s="97" t="s">
+      <c r="B42" s="100" t="s">
         <v>19</v>
       </c>
       <c r="C42" s="49" t="s">
@@ -6339,8 +6396,8 @@
       <c r="G42" s="50"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A43" s="95"/>
-      <c r="B43" s="98"/>
+      <c r="A43" s="98"/>
+      <c r="B43" s="101"/>
       <c r="C43" s="40" t="s">
         <v>4</v>
       </c>
@@ -6350,8 +6407,8 @@
       <c r="G43" s="6"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A44" s="95"/>
-      <c r="B44" s="99" t="s">
+      <c r="A44" s="98"/>
+      <c r="B44" s="102" t="s">
         <v>20</v>
       </c>
       <c r="C44" s="43" t="s">
@@ -6363,8 +6420,8 @@
       <c r="G44" s="6"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A45" s="96"/>
-      <c r="B45" s="100"/>
+      <c r="A45" s="99"/>
+      <c r="B45" s="103"/>
       <c r="C45" s="41" t="s">
         <v>4</v>
       </c>
@@ -6374,10 +6431,10 @@
       <c r="G45" s="7"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A46" s="94" t="s">
+      <c r="A46" s="97" t="s">
         <v>15</v>
       </c>
-      <c r="B46" s="97" t="s">
+      <c r="B46" s="100" t="s">
         <v>19</v>
       </c>
       <c r="C46" s="49" t="s">
@@ -6389,8 +6446,8 @@
       <c r="G46" s="50"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A47" s="95"/>
-      <c r="B47" s="98"/>
+      <c r="A47" s="98"/>
+      <c r="B47" s="101"/>
       <c r="C47" s="40" t="s">
         <v>4</v>
       </c>
@@ -6400,8 +6457,8 @@
       <c r="G47" s="6"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A48" s="95"/>
-      <c r="B48" s="99" t="s">
+      <c r="A48" s="98"/>
+      <c r="B48" s="102" t="s">
         <v>20</v>
       </c>
       <c r="C48" s="43" t="s">
@@ -6413,8 +6470,8 @@
       <c r="G48" s="6"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A49" s="96"/>
-      <c r="B49" s="100"/>
+      <c r="A49" s="99"/>
+      <c r="B49" s="103"/>
       <c r="C49" s="41" t="s">
         <v>4</v>
       </c>
@@ -6425,6 +6482,30 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="A46:A49"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B28:B29"/>
     <mergeCell ref="A14:A17"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="B16:B17"/>
@@ -6437,30 +6518,6 @@
     <mergeCell ref="A10:A13"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="B12:B13"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="A46:A49"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="B44:B45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>